<commit_message>
New renders, readme edits
</commit_message>
<xml_diff>
--- a/BOM/General Part List.xlsx
+++ b/BOM/General Part List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\Documents\3D Print\Clockmaker\clock-3\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F587EC-DDFC-497E-937E-8242D355909A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBA0AB88-63AC-4769-A951-2B22E933749E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-27600" yWindow="3060" windowWidth="23250" windowHeight="12480" xr2:uid="{6EB0A7B6-C6D7-4759-8B58-841D5EFF92F5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1173" uniqueCount="546">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1175" uniqueCount="546">
   <si>
     <t>ID</t>
   </si>
@@ -797,9 +797,6 @@
     <t>PN812</t>
   </si>
   <si>
-    <t>310x310mm Build Plate</t>
-  </si>
-  <si>
     <t>Creality</t>
   </si>
   <si>
@@ -824,9 +821,6 @@
     <t>PN814</t>
   </si>
   <si>
-    <t>Build Plate, Spring Steel</t>
-  </si>
-  <si>
     <t>Fulament</t>
   </si>
   <si>
@@ -1674,6 +1668,12 @@
   </si>
   <si>
     <t>1/2" or ~13mm will do.</t>
+  </si>
+  <si>
+    <t>310x310mm Heated Bed</t>
+  </si>
+  <si>
+    <t>Build Plate, Spring Steel, 310x310mm</t>
   </si>
 </sst>
 </file>
@@ -2089,8 +2089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D318B5EB-87D8-4D97-AE82-574AF33D7DA4}">
   <dimension ref="A1:H177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="H92" sqref="H92"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2114,7 +2114,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -2131,104 +2131,104 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B2" t="s">
+        <v>409</v>
+      </c>
+      <c r="C2" t="s">
+        <v>410</v>
+      </c>
+      <c r="D2" t="s">
+        <v>496</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>411</v>
       </c>
-      <c r="C2" t="s">
+      <c r="G2" s="8" t="s">
         <v>412</v>
       </c>
-      <c r="D2" t="s">
-        <v>498</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="6" t="s">
+      <c r="H2" t="s">
         <v>413</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>414</v>
-      </c>
-      <c r="H2" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B3" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C3" t="s">
+        <v>414</v>
+      </c>
+      <c r="D3" t="s">
+        <v>496</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="G3" s="9" t="s">
         <v>416</v>
       </c>
-      <c r="D3" t="s">
-        <v>498</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>417</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>418</v>
-      </c>
       <c r="H3" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B4" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C4" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D4" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="H4" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B5" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C5" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D5" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="G5" s="9"/>
       <c r="H5" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2242,7 +2242,7 @@
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>10</v>
@@ -2265,7 +2265,7 @@
         <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>10</v>
@@ -2288,7 +2288,7 @@
         <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>10</v>
@@ -2311,7 +2311,7 @@
         <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>10</v>
@@ -2334,7 +2334,7 @@
         <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>10</v>
@@ -2357,7 +2357,7 @@
         <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>10</v>
@@ -2378,7 +2378,7 @@
         <v>28</v>
       </c>
       <c r="D12" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>10</v>
@@ -2401,7 +2401,7 @@
         <v>31</v>
       </c>
       <c r="D13" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>10</v>
@@ -2425,7 +2425,7 @@
         <v>34</v>
       </c>
       <c r="D14" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>10</v>
@@ -2447,7 +2447,7 @@
         <v>36</v>
       </c>
       <c r="D15" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>37</v>
@@ -2473,7 +2473,7 @@
         <v>42</v>
       </c>
       <c r="D16" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>10</v>
@@ -2496,7 +2496,7 @@
         <v>45</v>
       </c>
       <c r="D17" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>10</v>
@@ -2508,7 +2508,7 @@
         <v>46</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -2522,7 +2522,7 @@
         <v>48</v>
       </c>
       <c r="D18" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>10</v>
@@ -2545,7 +2545,7 @@
         <v>51</v>
       </c>
       <c r="D19" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>10</v>
@@ -2565,12 +2565,17 @@
         <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="D20" t="s">
-        <v>498</v>
-      </c>
-      <c r="E20" s="3"/>
+        <v>496</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" t="s">
+        <v>67</v>
+      </c>
       <c r="G20" s="5"/>
       <c r="H20" s="1"/>
     </row>
@@ -2585,7 +2590,7 @@
         <v>55</v>
       </c>
       <c r="D21" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>10</v>
@@ -2611,7 +2616,7 @@
         <v>60</v>
       </c>
       <c r="D22" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>10</v>
@@ -2632,10 +2637,10 @@
         <v>8</v>
       </c>
       <c r="C23" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="D23" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>10</v>
@@ -2650,16 +2655,16 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B24" t="s">
         <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="D24" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>10</v>
@@ -2668,48 +2673,48 @@
         <v>11</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="H24" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B25" t="s">
         <v>8</v>
       </c>
       <c r="C25" t="s">
+        <v>433</v>
+      </c>
+      <c r="D25" t="s">
+        <v>496</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="D25" t="s">
-        <v>498</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>437</v>
-      </c>
       <c r="F25" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="G25" s="5"/>
       <c r="H25" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B26" t="s">
         <v>8</v>
       </c>
       <c r="C26" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="D26" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>10</v>
@@ -2719,7 +2724,7 @@
       </c>
       <c r="G26" s="5"/>
       <c r="H26" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -2733,7 +2738,7 @@
         <v>66</v>
       </c>
       <c r="D27" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>10</v>
@@ -2754,7 +2759,7 @@
         <v>69</v>
       </c>
       <c r="D28" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>10</v>
@@ -2775,7 +2780,7 @@
         <v>71</v>
       </c>
       <c r="D29" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>10</v>
@@ -2796,7 +2801,7 @@
         <v>73</v>
       </c>
       <c r="D30" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>10</v>
@@ -2817,7 +2822,7 @@
         <v>75</v>
       </c>
       <c r="D31" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>10</v>
@@ -2838,7 +2843,7 @@
         <v>77</v>
       </c>
       <c r="D32" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>10</v>
@@ -2859,7 +2864,7 @@
         <v>79</v>
       </c>
       <c r="D33" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>10</v>
@@ -2880,7 +2885,7 @@
         <v>81</v>
       </c>
       <c r="D34" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>10</v>
@@ -2901,7 +2906,7 @@
         <v>83</v>
       </c>
       <c r="D35" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>10</v>
@@ -2922,7 +2927,7 @@
         <v>85</v>
       </c>
       <c r="D36" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>10</v>
@@ -2946,7 +2951,7 @@
         <v>88</v>
       </c>
       <c r="D37" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>10</v>
@@ -2970,7 +2975,7 @@
         <v>91</v>
       </c>
       <c r="D38" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>10</v>
@@ -2991,7 +2996,7 @@
         <v>93</v>
       </c>
       <c r="D39" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>10</v>
@@ -3012,7 +3017,7 @@
         <v>96</v>
       </c>
       <c r="D40" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>10</v>
@@ -3033,7 +3038,7 @@
         <v>100</v>
       </c>
       <c r="D41" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>10</v>
@@ -3056,7 +3061,7 @@
         <v>104</v>
       </c>
       <c r="D42" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>10</v>
@@ -3079,7 +3084,7 @@
         <v>107</v>
       </c>
       <c r="D43" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>10</v>
@@ -3102,7 +3107,7 @@
         <v>110</v>
       </c>
       <c r="D44" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>10</v>
@@ -3125,7 +3130,7 @@
         <v>114</v>
       </c>
       <c r="D45" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>10</v>
@@ -3146,7 +3151,7 @@
         <v>116</v>
       </c>
       <c r="D46" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>10</v>
@@ -3158,7 +3163,7 @@
         <v>118</v>
       </c>
       <c r="H46" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -3172,7 +3177,7 @@
         <v>120</v>
       </c>
       <c r="D47" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>10</v>
@@ -3195,7 +3200,7 @@
         <v>123</v>
       </c>
       <c r="D48" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>10</v>
@@ -3218,7 +3223,7 @@
         <v>127</v>
       </c>
       <c r="D49" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>10</v>
@@ -3241,7 +3246,7 @@
         <v>131</v>
       </c>
       <c r="D50" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>10</v>
@@ -3264,7 +3269,7 @@
         <v>133</v>
       </c>
       <c r="D51" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>10</v>
@@ -3287,7 +3292,7 @@
         <v>136</v>
       </c>
       <c r="D52" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>10</v>
@@ -3310,7 +3315,7 @@
         <v>140</v>
       </c>
       <c r="D53" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>141</v>
@@ -3333,7 +3338,7 @@
         <v>144</v>
       </c>
       <c r="D54" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>10</v>
@@ -3354,7 +3359,7 @@
         <v>146</v>
       </c>
       <c r="D55" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>141</v>
@@ -3377,7 +3382,7 @@
         <v>149</v>
       </c>
       <c r="D56" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>141</v>
@@ -3400,7 +3405,7 @@
         <v>152</v>
       </c>
       <c r="D57" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>141</v>
@@ -3420,10 +3425,10 @@
         <v>139</v>
       </c>
       <c r="C58" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="D58" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="G58" s="5" t="s">
         <v>155</v>
@@ -3440,10 +3445,10 @@
         <v>139</v>
       </c>
       <c r="C59" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D59" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>141</v>
@@ -3455,21 +3460,21 @@
         <v>158</v>
       </c>
       <c r="H59" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B60" t="s">
         <v>139</v>
       </c>
       <c r="C60" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="D60" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>141</v>
@@ -3481,26 +3486,26 @@
         <v>158</v>
       </c>
       <c r="H60" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B61" t="s">
         <v>139</v>
       </c>
       <c r="C61" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="D61" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E61" s="1"/>
       <c r="G61" s="5"/>
       <c r="H61" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -3514,7 +3519,7 @@
         <v>160</v>
       </c>
       <c r="D62" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>141</v>
@@ -3540,7 +3545,7 @@
         <v>164</v>
       </c>
       <c r="D63" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>141</v>
@@ -3566,7 +3571,7 @@
         <v>168</v>
       </c>
       <c r="D64" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>141</v>
@@ -3592,7 +3597,7 @@
         <v>172</v>
       </c>
       <c r="D65" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>141</v>
@@ -3618,7 +3623,7 @@
         <v>176</v>
       </c>
       <c r="D66" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>141</v>
@@ -3644,7 +3649,7 @@
         <v>180</v>
       </c>
       <c r="D67" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>141</v>
@@ -3670,7 +3675,7 @@
         <v>184</v>
       </c>
       <c r="D68" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E68" t="s">
         <v>141</v>
@@ -3696,7 +3701,7 @@
         <v>187</v>
       </c>
       <c r="D69" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>141</v>
@@ -3722,7 +3727,7 @@
         <v>191</v>
       </c>
       <c r="D70" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>141</v>
@@ -3748,7 +3753,7 @@
         <v>194</v>
       </c>
       <c r="D71" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>141</v>
@@ -3774,7 +3779,7 @@
         <v>198</v>
       </c>
       <c r="D72" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>141</v>
@@ -3800,7 +3805,7 @@
         <v>202</v>
       </c>
       <c r="D73" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>141</v>
@@ -3826,7 +3831,7 @@
         <v>206</v>
       </c>
       <c r="D74" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>141</v>
@@ -3852,7 +3857,7 @@
         <v>210</v>
       </c>
       <c r="D75" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>141</v>
@@ -3878,7 +3883,7 @@
         <v>214</v>
       </c>
       <c r="D76" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>141</v>
@@ -3904,7 +3909,7 @@
         <v>218</v>
       </c>
       <c r="D77" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E77" t="s">
         <v>219</v>
@@ -3928,7 +3933,7 @@
         <v>222</v>
       </c>
       <c r="D78" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E78" t="s">
         <v>219</v>
@@ -3952,7 +3957,7 @@
         <v>225</v>
       </c>
       <c r="D79" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E79" t="s">
         <v>219</v>
@@ -3962,7 +3967,7 @@
       </c>
       <c r="G79" s="5"/>
       <c r="H79" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -3976,7 +3981,7 @@
         <v>227</v>
       </c>
       <c r="D80" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E80" t="s">
         <v>219</v>
@@ -3986,7 +3991,7 @@
       </c>
       <c r="G80" s="5"/>
       <c r="H80" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -3997,10 +4002,10 @@
         <v>139</v>
       </c>
       <c r="C81" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="D81" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E81" t="s">
         <v>219</v>
@@ -4010,7 +4015,7 @@
       </c>
       <c r="G81" s="5"/>
       <c r="H81" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
@@ -4021,10 +4026,10 @@
         <v>139</v>
       </c>
       <c r="C82" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="D82" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E82" t="s">
         <v>219</v>
@@ -4034,7 +4039,7 @@
       </c>
       <c r="G82" s="5"/>
       <c r="H82" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
@@ -4048,7 +4053,7 @@
         <v>231</v>
       </c>
       <c r="D83" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E83" t="s">
         <v>219</v>
@@ -4058,7 +4063,7 @@
       </c>
       <c r="G83" s="5"/>
       <c r="H83" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
@@ -4072,7 +4077,7 @@
         <v>233</v>
       </c>
       <c r="D84" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E84" t="s">
         <v>219</v>
@@ -4082,7 +4087,7 @@
       </c>
       <c r="G84" s="5"/>
       <c r="H84" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -4096,7 +4101,7 @@
         <v>235</v>
       </c>
       <c r="D85" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E85" t="s">
         <v>219</v>
@@ -4106,7 +4111,7 @@
       </c>
       <c r="G85" s="5"/>
       <c r="H85" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
@@ -4120,7 +4125,7 @@
         <v>237</v>
       </c>
       <c r="D86" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E86" t="s">
         <v>219</v>
@@ -4130,21 +4135,21 @@
       </c>
       <c r="G86" s="5"/>
       <c r="H86" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B87" t="s">
         <v>139</v>
       </c>
       <c r="C87" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="D87" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E87" t="s">
         <v>219</v>
@@ -4154,21 +4159,21 @@
       </c>
       <c r="G87" s="5"/>
       <c r="H87" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B88" t="s">
         <v>139</v>
       </c>
       <c r="C88" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="D88" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E88" t="s">
         <v>219</v>
@@ -4178,21 +4183,21 @@
       </c>
       <c r="G88" s="5"/>
       <c r="H88" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B89" t="s">
         <v>139</v>
       </c>
       <c r="C89" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="D89" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E89" t="s">
         <v>219</v>
@@ -4202,21 +4207,21 @@
       </c>
       <c r="G89" s="5"/>
       <c r="H89" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="B90" t="s">
         <v>139</v>
       </c>
       <c r="C90" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="D90" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E90" t="s">
         <v>219</v>
@@ -4226,21 +4231,21 @@
       </c>
       <c r="G90" s="5"/>
       <c r="H90" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="B91" t="s">
         <v>139</v>
       </c>
       <c r="C91" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="D91" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E91" t="s">
         <v>219</v>
@@ -4250,169 +4255,169 @@
       </c>
       <c r="G91" s="5"/>
       <c r="H91" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B92" t="s">
         <v>139</v>
       </c>
       <c r="C92" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="D92" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="G92" s="5"/>
       <c r="H92" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="B93" t="s">
         <v>139</v>
       </c>
       <c r="C93" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="D93" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="G93" s="5"/>
       <c r="H93" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="B94" t="s">
         <v>139</v>
       </c>
       <c r="C94" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="D94" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="G94" s="5"/>
       <c r="H94" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="B95" t="s">
         <v>139</v>
       </c>
       <c r="C95" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="D95" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="G95" s="5"/>
       <c r="H95" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B96" t="s">
         <v>139</v>
       </c>
       <c r="C96" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="D96" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="G96" s="5"/>
       <c r="H96" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="B97" t="s">
         <v>139</v>
       </c>
       <c r="C97" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="D97" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="G97" s="5"/>
       <c r="H97" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="B98" t="s">
         <v>139</v>
       </c>
       <c r="C98" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="D98" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="G98" s="5"/>
       <c r="H98" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="B99" t="s">
         <v>139</v>
       </c>
       <c r="C99" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="D99" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="G99" s="5"/>
       <c r="H99" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="B100" t="s">
         <v>139</v>
       </c>
       <c r="C100" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="D100" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="G100" s="5"/>
       <c r="H100" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
@@ -4426,7 +4431,7 @@
         <v>240</v>
       </c>
       <c r="D101" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>10</v>
@@ -4447,7 +4452,7 @@
         <v>243</v>
       </c>
       <c r="D102" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>10</v>
@@ -4468,7 +4473,7 @@
         <v>245</v>
       </c>
       <c r="D103" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>10</v>
@@ -4489,7 +4494,7 @@
         <v>248</v>
       </c>
       <c r="D104" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>10</v>
@@ -4515,7 +4520,7 @@
         <v>250</v>
       </c>
       <c r="D105" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>10</v>
@@ -4538,85 +4543,85 @@
         <v>239</v>
       </c>
       <c r="C106" t="s">
+        <v>544</v>
+      </c>
+      <c r="D106" t="s">
+        <v>496</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F106" t="s">
         <v>253</v>
       </c>
-      <c r="D106" t="s">
-        <v>498</v>
-      </c>
-      <c r="E106" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F106" t="s">
+      <c r="G106" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="G106" s="5" t="s">
+      <c r="H106" t="s">
         <v>255</v>
-      </c>
-      <c r="H106" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B107" t="s">
         <v>239</v>
       </c>
       <c r="C107" t="s">
+        <v>257</v>
+      </c>
+      <c r="D107" t="s">
+        <v>496</v>
+      </c>
+      <c r="E107" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="D107" t="s">
-        <v>498</v>
-      </c>
-      <c r="E107" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="F107" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G107" s="5">
         <v>570</v>
       </c>
       <c r="H107" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B108" t="s">
         <v>239</v>
       </c>
       <c r="C108" t="s">
+        <v>545</v>
+      </c>
+      <c r="D108" t="s">
+        <v>496</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F108" t="s">
+        <v>261</v>
+      </c>
+      <c r="G108" s="5" t="s">
         <v>262</v>
-      </c>
-      <c r="D108" t="s">
-        <v>498</v>
-      </c>
-      <c r="E108" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F108" t="s">
-        <v>263</v>
-      </c>
-      <c r="G108" s="5" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B109" t="s">
         <v>239</v>
       </c>
       <c r="C109" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D109" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>10</v>
@@ -4626,21 +4631,21 @@
       </c>
       <c r="G109" s="5"/>
       <c r="H109" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B110" t="s">
         <v>239</v>
       </c>
       <c r="C110" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D110" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>10</v>
@@ -4652,40 +4657,40 @@
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B111" t="s">
         <v>239</v>
       </c>
       <c r="C111" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D111" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F111" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G111" s="5"/>
       <c r="H111" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B112" t="s">
         <v>239</v>
       </c>
       <c r="C112" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D112" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>10</v>
@@ -4695,21 +4700,21 @@
       </c>
       <c r="G112" s="5"/>
       <c r="H112" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B113" t="s">
         <v>239</v>
       </c>
       <c r="C113" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D113" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>10</v>
@@ -4719,21 +4724,21 @@
       </c>
       <c r="G113" s="5"/>
       <c r="H113" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="B114" t="s">
         <v>239</v>
       </c>
       <c r="C114" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="D114" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E114" s="1" t="s">
         <v>10</v>
@@ -4743,21 +4748,21 @@
       </c>
       <c r="G114" s="5"/>
       <c r="H114" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B115" t="s">
         <v>239</v>
       </c>
       <c r="C115" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D115" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>10</v>
@@ -4769,189 +4774,189 @@
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
+        <v>278</v>
+      </c>
+      <c r="B116" t="s">
+        <v>279</v>
+      </c>
+      <c r="C116" t="s">
         <v>280</v>
       </c>
-      <c r="B116" t="s">
+      <c r="D116" t="s">
+        <v>496</v>
+      </c>
+      <c r="E116" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="C116" t="s">
+      <c r="F116" t="s">
         <v>282</v>
       </c>
-      <c r="D116" t="s">
-        <v>498</v>
-      </c>
-      <c r="E116" s="1" t="s">
+      <c r="G116" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="F116" t="s">
+      <c r="H116" t="s">
         <v>284</v>
-      </c>
-      <c r="G116" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="H116" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
+        <v>285</v>
+      </c>
+      <c r="B117" t="s">
+        <v>279</v>
+      </c>
+      <c r="C117" t="s">
+        <v>286</v>
+      </c>
+      <c r="D117" t="s">
+        <v>496</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="F117" t="s">
+        <v>282</v>
+      </c>
+      <c r="G117" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="B117" t="s">
-        <v>281</v>
-      </c>
-      <c r="C117" t="s">
+      <c r="H117" t="s">
         <v>288</v>
-      </c>
-      <c r="D117" t="s">
-        <v>498</v>
-      </c>
-      <c r="E117" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="F117" t="s">
-        <v>284</v>
-      </c>
-      <c r="G117" s="5" t="s">
-        <v>289</v>
-      </c>
-      <c r="H117" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
+        <v>289</v>
+      </c>
+      <c r="B118" t="s">
+        <v>279</v>
+      </c>
+      <c r="C118" t="s">
+        <v>290</v>
+      </c>
+      <c r="D118" t="s">
+        <v>496</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="F118" t="s">
+        <v>282</v>
+      </c>
+      <c r="G118" s="5" t="s">
         <v>291</v>
-      </c>
-      <c r="B118" t="s">
-        <v>281</v>
-      </c>
-      <c r="C118" t="s">
-        <v>292</v>
-      </c>
-      <c r="D118" t="s">
-        <v>498</v>
-      </c>
-      <c r="E118" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="F118" t="s">
-        <v>284</v>
-      </c>
-      <c r="G118" s="5" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
+        <v>292</v>
+      </c>
+      <c r="B119" t="s">
+        <v>279</v>
+      </c>
+      <c r="C119" t="s">
+        <v>293</v>
+      </c>
+      <c r="D119" t="s">
+        <v>496</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F119" t="s">
+        <v>253</v>
+      </c>
+      <c r="G119" s="5" t="s">
         <v>294</v>
       </c>
-      <c r="B119" t="s">
-        <v>281</v>
-      </c>
-      <c r="C119" t="s">
+      <c r="H119" t="s">
         <v>295</v>
-      </c>
-      <c r="D119" t="s">
-        <v>498</v>
-      </c>
-      <c r="E119" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F119" t="s">
-        <v>254</v>
-      </c>
-      <c r="G119" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="H119" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
+        <v>296</v>
+      </c>
+      <c r="B120" t="s">
+        <v>279</v>
+      </c>
+      <c r="C120" t="s">
+        <v>297</v>
+      </c>
+      <c r="D120" t="s">
+        <v>496</v>
+      </c>
+      <c r="E120" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="B120" t="s">
-        <v>281</v>
-      </c>
-      <c r="C120" t="s">
+      <c r="F120" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="D120" t="s">
-        <v>498</v>
-      </c>
-      <c r="E120" s="1" t="s">
+      <c r="G120" s="10" t="s">
         <v>300</v>
       </c>
-      <c r="F120" s="2" t="s">
+      <c r="H120" t="s">
         <v>301</v>
-      </c>
-      <c r="G120" s="10" t="s">
-        <v>302</v>
-      </c>
-      <c r="H120" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
+        <v>302</v>
+      </c>
+      <c r="B121" t="s">
+        <v>279</v>
+      </c>
+      <c r="C121" t="s">
+        <v>303</v>
+      </c>
+      <c r="D121" t="s">
+        <v>496</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="F121" t="s">
         <v>304</v>
       </c>
-      <c r="B121" t="s">
-        <v>281</v>
-      </c>
-      <c r="C121" t="s">
+      <c r="G121" s="5" t="s">
         <v>305</v>
-      </c>
-      <c r="D121" t="s">
-        <v>498</v>
-      </c>
-      <c r="E121" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="F121" t="s">
-        <v>306</v>
-      </c>
-      <c r="G121" s="5" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
+        <v>306</v>
+      </c>
+      <c r="B122" t="s">
+        <v>279</v>
+      </c>
+      <c r="C122" t="s">
+        <v>307</v>
+      </c>
+      <c r="D122" t="s">
+        <v>496</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="F122" t="s">
         <v>308</v>
       </c>
-      <c r="B122" t="s">
-        <v>281</v>
-      </c>
-      <c r="C122" t="s">
+      <c r="G122" s="5" t="s">
         <v>309</v>
-      </c>
-      <c r="D122" t="s">
-        <v>498</v>
-      </c>
-      <c r="E122" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="F122" t="s">
-        <v>310</v>
-      </c>
-      <c r="G122" s="5" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B123" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C123" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D123" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>10</v>
@@ -4961,21 +4966,21 @@
       </c>
       <c r="G123" s="5"/>
       <c r="H123" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B124" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C124" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D124" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>10</v>
@@ -4985,21 +4990,21 @@
       </c>
       <c r="G124" s="5"/>
       <c r="H124" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B125" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C125" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D125" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="E125" s="1" t="s">
         <v>10</v>
@@ -5009,21 +5014,21 @@
       </c>
       <c r="G125" s="5"/>
       <c r="H125" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B126" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C126" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D126" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="E126" s="1" t="s">
         <v>10</v>
@@ -5033,21 +5038,21 @@
       </c>
       <c r="G126" s="5"/>
       <c r="H126" s="4" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B127" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C127" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D127" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="E127" s="1" t="s">
         <v>10</v>
@@ -5057,421 +5062,421 @@
       </c>
       <c r="G127" s="5"/>
       <c r="H127" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
+        <v>319</v>
+      </c>
+      <c r="B128" t="s">
+        <v>279</v>
+      </c>
+      <c r="C128" t="s">
+        <v>320</v>
+      </c>
+      <c r="D128" t="s">
+        <v>496</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="F128" t="s">
         <v>321</v>
       </c>
-      <c r="B128" t="s">
-        <v>281</v>
-      </c>
-      <c r="C128" t="s">
+      <c r="G128" s="8" t="s">
         <v>322</v>
-      </c>
-      <c r="D128" t="s">
-        <v>498</v>
-      </c>
-      <c r="E128" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="F128" t="s">
-        <v>323</v>
-      </c>
-      <c r="G128" s="8" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
+        <v>323</v>
+      </c>
+      <c r="B129" t="s">
+        <v>279</v>
+      </c>
+      <c r="C129" t="s">
+        <v>324</v>
+      </c>
+      <c r="D129" t="s">
+        <v>496</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="F129" t="s">
+        <v>321</v>
+      </c>
+      <c r="G129" s="8" t="s">
         <v>325</v>
-      </c>
-      <c r="B129" t="s">
-        <v>281</v>
-      </c>
-      <c r="C129" t="s">
-        <v>326</v>
-      </c>
-      <c r="D129" t="s">
-        <v>498</v>
-      </c>
-      <c r="E129" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="F129" t="s">
-        <v>323</v>
-      </c>
-      <c r="G129" s="8" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
+        <v>326</v>
+      </c>
+      <c r="B130" t="s">
+        <v>279</v>
+      </c>
+      <c r="C130" t="s">
+        <v>327</v>
+      </c>
+      <c r="D130" t="s">
+        <v>496</v>
+      </c>
+      <c r="E130" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="F130" t="s">
+        <v>321</v>
+      </c>
+      <c r="G130" s="5" t="s">
         <v>328</v>
-      </c>
-      <c r="B130" t="s">
-        <v>281</v>
-      </c>
-      <c r="C130" t="s">
-        <v>329</v>
-      </c>
-      <c r="D130" t="s">
-        <v>498</v>
-      </c>
-      <c r="E130" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="F130" t="s">
-        <v>323</v>
-      </c>
-      <c r="G130" s="5" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
+        <v>329</v>
+      </c>
+      <c r="B131" t="s">
+        <v>279</v>
+      </c>
+      <c r="C131" t="s">
+        <v>330</v>
+      </c>
+      <c r="D131" t="s">
+        <v>496</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="F131" t="s">
+        <v>321</v>
+      </c>
+      <c r="G131" s="5" t="s">
         <v>331</v>
-      </c>
-      <c r="B131" t="s">
-        <v>281</v>
-      </c>
-      <c r="C131" t="s">
-        <v>332</v>
-      </c>
-      <c r="D131" t="s">
-        <v>498</v>
-      </c>
-      <c r="E131" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="F131" t="s">
-        <v>323</v>
-      </c>
-      <c r="G131" s="5" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
+        <v>332</v>
+      </c>
+      <c r="B132" t="s">
+        <v>279</v>
+      </c>
+      <c r="C132" t="s">
+        <v>333</v>
+      </c>
+      <c r="D132" t="s">
+        <v>496</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="F132" t="s">
+        <v>321</v>
+      </c>
+      <c r="G132" s="5" t="s">
         <v>334</v>
-      </c>
-      <c r="B132" t="s">
-        <v>281</v>
-      </c>
-      <c r="C132" t="s">
-        <v>335</v>
-      </c>
-      <c r="D132" t="s">
-        <v>498</v>
-      </c>
-      <c r="E132" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="F132" t="s">
-        <v>323</v>
-      </c>
-      <c r="G132" s="5" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
+        <v>335</v>
+      </c>
+      <c r="B133" t="s">
+        <v>279</v>
+      </c>
+      <c r="C133" t="s">
+        <v>336</v>
+      </c>
+      <c r="D133" t="s">
+        <v>496</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="F133" t="s">
+        <v>321</v>
+      </c>
+      <c r="G133" s="5" t="s">
         <v>337</v>
-      </c>
-      <c r="B133" t="s">
-        <v>281</v>
-      </c>
-      <c r="C133" t="s">
-        <v>338</v>
-      </c>
-      <c r="D133" t="s">
-        <v>498</v>
-      </c>
-      <c r="E133" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="F133" t="s">
-        <v>323</v>
-      </c>
-      <c r="G133" s="5" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
+        <v>338</v>
+      </c>
+      <c r="B134" t="s">
+        <v>279</v>
+      </c>
+      <c r="C134" t="s">
+        <v>339</v>
+      </c>
+      <c r="D134" t="s">
+        <v>496</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="F134" t="s">
+        <v>321</v>
+      </c>
+      <c r="G134" s="5" t="s">
         <v>340</v>
-      </c>
-      <c r="B134" t="s">
-        <v>281</v>
-      </c>
-      <c r="C134" t="s">
-        <v>341</v>
-      </c>
-      <c r="D134" t="s">
-        <v>498</v>
-      </c>
-      <c r="E134" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="F134" t="s">
-        <v>323</v>
-      </c>
-      <c r="G134" s="5" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
+        <v>341</v>
+      </c>
+      <c r="B135" t="s">
+        <v>279</v>
+      </c>
+      <c r="C135" t="s">
+        <v>342</v>
+      </c>
+      <c r="D135" t="s">
+        <v>496</v>
+      </c>
+      <c r="E135" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="F135" t="s">
+        <v>321</v>
+      </c>
+      <c r="G135" s="5" t="s">
         <v>343</v>
-      </c>
-      <c r="B135" t="s">
-        <v>281</v>
-      </c>
-      <c r="C135" t="s">
-        <v>344</v>
-      </c>
-      <c r="D135" t="s">
-        <v>498</v>
-      </c>
-      <c r="E135" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="F135" t="s">
-        <v>323</v>
-      </c>
-      <c r="G135" s="5" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
+        <v>344</v>
+      </c>
+      <c r="B136" t="s">
+        <v>279</v>
+      </c>
+      <c r="C136" t="s">
+        <v>345</v>
+      </c>
+      <c r="D136" t="s">
+        <v>496</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="F136" t="s">
+        <v>321</v>
+      </c>
+      <c r="G136" s="5" t="s">
         <v>346</v>
-      </c>
-      <c r="B136" t="s">
-        <v>281</v>
-      </c>
-      <c r="C136" t="s">
-        <v>347</v>
-      </c>
-      <c r="D136" t="s">
-        <v>498</v>
-      </c>
-      <c r="E136" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="F136" t="s">
-        <v>323</v>
-      </c>
-      <c r="G136" s="5" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B137" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C137" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D137" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E137" s="1" t="s">
         <v>141</v>
       </c>
       <c r="F137" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="G137" s="5" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="H137" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B138" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C138" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="D138" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F138" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="G138" s="5" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B139" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C139" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D139" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E139" s="3" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F139" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="G139" s="5" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B140" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C140" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D140" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F140" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="G140" s="5" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B141" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C141" t="s">
+        <v>500</v>
+      </c>
+      <c r="D141" t="s">
+        <v>496</v>
+      </c>
+      <c r="E141" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="F141" t="s">
+        <v>321</v>
+      </c>
+      <c r="G141" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="H141" t="s">
         <v>502</v>
-      </c>
-      <c r="D141" t="s">
-        <v>498</v>
-      </c>
-      <c r="E141" s="3" t="s">
-        <v>300</v>
-      </c>
-      <c r="F141" t="s">
-        <v>323</v>
-      </c>
-      <c r="G141" s="5" t="s">
-        <v>447</v>
-      </c>
-      <c r="H141" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B142" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C142" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="D142" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F142" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="G142" s="5" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="H142" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B143" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C143" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="D143" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F143" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="G143" s="10" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
+        <v>354</v>
+      </c>
+      <c r="B144" t="s">
+        <v>279</v>
+      </c>
+      <c r="C144" t="s">
+        <v>355</v>
+      </c>
+      <c r="D144" t="s">
+        <v>496</v>
+      </c>
+      <c r="E144" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F144" t="s">
         <v>356</v>
       </c>
-      <c r="B144" t="s">
-        <v>281</v>
-      </c>
-      <c r="C144" t="s">
+      <c r="G144" s="5" t="s">
         <v>357</v>
-      </c>
-      <c r="D144" t="s">
-        <v>498</v>
-      </c>
-      <c r="E144" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F144" t="s">
-        <v>358</v>
-      </c>
-      <c r="G144" s="5" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B145" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C145" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D145" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E145" s="1" t="s">
         <v>10</v>
@@ -5483,63 +5488,63 @@
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
+        <v>360</v>
+      </c>
+      <c r="B146" t="s">
+        <v>279</v>
+      </c>
+      <c r="C146" t="s">
+        <v>361</v>
+      </c>
+      <c r="D146" t="s">
+        <v>496</v>
+      </c>
+      <c r="E146" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F146" t="s">
         <v>362</v>
       </c>
-      <c r="B146" t="s">
-        <v>281</v>
-      </c>
-      <c r="C146" t="s">
+      <c r="G146" s="5" t="s">
         <v>363</v>
-      </c>
-      <c r="D146" t="s">
-        <v>498</v>
-      </c>
-      <c r="E146" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F146" t="s">
-        <v>364</v>
-      </c>
-      <c r="G146" s="5" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
+        <v>364</v>
+      </c>
+      <c r="B147" t="s">
+        <v>279</v>
+      </c>
+      <c r="C147" t="s">
+        <v>365</v>
+      </c>
+      <c r="D147" t="s">
+        <v>496</v>
+      </c>
+      <c r="E147" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F147" t="s">
         <v>366</v>
-      </c>
-      <c r="B147" t="s">
-        <v>281</v>
-      </c>
-      <c r="C147" t="s">
-        <v>367</v>
-      </c>
-      <c r="D147" t="s">
-        <v>498</v>
-      </c>
-      <c r="E147" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F147" t="s">
-        <v>368</v>
       </c>
       <c r="G147" s="5"/>
       <c r="H147" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B148" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C148" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D148" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E148" s="1" t="s">
         <v>10</v>
@@ -5551,16 +5556,16 @@
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B149" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C149" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D149" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E149" s="1" t="s">
         <v>10</v>
@@ -5572,16 +5577,16 @@
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B150" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C150" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D150" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E150" s="1" t="s">
         <v>10</v>
@@ -5591,47 +5596,47 @@
       </c>
       <c r="G150" s="5"/>
       <c r="H150" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
+        <v>375</v>
+      </c>
+      <c r="B151" t="s">
+        <v>279</v>
+      </c>
+      <c r="C151" t="s">
+        <v>376</v>
+      </c>
+      <c r="D151" t="s">
+        <v>496</v>
+      </c>
+      <c r="E151" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F151" t="s">
         <v>377</v>
       </c>
-      <c r="B151" t="s">
-        <v>281</v>
-      </c>
-      <c r="C151" t="s">
+      <c r="G151" s="5" t="s">
         <v>378</v>
       </c>
-      <c r="D151" t="s">
-        <v>498</v>
-      </c>
-      <c r="E151" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F151" t="s">
+      <c r="H151" t="s">
         <v>379</v>
-      </c>
-      <c r="G151" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="H151" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B152" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C152" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D152" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E152" s="1" t="s">
         <v>141</v>
@@ -5640,24 +5645,24 @@
         <v>37</v>
       </c>
       <c r="G152" s="5" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="H152" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B153" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C153" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D153" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E153" s="1" t="s">
         <v>10</v>
@@ -5667,21 +5672,21 @@
       </c>
       <c r="G153" s="5"/>
       <c r="H153" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B154" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C154" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D154" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E154" s="1" t="s">
         <v>10</v>
@@ -5691,21 +5696,21 @@
       </c>
       <c r="G154" s="5"/>
       <c r="H154" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B155" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C155" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D155" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E155" s="1" t="s">
         <v>10</v>
@@ -5714,42 +5719,42 @@
         <v>117</v>
       </c>
       <c r="G155" s="5" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B156" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C156" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D156" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E156" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G156" s="5"/>
       <c r="H156" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B157" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C157" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="D157" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E157" s="1" t="s">
         <v>10</v>
@@ -5758,21 +5763,21 @@
         <v>241</v>
       </c>
       <c r="G157" s="5" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B158" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C158" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D158" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E158" s="1" t="s">
         <v>10</v>
@@ -5781,21 +5786,21 @@
         <v>241</v>
       </c>
       <c r="G158" s="5" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B159" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C159" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="D159" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E159" s="1" t="s">
         <v>10</v>
@@ -5804,93 +5809,93 @@
         <v>241</v>
       </c>
       <c r="G159" s="5" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
+        <v>399</v>
+      </c>
+      <c r="B160" t="s">
+        <v>279</v>
+      </c>
+      <c r="C160" t="s">
+        <v>400</v>
+      </c>
+      <c r="D160" t="s">
+        <v>496</v>
+      </c>
+      <c r="E160" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="F160" t="s">
         <v>401</v>
       </c>
-      <c r="B160" t="s">
-        <v>281</v>
-      </c>
-      <c r="C160" t="s">
+      <c r="G160" s="5" t="s">
         <v>402</v>
-      </c>
-      <c r="D160" t="s">
-        <v>498</v>
-      </c>
-      <c r="E160" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="F160" t="s">
-        <v>403</v>
-      </c>
-      <c r="G160" s="5" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
+        <v>403</v>
+      </c>
+      <c r="B161" t="s">
+        <v>279</v>
+      </c>
+      <c r="C161" t="s">
+        <v>404</v>
+      </c>
+      <c r="D161" t="s">
+        <v>496</v>
+      </c>
+      <c r="E161" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F161" t="s">
         <v>405</v>
       </c>
-      <c r="B161" t="s">
-        <v>281</v>
-      </c>
-      <c r="C161" t="s">
+      <c r="G161" s="5" t="s">
         <v>406</v>
-      </c>
-      <c r="D161" t="s">
-        <v>498</v>
-      </c>
-      <c r="E161" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F161" t="s">
-        <v>407</v>
-      </c>
-      <c r="G161" s="5" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B162" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C162" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D162" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E162" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F162" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="G162" s="5" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B163" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C163" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="D163" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="E163" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F163" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="G163" s="5">
         <v>92003</v>
@@ -5898,179 +5903,179 @@
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B164" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C164" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="D164" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="G164" s="5"/>
       <c r="H164" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B165" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C165" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="D165" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="G165" s="5"/>
       <c r="H165" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B166" t="s">
+        <v>459</v>
+      </c>
+      <c r="C166" t="s">
         <v>461</v>
       </c>
-      <c r="C166" t="s">
-        <v>463</v>
-      </c>
       <c r="D166" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="G166" s="5"/>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C167" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D167" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="G167" s="5"/>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B168" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C168" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D168" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="G168" s="5"/>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B169" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C169" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D169" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="G169" s="5"/>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B170" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C170" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="D170" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="G170" s="5"/>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B171" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C171" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D171" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="G171" s="5"/>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B172" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C172" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D172" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="G172" s="5"/>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C173" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="D173" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="G173" s="5"/>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B174" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C174" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D174" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="G174" s="5"/>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B175" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C175" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D175" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="G175" s="5"/>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B176" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C176" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="D176" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="G176" s="5"/>
     </row>
     <row r="177" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B177" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C177" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="D177" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="G177" s="5"/>
       <c r="H177" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
   </sheetData>
@@ -6210,14 +6215,15 @@
     <hyperlink ref="E24" r:id="rId133" xr:uid="{648BFDEF-0776-40CB-96BD-3105232BF7C5}"/>
     <hyperlink ref="E114" r:id="rId134" xr:uid="{E8DEB348-3B00-41C7-85D4-7BD6198F40E2}"/>
     <hyperlink ref="E26" r:id="rId135" xr:uid="{365853CB-05CC-49D9-935A-4155641501C2}"/>
+    <hyperlink ref="E20" r:id="rId136" xr:uid="{1434FB4A-AD21-4365-A9D6-F5C278481092}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId136"/>
+  <pageSetup orientation="portrait" r:id="rId137"/>
   <ignoredErrors>
     <ignoredError sqref="G108" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="1">
-    <tablePart r:id="rId137"/>
+    <tablePart r:id="rId138"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
New Handles, fan finger guard, plenty of part updates
## 2022-02-28

- Massive number of small edits to filenames, `Printed Part List.xlsx` and model to ensure consistency.
- Updated Raspberry Pi in the model, adding heatsink, HDMI adapter, and SD card.
- Removed even more stale STL files.
- Added PN111, a fan finger guard with about the right amount of spacing for a M3x35mm screw.
- Added SD cards, thumb screws, and other small details to the models.
- Updated the Readme file with my spare time while Fusion saves.
- Designed two styles of pull handles: one is narrow to fit the V-slot door, the other is 25mm wide for everywhere else. PN125 and 126
- Started work on wire pass-thrus for the flooring.
</commit_message>
<xml_diff>
--- a/BOM/General Part List.xlsx
+++ b/BOM/General Part List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\Documents\3D Print\Clockmaker\clock-3\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A0865F-359F-4E00-890D-FCD1E59AA660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC163C7-5CE1-4F48-9A1C-FC23815FCF97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="7" xr2:uid="{6EB0A7B6-C6D7-4759-8B58-841D5EFF92F5}"/>
+    <workbookView xWindow="-27600" yWindow="3060" windowWidth="23250" windowHeight="12480" firstSheet="1" activeTab="7" xr2:uid="{6EB0A7B6-C6D7-4759-8B58-841D5EFF92F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Electrical" sheetId="4" r:id="rId1"/>
@@ -20,8 +20,8 @@
     <sheet name="Supplies" sheetId="10" r:id="rId5"/>
     <sheet name="Toolhead" sheetId="7" r:id="rId6"/>
     <sheet name="Transmission" sheetId="9" r:id="rId7"/>
-    <sheet name="Part Codes" sheetId="1" r:id="rId8"/>
-    <sheet name="Default Values" sheetId="2" r:id="rId9"/>
+    <sheet name="Default Values" sheetId="2" r:id="rId8"/>
+    <sheet name="Part Codes" sheetId="1" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">Electrical!$A$1:$H$48</definedName>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2510" uniqueCount="584">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2555" uniqueCount="611">
   <si>
     <t>ID</t>
   </si>
@@ -1830,6 +1830,87 @@
   </si>
   <si>
     <t>Lily White Lubricating Oil</t>
+  </si>
+  <si>
+    <t>PN966</t>
+  </si>
+  <si>
+    <t>IEC C13 Cable, 1m</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>PIR Foam, 1/2", Rear Panel</t>
+  </si>
+  <si>
+    <t>PIR Foam, 1/2", Side Floor Cover, Rear</t>
+  </si>
+  <si>
+    <t>PIR Foam, 1/2", Side Floor Cover, Front</t>
+  </si>
+  <si>
+    <t>Z heatsinks optional</t>
+  </si>
+  <si>
+    <t>UN017</t>
+  </si>
+  <si>
+    <t>Heated Bed, 310x310mm</t>
+  </si>
+  <si>
+    <t>UN018</t>
+  </si>
+  <si>
+    <t>Micro SD to SD Extension</t>
+  </si>
+  <si>
+    <t>Heatsink, 14x14x6mm</t>
+  </si>
+  <si>
+    <t>For RPi</t>
+  </si>
+  <si>
+    <t>PN823</t>
+  </si>
+  <si>
+    <t>PN824</t>
+  </si>
+  <si>
+    <t>SD Card</t>
+  </si>
+  <si>
+    <t>Micro SD Card, Class A1</t>
+  </si>
+  <si>
+    <t>Class A1, 32GB</t>
+  </si>
+  <si>
+    <t>PN987</t>
+  </si>
+  <si>
+    <t>Buck Converter, 3A, USB C out</t>
+  </si>
+  <si>
+    <t>Must accept up 24VDC in.</t>
+  </si>
+  <si>
+    <t>Fan Grill Guard, 80mm</t>
+  </si>
+  <si>
+    <t>Must be plastic, not steel or another metal</t>
+  </si>
+  <si>
+    <t>Pull Handle, 90mm Holes</t>
+  </si>
+  <si>
+    <t>SanDisk</t>
+  </si>
+  <si>
+    <t>SDSQXAF-032G-GN6MA</t>
+  </si>
+  <si>
+    <t>Any size works; solely for flashing MCU.</t>
   </si>
 </sst>
 </file>
@@ -1910,7 +1991,10 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="50">
+  <dxfs count="51">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -2197,14 +2281,14 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4260B767-181E-4AB4-97E2-C92BA360A456}" name="Electrical" displayName="Electrical" ref="A1:H48" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:H48" xr:uid="{4260B767-181E-4AB4-97E2-C92BA360A456}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{D791B897-7CA3-455A-A34C-C1FCF05B96AD}" uniqueName="1" name="ID" queryTableFieldId="1" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{98B77A3B-123C-4C32-AF1E-EB52CF00B8F9}" uniqueName="2" name="Type" queryTableFieldId="2" dataDxfId="40"/>
-    <tableColumn id="3" xr3:uid="{7E0B359E-4CDE-4ADE-8978-74BE58FEF680}" uniqueName="3" name="Description String" queryTableFieldId="3" dataDxfId="39"/>
-    <tableColumn id="4" xr3:uid="{093110EE-05E5-4661-AD53-5C9DBE8D3496}" uniqueName="4" name="UOM" queryTableFieldId="4" dataDxfId="38"/>
-    <tableColumn id="5" xr3:uid="{D048A693-19DC-4300-987E-811281098CD9}" uniqueName="5" name="Ref Supplier" queryTableFieldId="5" dataDxfId="37"/>
-    <tableColumn id="6" xr3:uid="{4F0F47CC-8388-4676-881F-59C665A4E3E5}" uniqueName="6" name="Ref Mfgr" queryTableFieldId="6" dataDxfId="36"/>
+    <tableColumn id="1" xr3:uid="{D791B897-7CA3-455A-A34C-C1FCF05B96AD}" uniqueName="1" name="ID" queryTableFieldId="1" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{98B77A3B-123C-4C32-AF1E-EB52CF00B8F9}" uniqueName="2" name="Type" queryTableFieldId="2" dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{7E0B359E-4CDE-4ADE-8978-74BE58FEF680}" uniqueName="3" name="Description String" queryTableFieldId="3" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{093110EE-05E5-4661-AD53-5C9DBE8D3496}" uniqueName="4" name="UOM" queryTableFieldId="4" dataDxfId="39"/>
+    <tableColumn id="5" xr3:uid="{D048A693-19DC-4300-987E-811281098CD9}" uniqueName="5" name="Ref Supplier" queryTableFieldId="5" dataDxfId="38"/>
+    <tableColumn id="6" xr3:uid="{4F0F47CC-8388-4676-881F-59C665A4E3E5}" uniqueName="6" name="Ref Mfgr" queryTableFieldId="6" dataDxfId="37"/>
     <tableColumn id="7" xr3:uid="{644FAD62-0086-4A7C-AB2F-7D7BD14362BA}" uniqueName="7" name="Ref Mfgr PN" queryTableFieldId="7"/>
-    <tableColumn id="8" xr3:uid="{A263ED3B-A544-44B1-9085-B159535F541F}" uniqueName="8" name="Notes" queryTableFieldId="8" dataDxfId="35"/>
+    <tableColumn id="8" xr3:uid="{A263ED3B-A544-44B1-9085-B159535F541F}" uniqueName="8" name="Notes" queryTableFieldId="8" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2214,14 +2298,14 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{10C9598A-E171-4BE3-9A7C-07950EE5C687}" name="Fasteners" displayName="Fasteners" ref="A1:H37" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:H37" xr:uid="{10C9598A-E171-4BE3-9A7C-07950EE5C687}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{C1D2BBCD-78E5-4826-87F5-A5C04B89BBAC}" uniqueName="1" name="ID" queryTableFieldId="1" dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{32F37205-F979-4631-8EB6-78544BF5D278}" uniqueName="2" name="Type" queryTableFieldId="2" dataDxfId="33"/>
-    <tableColumn id="3" xr3:uid="{DEE8823E-50E3-43D4-A341-B081030250DB}" uniqueName="3" name="Description String" queryTableFieldId="3" dataDxfId="32"/>
-    <tableColumn id="4" xr3:uid="{EDCA880C-10D6-45DF-8A14-0DB0897568BD}" uniqueName="4" name="UOM" queryTableFieldId="4" dataDxfId="31"/>
-    <tableColumn id="5" xr3:uid="{10A4F109-7B07-4538-9F56-4C994A8179B2}" uniqueName="5" name="Ref Supplier" queryTableFieldId="5" dataDxfId="30"/>
-    <tableColumn id="6" xr3:uid="{8B097D17-5C82-497E-A60B-0DC71A57357D}" uniqueName="6" name="Ref Mfgr" queryTableFieldId="6" dataDxfId="29"/>
+    <tableColumn id="1" xr3:uid="{C1D2BBCD-78E5-4826-87F5-A5C04B89BBAC}" uniqueName="1" name="ID" queryTableFieldId="1" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{32F37205-F979-4631-8EB6-78544BF5D278}" uniqueName="2" name="Type" queryTableFieldId="2" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{DEE8823E-50E3-43D4-A341-B081030250DB}" uniqueName="3" name="Description String" queryTableFieldId="3" dataDxfId="33"/>
+    <tableColumn id="4" xr3:uid="{EDCA880C-10D6-45DF-8A14-0DB0897568BD}" uniqueName="4" name="UOM" queryTableFieldId="4" dataDxfId="32"/>
+    <tableColumn id="5" xr3:uid="{10A4F109-7B07-4538-9F56-4C994A8179B2}" uniqueName="5" name="Ref Supplier" queryTableFieldId="5" dataDxfId="31"/>
+    <tableColumn id="6" xr3:uid="{8B097D17-5C82-497E-A60B-0DC71A57357D}" uniqueName="6" name="Ref Mfgr" queryTableFieldId="6" dataDxfId="30"/>
     <tableColumn id="7" xr3:uid="{8AEDB347-2A07-4AD3-841A-53F750C7FF12}" uniqueName="7" name="Ref Mfgr PN" queryTableFieldId="7"/>
-    <tableColumn id="8" xr3:uid="{70FB6BD0-FDF9-4469-9B0D-B858BE78B550}" uniqueName="8" name="Notes" queryTableFieldId="8" dataDxfId="28"/>
+    <tableColumn id="8" xr3:uid="{70FB6BD0-FDF9-4469-9B0D-B858BE78B550}" uniqueName="8" name="Notes" queryTableFieldId="8" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2231,14 +2315,14 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1BDD4046-65F3-430B-995D-2264AC8164AE}" name="Framing" displayName="Framing" ref="A1:H52" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:H52" xr:uid="{1BDD4046-65F3-430B-995D-2264AC8164AE}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{C5ED764A-DDC6-4C43-9E3D-A13AF47C073B}" uniqueName="1" name="ID" queryTableFieldId="1" dataDxfId="48"/>
-    <tableColumn id="2" xr3:uid="{E35E7316-3770-4D37-B29F-DDE07655B6D5}" uniqueName="2" name="Type" queryTableFieldId="2" dataDxfId="47"/>
-    <tableColumn id="3" xr3:uid="{B8A1FA64-71CC-4352-8763-3CB67CA7C167}" uniqueName="3" name="Description String" queryTableFieldId="3" dataDxfId="46"/>
-    <tableColumn id="4" xr3:uid="{0E052177-3F19-4591-BABC-D51865AB00A2}" uniqueName="4" name="UOM" queryTableFieldId="4" dataDxfId="45"/>
-    <tableColumn id="5" xr3:uid="{16E729CE-7CA8-4D7B-A2DB-894E1ED6687E}" uniqueName="5" name="Ref Supplier" queryTableFieldId="5" dataDxfId="44"/>
-    <tableColumn id="6" xr3:uid="{95E40C72-A013-4DF2-9140-51D75C1FF8FF}" uniqueName="6" name="Ref Mfgr" queryTableFieldId="6" dataDxfId="43"/>
+    <tableColumn id="1" xr3:uid="{C5ED764A-DDC6-4C43-9E3D-A13AF47C073B}" uniqueName="1" name="ID" queryTableFieldId="1" dataDxfId="49"/>
+    <tableColumn id="2" xr3:uid="{E35E7316-3770-4D37-B29F-DDE07655B6D5}" uniqueName="2" name="Type" queryTableFieldId="2" dataDxfId="48"/>
+    <tableColumn id="3" xr3:uid="{B8A1FA64-71CC-4352-8763-3CB67CA7C167}" uniqueName="3" name="Description String" queryTableFieldId="3" dataDxfId="47"/>
+    <tableColumn id="4" xr3:uid="{0E052177-3F19-4591-BABC-D51865AB00A2}" uniqueName="4" name="UOM" queryTableFieldId="4" dataDxfId="46"/>
+    <tableColumn id="5" xr3:uid="{16E729CE-7CA8-4D7B-A2DB-894E1ED6687E}" uniqueName="5" name="Ref Supplier" queryTableFieldId="5" dataDxfId="45"/>
+    <tableColumn id="6" xr3:uid="{95E40C72-A013-4DF2-9140-51D75C1FF8FF}" uniqueName="6" name="Ref Mfgr" queryTableFieldId="6" dataDxfId="44"/>
     <tableColumn id="7" xr3:uid="{914A5065-23DE-4B04-99CF-8C90B5FD0CA2}" uniqueName="7" name="Ref Mfgr PN" queryTableFieldId="7"/>
-    <tableColumn id="8" xr3:uid="{86485893-7DA3-4F2F-95AA-35919E356E68}" uniqueName="8" name="Notes" queryTableFieldId="8" dataDxfId="42"/>
+    <tableColumn id="8" xr3:uid="{86485893-7DA3-4F2F-95AA-35919E356E68}" uniqueName="8" name="Notes" queryTableFieldId="8" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2248,14 +2332,14 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{2660B5B0-B0D6-43FF-84AB-A3F180AEA3F7}" name="Misc" displayName="Misc" ref="A1:H17" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:H17" xr:uid="{2660B5B0-B0D6-43FF-84AB-A3F180AEA3F7}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{0E61CC9D-0690-4560-A41A-E0A16444A11A}" uniqueName="1" name="ID" queryTableFieldId="1" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{30FD13E6-29F4-4AEB-890A-F9D364C03732}" uniqueName="2" name="Type" queryTableFieldId="2" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{2BBA0BE4-9384-4589-88A0-7F11239D48AF}" uniqueName="3" name="Description String" queryTableFieldId="3" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{3B9D3BC9-F027-4FA7-B27D-02424CFA69BB}" uniqueName="4" name="UOM" queryTableFieldId="4" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{694A7969-FFB6-410E-9872-D21B0704DE75}" uniqueName="5" name="Ref Supplier" queryTableFieldId="5" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{C50F669B-D04F-4788-901C-D096CCA79D82}" uniqueName="6" name="Ref Mfgr" queryTableFieldId="6" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{0E61CC9D-0690-4560-A41A-E0A16444A11A}" uniqueName="1" name="ID" queryTableFieldId="1" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{30FD13E6-29F4-4AEB-890A-F9D364C03732}" uniqueName="2" name="Type" queryTableFieldId="2" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{2BBA0BE4-9384-4589-88A0-7F11239D48AF}" uniqueName="3" name="Description String" queryTableFieldId="3" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{3B9D3BC9-F027-4FA7-B27D-02424CFA69BB}" uniqueName="4" name="UOM" queryTableFieldId="4" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{694A7969-FFB6-410E-9872-D21B0704DE75}" uniqueName="5" name="Ref Supplier" queryTableFieldId="5" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{C50F669B-D04F-4788-901C-D096CCA79D82}" uniqueName="6" name="Ref Mfgr" queryTableFieldId="6" dataDxfId="23"/>
     <tableColumn id="7" xr3:uid="{9384A680-B33F-4DE9-B5BF-166ACCD77017}" uniqueName="7" name="Ref Mfgr PN" queryTableFieldId="7"/>
-    <tableColumn id="8" xr3:uid="{B710B06E-11E7-4E9F-B829-CA26A2400DDB}" uniqueName="8" name="Notes" queryTableFieldId="8" dataDxfId="21"/>
+    <tableColumn id="8" xr3:uid="{B710B06E-11E7-4E9F-B829-CA26A2400DDB}" uniqueName="8" name="Notes" queryTableFieldId="8" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2265,14 +2349,14 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{AABA9D3A-02DA-409F-ABC6-21BADA70C55E}" name="Supplies" displayName="Supplies" ref="A1:H18" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:H18" xr:uid="{AABA9D3A-02DA-409F-ABC6-21BADA70C55E}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{348C0250-F42A-412E-9197-F208C6431A02}" uniqueName="1" name="ID" queryTableFieldId="1" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{3629EDA8-49DA-40A5-B84A-D18F3DF0D186}" uniqueName="2" name="Type" queryTableFieldId="2" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{DF2A4E09-86C6-43F7-8F28-3879E18FAA5A}" uniqueName="3" name="Description String" queryTableFieldId="3" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{934B53B9-43A8-412D-9AA2-F61C3B1495F0}" uniqueName="4" name="UOM" queryTableFieldId="4" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{3C209CA0-21DF-4C36-BD22-365F9C9C4A7D}" uniqueName="5" name="Ref Supplier" queryTableFieldId="5" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{6FEF683B-8D43-4EA3-963D-D5E10D36507F}" uniqueName="6" name="Ref Mfgr" queryTableFieldId="6" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{348C0250-F42A-412E-9197-F208C6431A02}" uniqueName="1" name="ID" queryTableFieldId="1" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{3629EDA8-49DA-40A5-B84A-D18F3DF0D186}" uniqueName="2" name="Type" queryTableFieldId="2" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{DF2A4E09-86C6-43F7-8F28-3879E18FAA5A}" uniqueName="3" name="Description String" queryTableFieldId="3" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{934B53B9-43A8-412D-9AA2-F61C3B1495F0}" uniqueName="4" name="UOM" queryTableFieldId="4" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{3C209CA0-21DF-4C36-BD22-365F9C9C4A7D}" uniqueName="5" name="Ref Supplier" queryTableFieldId="5" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{6FEF683B-8D43-4EA3-963D-D5E10D36507F}" uniqueName="6" name="Ref Mfgr" queryTableFieldId="6" dataDxfId="16"/>
     <tableColumn id="7" xr3:uid="{D8C29579-2A2B-450D-860F-5358B567EBE5}" uniqueName="7" name="Ref Mfgr PN" queryTableFieldId="7"/>
-    <tableColumn id="8" xr3:uid="{57203ED6-26D8-4B30-931A-DA598B6871B5}" uniqueName="8" name="Notes" queryTableFieldId="8" dataDxfId="14"/>
+    <tableColumn id="8" xr3:uid="{57203ED6-26D8-4B30-931A-DA598B6871B5}" uniqueName="8" name="Notes" queryTableFieldId="8" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2282,14 +2366,14 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{B16CB437-03BE-4C78-BE0F-AAB4BAA6005A}" name="Toolhead" displayName="Toolhead" ref="A1:H5" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:H5" xr:uid="{B16CB437-03BE-4C78-BE0F-AAB4BAA6005A}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{8ED14874-2F87-4B7D-8DC5-CCAC7F570B29}" uniqueName="1" name="ID" queryTableFieldId="1" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{835E7DB3-3442-428D-ADAF-8388FC119BA0}" uniqueName="2" name="Type" queryTableFieldId="2" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{61B49CF9-52E6-48F5-838D-14F7875E24AD}" uniqueName="3" name="Description String" queryTableFieldId="3" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{1167378B-95E1-4CDC-BD82-F1C523211FFB}" uniqueName="4" name="UOM" queryTableFieldId="4" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{4FA174D6-370C-45F4-AF93-A68E4D66866C}" uniqueName="5" name="Ref Supplier" queryTableFieldId="5" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{9C3900BA-052E-4804-B0F6-25FEED984705}" uniqueName="6" name="Ref Mfgr" queryTableFieldId="6" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{8ED14874-2F87-4B7D-8DC5-CCAC7F570B29}" uniqueName="1" name="ID" queryTableFieldId="1" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{835E7DB3-3442-428D-ADAF-8388FC119BA0}" uniqueName="2" name="Type" queryTableFieldId="2" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{61B49CF9-52E6-48F5-838D-14F7875E24AD}" uniqueName="3" name="Description String" queryTableFieldId="3" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{1167378B-95E1-4CDC-BD82-F1C523211FFB}" uniqueName="4" name="UOM" queryTableFieldId="4" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{4FA174D6-370C-45F4-AF93-A68E4D66866C}" uniqueName="5" name="Ref Supplier" queryTableFieldId="5" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{9C3900BA-052E-4804-B0F6-25FEED984705}" uniqueName="6" name="Ref Mfgr" queryTableFieldId="6" dataDxfId="2"/>
     <tableColumn id="7" xr3:uid="{302B25EC-488D-48CF-8D39-5B48BC7F5691}" uniqueName="7" name="Ref Mfgr PN" queryTableFieldId="7"/>
-    <tableColumn id="8" xr3:uid="{FF2587EA-CBFF-46C3-90AB-6F369227E421}" uniqueName="8" name="Notes" queryTableFieldId="8" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{FF2587EA-CBFF-46C3-90AB-6F369227E421}" uniqueName="8" name="Notes" queryTableFieldId="8" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2299,24 +2383,36 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{43592D39-3E6E-4862-B567-02A63CEABEAE}" name="Transmission" displayName="Transmission" ref="A1:H13" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:H13" xr:uid="{43592D39-3E6E-4862-B567-02A63CEABEAE}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{F64224BC-30E1-43CA-B79D-7715583B125F}" uniqueName="1" name="ID" queryTableFieldId="1" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{E7F0D748-E283-48CA-A804-7FE69A6801F6}" uniqueName="2" name="Type" queryTableFieldId="2" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{1608A168-8D92-4F72-9725-9D15AF4DF03D}" uniqueName="3" name="Description String" queryTableFieldId="3" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{25255DA7-E062-408D-AC96-358AE9F6B3A8}" uniqueName="4" name="UOM" queryTableFieldId="4" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{9278596B-DF57-47DA-977F-86D88A6872F9}" uniqueName="5" name="Ref Supplier" queryTableFieldId="5" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{A4C3A866-96D9-4A0A-9FEE-DC8F1B0E0AF1}" uniqueName="6" name="Ref Mfgr" queryTableFieldId="6" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{F64224BC-30E1-43CA-B79D-7715583B125F}" uniqueName="1" name="ID" queryTableFieldId="1" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{E7F0D748-E283-48CA-A804-7FE69A6801F6}" uniqueName="2" name="Type" queryTableFieldId="2" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{1608A168-8D92-4F72-9725-9D15AF4DF03D}" uniqueName="3" name="Description String" queryTableFieldId="3" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{25255DA7-E062-408D-AC96-358AE9F6B3A8}" uniqueName="4" name="UOM" queryTableFieldId="4" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{9278596B-DF57-47DA-977F-86D88A6872F9}" uniqueName="5" name="Ref Supplier" queryTableFieldId="5" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{A4C3A866-96D9-4A0A-9FEE-DC8F1B0E0AF1}" uniqueName="6" name="Ref Mfgr" queryTableFieldId="6" dataDxfId="9"/>
     <tableColumn id="7" xr3:uid="{8C60E940-59AC-48F1-A6DB-5345E699C7BD}" uniqueName="7" name="Ref Mfgr PN" queryTableFieldId="7"/>
-    <tableColumn id="8" xr3:uid="{653FEA69-C86A-42D0-9117-FD1D5A0A58B6}" uniqueName="8" name="Notes" queryTableFieldId="8" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{653FEA69-C86A-42D0-9117-FD1D5A0A58B6}" uniqueName="8" name="Notes" queryTableFieldId="8" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BCCEB002-6247-475F-8E59-4D3290F5D0AB}" name="Table13" displayName="Table13" ref="A1:H185" totalsRowShown="0">
-  <autoFilter ref="A1:H185" xr:uid="{BCCEB002-6247-475F-8E59-4D3290F5D0AB}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H184">
-    <sortCondition ref="A1:A184"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{7676A875-1964-41AB-918A-9C0D9855E0B8}" name="Table9" displayName="Table9" ref="A1:C8" totalsRowShown="0">
+  <autoFilter ref="A1:C8" xr:uid="{7676A875-1964-41AB-918A-9C0D9855E0B8}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{A802BA72-926A-46D8-9780-D60FFCDAB3DF}" name="ID"/>
+    <tableColumn id="2" xr3:uid="{6F37B796-105C-4A29-AD6D-50AF2CA7B7AC}" name="Qty"/>
+    <tableColumn id="3" xr3:uid="{B5412E12-4127-403A-B127-C77D20E89F69}" name="UOM" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BCCEB002-6247-475F-8E59-4D3290F5D0AB}" name="Table13" displayName="Table13" ref="A1:H189" totalsRowShown="0">
+  <autoFilter ref="A1:H189" xr:uid="{BCCEB002-6247-475F-8E59-4D3290F5D0AB}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H189">
+    <sortCondition ref="A1:A189"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{5013DA2C-AE55-4442-B536-8693A638A779}" name="ID"/>
@@ -2325,7 +2421,7 @@
     <tableColumn id="3" xr3:uid="{5BC43D25-FC61-43F5-AAA6-A95F7C6253BB}" name="UOM"/>
     <tableColumn id="4" xr3:uid="{266B9222-B8C0-42F4-A609-77FADF3190D7}" name="Ref Supplier"/>
     <tableColumn id="5" xr3:uid="{DF9FDF93-7823-426E-9E96-0C1089D2AEB8}" name="Ref Mfgr"/>
-    <tableColumn id="7" xr3:uid="{17D8E79D-E73F-4CC1-82CE-55E0FC757E96}" name="Ref Mfgr PN" dataDxfId="49"/>
+    <tableColumn id="7" xr3:uid="{17D8E79D-E73F-4CC1-82CE-55E0FC757E96}" name="Ref Mfgr PN" dataDxfId="50"/>
     <tableColumn id="8" xr3:uid="{FF1147A0-E60B-465B-8E2F-C451EF509326}" name="Notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2631,7 +2727,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2311C413-BD03-4A1E-950D-0B2A8E7F4C8A}">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -3810,7 +3906,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17FB0674-52C5-46E6-AD95-3C49D3B43E74}">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5899,7 +5997,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H17"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6710,7 +6808,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7200,11 +7298,120 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE3AEE9E-D21D-4ECD-BA1D-6BDD55688F9A}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>586</v>
+      </c>
+      <c r="C1" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>584</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>261</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>268</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>308</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>309</v>
+      </c>
+      <c r="B7">
+        <v>1.2</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>584</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>488</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D318B5EB-87D8-4D97-AE82-574AF33D7DA4}">
-  <dimension ref="A1:H185"/>
+  <dimension ref="A1:H189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="J163" sqref="J163"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="H69" sqref="H69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8567,16 +8774,22 @@
         <v>139</v>
       </c>
       <c r="C59" t="s">
-        <v>484</v>
+        <v>607</v>
       </c>
       <c r="D59" t="s">
         <v>488</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F59" t="s">
+        <v>67</v>
       </c>
       <c r="G59" s="5" t="s">
         <v>155</v>
       </c>
       <c r="H59" s="4" t="s">
-        <v>156</v>
+        <v>606</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -8808,39 +9021,39 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="B69" t="s">
         <v>139</v>
       </c>
       <c r="C69" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="D69" t="s">
         <v>488</v>
       </c>
-      <c r="E69" t="s">
+      <c r="E69" s="1" t="s">
         <v>141</v>
       </c>
       <c r="F69" t="s">
         <v>37</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="H69" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="B70" t="s">
         <v>139</v>
       </c>
       <c r="C70" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="D70" t="s">
         <v>488</v>
@@ -8852,7 +9065,7 @@
         <v>37</v>
       </c>
       <c r="G70" s="5" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="H70" t="s">
         <v>189</v>
@@ -8860,13 +9073,13 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="B71" t="s">
         <v>139</v>
       </c>
       <c r="C71" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="D71" t="s">
         <v>488</v>
@@ -8878,21 +9091,21 @@
         <v>37</v>
       </c>
       <c r="G71" s="5" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="H71" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="B72" t="s">
         <v>139</v>
       </c>
       <c r="C72" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="D72" t="s">
         <v>488</v>
@@ -8904,21 +9117,21 @@
         <v>37</v>
       </c>
       <c r="G72" s="5" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="H72" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="B73" t="s">
         <v>139</v>
       </c>
       <c r="C73" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="D73" t="s">
         <v>488</v>
@@ -8930,21 +9143,21 @@
         <v>37</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="H73" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="B74" t="s">
         <v>139</v>
       </c>
       <c r="C74" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="D74" t="s">
         <v>488</v>
@@ -8956,21 +9169,21 @@
         <v>37</v>
       </c>
       <c r="G74" s="5" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="H74" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="B75" t="s">
         <v>139</v>
       </c>
       <c r="C75" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="D75" t="s">
         <v>488</v>
@@ -8982,21 +9195,21 @@
         <v>37</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="H75" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="B76" t="s">
         <v>139</v>
       </c>
       <c r="C76" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="D76" t="s">
         <v>488</v>
@@ -9008,47 +9221,45 @@
         <v>37</v>
       </c>
       <c r="G76" s="5" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="H76" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="B77" t="s">
         <v>139</v>
       </c>
       <c r="C77" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="D77" t="s">
         <v>488</v>
       </c>
-      <c r="E77" s="1" t="s">
-        <v>141</v>
+      <c r="E77" t="s">
+        <v>219</v>
       </c>
       <c r="F77" t="s">
-        <v>37</v>
-      </c>
-      <c r="G77" s="5" t="s">
-        <v>215</v>
-      </c>
+        <v>219</v>
+      </c>
+      <c r="G77" s="5"/>
       <c r="H77" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="B78" t="s">
         <v>139</v>
       </c>
       <c r="C78" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="D78" t="s">
         <v>488</v>
@@ -9061,18 +9272,18 @@
       </c>
       <c r="G78" s="5"/>
       <c r="H78" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="B79" t="s">
         <v>139</v>
       </c>
       <c r="C79" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="D79" t="s">
         <v>488</v>
@@ -9084,19 +9295,16 @@
         <v>219</v>
       </c>
       <c r="G79" s="5"/>
-      <c r="H79" t="s">
-        <v>223</v>
-      </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B80" t="s">
         <v>139</v>
       </c>
       <c r="C80" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D80" t="s">
         <v>488</v>
@@ -9111,13 +9319,13 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B81" t="s">
         <v>139</v>
       </c>
       <c r="C81" t="s">
-        <v>227</v>
+        <v>473</v>
       </c>
       <c r="D81" t="s">
         <v>488</v>
@@ -9132,13 +9340,13 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B82" t="s">
         <v>139</v>
       </c>
       <c r="C82" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="D82" t="s">
         <v>488</v>
@@ -9153,13 +9361,13 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B83" t="s">
         <v>139</v>
       </c>
       <c r="C83" t="s">
-        <v>474</v>
+        <v>231</v>
       </c>
       <c r="D83" t="s">
         <v>488</v>
@@ -9174,13 +9382,13 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B84" t="s">
         <v>139</v>
       </c>
       <c r="C84" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="D84" t="s">
         <v>488</v>
@@ -9195,13 +9403,13 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B85" t="s">
         <v>139</v>
       </c>
       <c r="C85" t="s">
-        <v>233</v>
+        <v>574</v>
       </c>
       <c r="D85" t="s">
         <v>488</v>
@@ -9216,13 +9424,13 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B86" t="s">
         <v>139</v>
       </c>
       <c r="C86" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="D86" t="s">
         <v>488</v>
@@ -9237,13 +9445,13 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>235</v>
+        <v>475</v>
       </c>
       <c r="B87" t="s">
         <v>139</v>
       </c>
       <c r="C87" t="s">
-        <v>575</v>
+        <v>476</v>
       </c>
       <c r="D87" t="s">
         <v>488</v>
@@ -9258,13 +9466,13 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="B88" t="s">
         <v>139</v>
       </c>
       <c r="C88" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
       <c r="D88" t="s">
         <v>488</v>
@@ -9279,13 +9487,13 @@
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B89" t="s">
         <v>139</v>
       </c>
       <c r="C89" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="D89" t="s">
         <v>488</v>
@@ -9300,13 +9508,13 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="B90" t="s">
         <v>139</v>
       </c>
       <c r="C90" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="D90" t="s">
         <v>488</v>
@@ -9321,13 +9529,13 @@
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>481</v>
+        <v>532</v>
       </c>
       <c r="B91" t="s">
         <v>139</v>
       </c>
       <c r="C91" t="s">
-        <v>482</v>
+        <v>544</v>
       </c>
       <c r="D91" t="s">
         <v>488</v>
@@ -9339,40 +9547,37 @@
         <v>219</v>
       </c>
       <c r="G91" s="5"/>
+      <c r="H91" t="s">
+        <v>533</v>
+      </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>532</v>
+        <v>499</v>
       </c>
       <c r="B92" t="s">
         <v>139</v>
       </c>
       <c r="C92" t="s">
-        <v>544</v>
+        <v>587</v>
       </c>
       <c r="D92" t="s">
         <v>488</v>
-      </c>
-      <c r="E92" t="s">
-        <v>219</v>
-      </c>
-      <c r="F92" t="s">
-        <v>219</v>
       </c>
       <c r="G92" s="5"/>
       <c r="H92" t="s">
-        <v>533</v>
+        <v>509</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="B93" t="s">
         <v>139</v>
       </c>
       <c r="C93" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D93" t="s">
         <v>488</v>
@@ -9384,13 +9589,13 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B94" t="s">
         <v>139</v>
       </c>
       <c r="C94" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="D94" t="s">
         <v>488</v>
@@ -9402,31 +9607,31 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>501</v>
+        <v>506</v>
       </c>
       <c r="B95" t="s">
         <v>139</v>
       </c>
       <c r="C95" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="D95" t="s">
         <v>488</v>
       </c>
       <c r="G95" s="5"/>
       <c r="H95" t="s">
-        <v>509</v>
+        <v>518</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="B96" t="s">
         <v>139</v>
       </c>
       <c r="C96" t="s">
-        <v>505</v>
+        <v>508</v>
       </c>
       <c r="D96" t="s">
         <v>488</v>
@@ -9438,13 +9643,13 @@
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>507</v>
+        <v>510</v>
       </c>
       <c r="B97" t="s">
         <v>139</v>
       </c>
       <c r="C97" t="s">
-        <v>508</v>
+        <v>514</v>
       </c>
       <c r="D97" t="s">
         <v>488</v>
@@ -9456,49 +9661,49 @@
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="B98" t="s">
         <v>139</v>
       </c>
       <c r="C98" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="D98" t="s">
         <v>488</v>
       </c>
       <c r="G98" s="5"/>
       <c r="H98" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="B99" t="s">
         <v>139</v>
       </c>
       <c r="C99" t="s">
-        <v>515</v>
+        <v>588</v>
       </c>
       <c r="D99" t="s">
         <v>488</v>
       </c>
       <c r="G99" s="5"/>
       <c r="H99" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="B100" t="s">
         <v>139</v>
       </c>
       <c r="C100" t="s">
-        <v>516</v>
+        <v>589</v>
       </c>
       <c r="D100" t="s">
         <v>488</v>
@@ -9510,55 +9715,58 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>513</v>
+        <v>536</v>
       </c>
       <c r="B101" t="s">
         <v>139</v>
       </c>
       <c r="C101" t="s">
-        <v>517</v>
+        <v>538</v>
       </c>
       <c r="D101" t="s">
-        <v>488</v>
+        <v>537</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="F101" t="s">
+        <v>67</v>
       </c>
       <c r="G101" s="5"/>
       <c r="H101" t="s">
-        <v>518</v>
+        <v>539</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>536</v>
+        <v>576</v>
       </c>
       <c r="B102" t="s">
         <v>139</v>
       </c>
       <c r="C102" t="s">
-        <v>538</v>
+        <v>578</v>
       </c>
       <c r="D102" t="s">
-        <v>537</v>
-      </c>
-      <c r="E102" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="F102" t="s">
-        <v>67</v>
+        <v>488</v>
+      </c>
+      <c r="E102" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="F102" s="6" t="s">
+        <v>219</v>
       </c>
       <c r="G102" s="5"/>
-      <c r="H102" t="s">
-        <v>539</v>
-      </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="B103" t="s">
         <v>139</v>
       </c>
       <c r="C103" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="D103" t="s">
         <v>488</v>
@@ -9573,34 +9781,34 @@
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>577</v>
+        <v>236</v>
       </c>
       <c r="B104" t="s">
-        <v>139</v>
+        <v>237</v>
       </c>
       <c r="C104" t="s">
-        <v>579</v>
+        <v>238</v>
       </c>
       <c r="D104" t="s">
         <v>488</v>
       </c>
-      <c r="E104" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="F104" s="6" t="s">
-        <v>219</v>
+      <c r="E104" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F104" t="s">
+        <v>239</v>
       </c>
       <c r="G104" s="5"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="B105" t="s">
         <v>237</v>
       </c>
       <c r="C105" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="D105" t="s">
         <v>488</v>
@@ -9612,16 +9820,19 @@
         <v>239</v>
       </c>
       <c r="G105" s="5"/>
+      <c r="H105" t="s">
+        <v>590</v>
+      </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B106" t="s">
         <v>237</v>
       </c>
       <c r="C106" t="s">
-        <v>241</v>
+        <v>595</v>
       </c>
       <c r="D106" t="s">
         <v>488</v>
@@ -9630,19 +9841,22 @@
         <v>10</v>
       </c>
       <c r="F106" t="s">
-        <v>239</v>
+        <v>67</v>
       </c>
       <c r="G106" s="5"/>
+      <c r="H106" t="s">
+        <v>596</v>
+      </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="B107" t="s">
         <v>237</v>
       </c>
       <c r="C107" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="D107" t="s">
         <v>488</v>
@@ -9651,19 +9865,24 @@
         <v>10</v>
       </c>
       <c r="F107" t="s">
-        <v>244</v>
-      </c>
-      <c r="G107" s="5"/>
+        <v>56</v>
+      </c>
+      <c r="G107" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="H107" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B108" t="s">
         <v>237</v>
       </c>
       <c r="C108" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="D108" t="s">
         <v>488</v>
@@ -9683,13 +9902,13 @@
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="B109" t="s">
         <v>237</v>
       </c>
       <c r="C109" t="s">
-        <v>248</v>
+        <v>592</v>
       </c>
       <c r="D109" t="s">
         <v>488</v>
@@ -9698,102 +9917,100 @@
         <v>10</v>
       </c>
       <c r="F109" t="s">
-        <v>56</v>
+        <v>251</v>
       </c>
       <c r="G109" s="5" t="s">
-        <v>57</v>
+        <v>252</v>
       </c>
       <c r="H109" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="B110" t="s">
         <v>237</v>
       </c>
       <c r="C110" t="s">
-        <v>534</v>
+        <v>255</v>
       </c>
       <c r="D110" t="s">
         <v>488</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>10</v>
+        <v>256</v>
       </c>
       <c r="F110" t="s">
-        <v>251</v>
-      </c>
-      <c r="G110" s="5" t="s">
-        <v>252</v>
+        <v>256</v>
+      </c>
+      <c r="G110" s="5">
+        <v>570</v>
       </c>
       <c r="H110" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="B111" t="s">
         <v>237</v>
       </c>
       <c r="C111" t="s">
-        <v>255</v>
+        <v>535</v>
       </c>
       <c r="D111" t="s">
         <v>488</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>256</v>
+        <v>10</v>
       </c>
       <c r="F111" t="s">
-        <v>256</v>
-      </c>
-      <c r="G111" s="5">
-        <v>570</v>
-      </c>
-      <c r="H111" t="s">
-        <v>257</v>
+        <v>259</v>
+      </c>
+      <c r="G111" s="5" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="B112" t="s">
         <v>237</v>
       </c>
       <c r="C112" t="s">
-        <v>535</v>
+        <v>262</v>
       </c>
       <c r="D112" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F112" t="s">
-        <v>259</v>
-      </c>
-      <c r="G112" s="5" t="s">
-        <v>260</v>
+        <v>67</v>
+      </c>
+      <c r="G112" s="5"/>
+      <c r="H112" t="s">
+        <v>497</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B113" t="s">
         <v>237</v>
       </c>
       <c r="C113" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="D113" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>10</v>
@@ -9802,22 +10019,19 @@
         <v>67</v>
       </c>
       <c r="G113" s="5"/>
-      <c r="H113" t="s">
-        <v>497</v>
-      </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="B114" t="s">
         <v>237</v>
       </c>
       <c r="C114" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="D114" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="E114" s="1" t="s">
         <v>10</v>
@@ -9826,43 +10040,46 @@
         <v>67</v>
       </c>
       <c r="G114" s="5"/>
+      <c r="H114" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="B115" t="s">
         <v>237</v>
       </c>
       <c r="C115" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
       <c r="D115" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F115" t="s">
-        <v>267</v>
+        <v>67</v>
       </c>
       <c r="G115" s="5"/>
       <c r="H115" t="s">
-        <v>498</v>
+        <v>273</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="B116" t="s">
         <v>237</v>
       </c>
       <c r="C116" t="s">
-        <v>269</v>
+        <v>605</v>
       </c>
       <c r="D116" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>10</v>
@@ -9871,19 +10088,16 @@
         <v>67</v>
       </c>
       <c r="G116" s="5"/>
-      <c r="H116" t="s">
-        <v>270</v>
-      </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>271</v>
+        <v>525</v>
       </c>
       <c r="B117" t="s">
         <v>237</v>
       </c>
       <c r="C117" t="s">
-        <v>272</v>
+        <v>524</v>
       </c>
       <c r="D117" t="s">
         <v>488</v>
@@ -9896,18 +10110,18 @@
       </c>
       <c r="G117" s="5"/>
       <c r="H117" t="s">
-        <v>273</v>
+        <v>526</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>274</v>
+        <v>541</v>
       </c>
       <c r="B118" t="s">
         <v>237</v>
       </c>
       <c r="C118" t="s">
-        <v>275</v>
+        <v>542</v>
       </c>
       <c r="D118" t="s">
         <v>488</v>
@@ -9919,16 +10133,19 @@
         <v>67</v>
       </c>
       <c r="G118" s="5"/>
+      <c r="H118" t="s">
+        <v>543</v>
+      </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>525</v>
+        <v>597</v>
       </c>
       <c r="B119" t="s">
         <v>237</v>
       </c>
       <c r="C119" t="s">
-        <v>524</v>
+        <v>600</v>
       </c>
       <c r="D119" t="s">
         <v>488</v>
@@ -9937,27 +10154,26 @@
         <v>10</v>
       </c>
       <c r="F119" t="s">
-        <v>67</v>
-      </c>
-      <c r="G119" s="5"/>
+        <v>608</v>
+      </c>
+      <c r="G119" s="5" t="s">
+        <v>609</v>
+      </c>
       <c r="H119" t="s">
-        <v>526</v>
+        <v>601</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>541</v>
+        <v>598</v>
       </c>
       <c r="B120" t="s">
         <v>237</v>
       </c>
       <c r="C120" t="s">
-        <v>542</v>
-      </c>
-      <c r="D120" t="s">
-        <v>488</v>
-      </c>
-      <c r="E120" s="6" t="s">
+        <v>599</v>
+      </c>
+      <c r="E120" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F120" t="s">
@@ -9965,7 +10181,7 @@
       </c>
       <c r="G120" s="5"/>
       <c r="H120" t="s">
-        <v>543</v>
+        <v>610</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
@@ -10803,7 +11019,7 @@
         <v>277</v>
       </c>
       <c r="C156" t="s">
-        <v>374</v>
+        <v>594</v>
       </c>
       <c r="D156" t="s">
         <v>488</v>
@@ -10873,37 +11089,32 @@
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>384</v>
+        <v>584</v>
       </c>
       <c r="B159" t="s">
         <v>277</v>
       </c>
       <c r="C159" t="s">
-        <v>385</v>
+        <v>585</v>
       </c>
       <c r="D159" t="s">
         <v>488</v>
       </c>
-      <c r="E159" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="E159" s="1"/>
       <c r="F159" t="s">
         <v>67</v>
       </c>
       <c r="G159" s="5"/>
-      <c r="H159" t="s">
-        <v>386</v>
-      </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="B160" t="s">
         <v>277</v>
       </c>
       <c r="C160" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="D160" t="s">
         <v>488</v>
@@ -10912,21 +11123,22 @@
         <v>10</v>
       </c>
       <c r="F160" t="s">
-        <v>117</v>
-      </c>
-      <c r="G160" s="5" t="s">
-        <v>455</v>
+        <v>67</v>
+      </c>
+      <c r="G160" s="5"/>
+      <c r="H160" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B161" t="s">
         <v>277</v>
       </c>
       <c r="C161" t="s">
-        <v>453</v>
+        <v>388</v>
       </c>
       <c r="D161" t="s">
         <v>488</v>
@@ -10934,20 +11146,22 @@
       <c r="E161" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G161" s="5"/>
-      <c r="H161" t="s">
-        <v>454</v>
+      <c r="F161" t="s">
+        <v>117</v>
+      </c>
+      <c r="G161" s="5" t="s">
+        <v>455</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B162" t="s">
         <v>277</v>
       </c>
       <c r="C162" t="s">
-        <v>470</v>
+        <v>453</v>
       </c>
       <c r="D162" t="s">
         <v>488</v>
@@ -10955,22 +11169,20 @@
       <c r="E162" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F162" t="s">
-        <v>239</v>
-      </c>
-      <c r="G162" s="5" t="s">
-        <v>391</v>
+      <c r="G162" s="5"/>
+      <c r="H162" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B163" t="s">
         <v>277</v>
       </c>
       <c r="C163" t="s">
-        <v>393</v>
+        <v>470</v>
       </c>
       <c r="D163" t="s">
         <v>488</v>
@@ -10982,18 +11194,18 @@
         <v>239</v>
       </c>
       <c r="G163" s="5" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="B164" t="s">
         <v>277</v>
       </c>
       <c r="C164" t="s">
-        <v>469</v>
+        <v>393</v>
       </c>
       <c r="D164" t="s">
         <v>488</v>
@@ -11005,64 +11217,64 @@
         <v>239</v>
       </c>
       <c r="G164" s="5" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B165" t="s">
         <v>277</v>
       </c>
       <c r="C165" t="s">
-        <v>398</v>
+        <v>469</v>
       </c>
       <c r="D165" t="s">
         <v>488</v>
       </c>
       <c r="E165" s="1" t="s">
-        <v>296</v>
+        <v>10</v>
       </c>
       <c r="F165" t="s">
-        <v>399</v>
+        <v>239</v>
       </c>
       <c r="G165" s="5" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="B166" t="s">
         <v>277</v>
       </c>
       <c r="C166" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="D166" t="s">
         <v>488</v>
       </c>
       <c r="E166" s="1" t="s">
-        <v>10</v>
+        <v>296</v>
       </c>
       <c r="F166" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="G166" s="5" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="B167" t="s">
         <v>277</v>
       </c>
       <c r="C167" t="s">
-        <v>452</v>
+        <v>402</v>
       </c>
       <c r="D167" t="s">
         <v>488</v>
@@ -11071,92 +11283,109 @@
         <v>10</v>
       </c>
       <c r="F167" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="G167" s="5" t="s">
-        <v>451</v>
+        <v>404</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>548</v>
+        <v>405</v>
       </c>
       <c r="B168" t="s">
-        <v>456</v>
+        <v>277</v>
       </c>
       <c r="C168" t="s">
-        <v>486</v>
+        <v>452</v>
       </c>
       <c r="D168" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="E168" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F168" t="s">
-        <v>472</v>
-      </c>
-      <c r="G168" s="5">
-        <v>92003</v>
+        <v>406</v>
+      </c>
+      <c r="G168" s="5" t="s">
+        <v>451</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>549</v>
+        <v>602</v>
       </c>
       <c r="B169" t="s">
-        <v>456</v>
+        <v>277</v>
       </c>
       <c r="C169" t="s">
-        <v>457</v>
+        <v>603</v>
       </c>
       <c r="D169" t="s">
-        <v>491</v>
+        <v>488</v>
+      </c>
+      <c r="E169" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F169" t="s">
+        <v>67</v>
       </c>
       <c r="G169" s="5"/>
       <c r="H169" t="s">
-        <v>471</v>
+        <v>604</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B170" t="s">
         <v>456</v>
       </c>
       <c r="C170" t="s">
-        <v>458</v>
+        <v>486</v>
       </c>
       <c r="D170" t="s">
-        <v>488</v>
-      </c>
-      <c r="G170" s="5"/>
+        <v>491</v>
+      </c>
+      <c r="E170" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F170" t="s">
+        <v>472</v>
+      </c>
+      <c r="G170" s="5">
+        <v>92003</v>
+      </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="B171" t="s">
         <v>456</v>
       </c>
       <c r="C171" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="D171" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="G171" s="5"/>
+      <c r="H171" t="s">
+        <v>471</v>
+      </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="B172" t="s">
         <v>456</v>
       </c>
       <c r="C172" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D172" t="s">
         <v>488</v>
@@ -11165,13 +11394,13 @@
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="B173" t="s">
         <v>456</v>
       </c>
       <c r="C173" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="D173" t="s">
         <v>488</v>
@@ -11180,13 +11409,13 @@
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="B174" t="s">
         <v>456</v>
       </c>
       <c r="C174" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="D174" t="s">
         <v>488</v>
@@ -11195,13 +11424,13 @@
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="B175" t="s">
         <v>456</v>
       </c>
       <c r="C175" t="s">
-        <v>556</v>
+        <v>461</v>
       </c>
       <c r="D175" t="s">
         <v>488</v>
@@ -11210,13 +11439,13 @@
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="B176" t="s">
         <v>456</v>
       </c>
       <c r="C176" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="D176" t="s">
         <v>488</v>
@@ -11225,13 +11454,13 @@
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="B177" t="s">
         <v>456</v>
       </c>
       <c r="C177" t="s">
-        <v>463</v>
+        <v>556</v>
       </c>
       <c r="D177" t="s">
         <v>488</v>
@@ -11240,13 +11469,13 @@
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="B178" t="s">
         <v>456</v>
       </c>
       <c r="C178" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D178" t="s">
         <v>488</v>
@@ -11255,43 +11484,43 @@
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="B179" t="s">
         <v>456</v>
       </c>
       <c r="C179" t="s">
-        <v>561</v>
+        <v>463</v>
       </c>
       <c r="D179" t="s">
-        <v>570</v>
+        <v>488</v>
       </c>
       <c r="G179" s="5"/>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="B180" t="s">
         <v>456</v>
       </c>
       <c r="C180" t="s">
-        <v>564</v>
+        <v>464</v>
       </c>
       <c r="D180" t="s">
-        <v>570</v>
+        <v>488</v>
       </c>
       <c r="G180" s="5"/>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
       <c r="B181" t="s">
         <v>456</v>
       </c>
       <c r="C181" t="s">
-        <v>567</v>
+        <v>561</v>
       </c>
       <c r="D181" t="s">
         <v>570</v>
@@ -11300,13 +11529,13 @@
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="B182" t="s">
         <v>456</v>
       </c>
       <c r="C182" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="D182" t="s">
         <v>570</v>
@@ -11315,13 +11544,13 @@
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>562</v>
+        <v>565</v>
       </c>
       <c r="B183" t="s">
         <v>456</v>
       </c>
       <c r="C183" t="s">
-        <v>468</v>
+        <v>567</v>
       </c>
       <c r="D183" t="s">
         <v>570</v>
@@ -11330,21 +11559,18 @@
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="B184" t="s">
         <v>456</v>
       </c>
       <c r="C184" t="s">
-        <v>466</v>
+        <v>568</v>
       </c>
       <c r="D184" t="s">
         <v>570</v>
       </c>
       <c r="G184" s="5"/>
-      <c r="H184" t="s">
-        <v>467</v>
-      </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
@@ -11364,6 +11590,84 @@
       </c>
       <c r="G185" s="5" t="s">
         <v>582</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>591</v>
+      </c>
+      <c r="B186" t="s">
+        <v>456</v>
+      </c>
+      <c r="C186" t="s">
+        <v>243</v>
+      </c>
+      <c r="D186" t="s">
+        <v>488</v>
+      </c>
+      <c r="E186" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F186" t="s">
+        <v>244</v>
+      </c>
+      <c r="G186" s="5"/>
+    </row>
+    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>593</v>
+      </c>
+      <c r="B187" t="s">
+        <v>237</v>
+      </c>
+      <c r="C187" t="s">
+        <v>266</v>
+      </c>
+      <c r="D187" t="s">
+        <v>490</v>
+      </c>
+      <c r="E187" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F187" t="s">
+        <v>267</v>
+      </c>
+      <c r="G187" s="5"/>
+      <c r="H187" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>562</v>
+      </c>
+      <c r="B188" t="s">
+        <v>456</v>
+      </c>
+      <c r="C188" t="s">
+        <v>468</v>
+      </c>
+      <c r="D188" t="s">
+        <v>570</v>
+      </c>
+      <c r="G188" s="5"/>
+    </row>
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>569</v>
+      </c>
+      <c r="B189" t="s">
+        <v>456</v>
+      </c>
+      <c r="C189" t="s">
+        <v>466</v>
+      </c>
+      <c r="D189" t="s">
+        <v>570</v>
+      </c>
+      <c r="G189" s="5"/>
+      <c r="H189" t="s">
+        <v>467</v>
       </c>
     </row>
   </sheetData>
@@ -11420,29 +11724,29 @@
     <hyperlink ref="E65" r:id="rId50" xr:uid="{B5DAC180-9B3B-41CB-82EB-134E54507853}"/>
     <hyperlink ref="E66" r:id="rId51" xr:uid="{FCD67149-1EF3-40DA-BB29-03662DB0E615}"/>
     <hyperlink ref="E64" r:id="rId52" xr:uid="{85A32931-0A6D-4FED-BFFA-62A12F314D92}"/>
-    <hyperlink ref="E72" r:id="rId53" xr:uid="{B5C2A792-3025-4E08-BFB9-61ECF51B374D}"/>
-    <hyperlink ref="E73" r:id="rId54" xr:uid="{97CED2FD-9F84-464D-9342-72A124A363BC}"/>
-    <hyperlink ref="E75" r:id="rId55" xr:uid="{980BBB81-A1C1-4ACA-8663-5B0460438D1D}"/>
-    <hyperlink ref="E74" r:id="rId56" xr:uid="{02868430-C4CD-4A7F-88A2-39B6B75D371E}"/>
+    <hyperlink ref="E71" r:id="rId53" xr:uid="{B5C2A792-3025-4E08-BFB9-61ECF51B374D}"/>
+    <hyperlink ref="E72" r:id="rId54" xr:uid="{97CED2FD-9F84-464D-9342-72A124A363BC}"/>
+    <hyperlink ref="E74" r:id="rId55" xr:uid="{980BBB81-A1C1-4ACA-8663-5B0460438D1D}"/>
+    <hyperlink ref="E73" r:id="rId56" xr:uid="{02868430-C4CD-4A7F-88A2-39B6B75D371E}"/>
     <hyperlink ref="E67" r:id="rId57" xr:uid="{1E13D856-EEFD-4ABB-A5C0-5D1E0BF95A82}"/>
     <hyperlink ref="E68" r:id="rId58" xr:uid="{5FB21DD1-70AF-4D29-A5BB-7D9EB3DA55F6}"/>
-    <hyperlink ref="E70" r:id="rId59" xr:uid="{DDD755CF-63DF-476F-8368-DCF07DCD4609}"/>
-    <hyperlink ref="E71" r:id="rId60" xr:uid="{2FBCBAC4-D205-410D-8C00-8356A8ECB67E}"/>
-    <hyperlink ref="E76" r:id="rId61" xr:uid="{AA939156-F9E5-43B8-8761-6EE0951EA9FF}"/>
-    <hyperlink ref="E77" r:id="rId62" xr:uid="{B5798FB4-C1E2-456D-9711-87A309BD6878}"/>
-    <hyperlink ref="E108" r:id="rId63" xr:uid="{DE574022-7D55-4097-9D55-6421929BB4D6}"/>
-    <hyperlink ref="E109" r:id="rId64" xr:uid="{17BD79E0-0F48-49EC-8C65-CB173907FEB0}"/>
-    <hyperlink ref="E105" r:id="rId65" xr:uid="{ADD3565F-8131-4C8E-BEF2-FA6062A0F466}"/>
-    <hyperlink ref="E106" r:id="rId66" xr:uid="{31F424C2-D731-4E26-ACED-E2DE4D8451E9}"/>
-    <hyperlink ref="E107" r:id="rId67" xr:uid="{8C8DD198-5284-45E6-AC60-523B30266C35}"/>
-    <hyperlink ref="E110" r:id="rId68" xr:uid="{03FFC474-5820-4AA4-BF45-21ED811B5D6B}"/>
-    <hyperlink ref="E111" r:id="rId69" xr:uid="{1D5962C8-1986-4122-8F07-ED623C46A3C9}"/>
-    <hyperlink ref="E112" r:id="rId70" xr:uid="{F572B91D-DA7D-4AB2-978B-0BA81A3AB914}"/>
-    <hyperlink ref="E113" r:id="rId71" xr:uid="{2472D891-5A22-47C0-B741-7E0E5ADD05A1}"/>
-    <hyperlink ref="E115" r:id="rId72" xr:uid="{C21B974D-1E8B-4463-8243-F86F1DB608FC}"/>
-    <hyperlink ref="E114" r:id="rId73" xr:uid="{24BB6E77-83B4-4F7F-A249-3E020A224BE1}"/>
-    <hyperlink ref="E116" r:id="rId74" xr:uid="{1DF76622-6E9B-4B29-8601-44F2E3930EB0}"/>
-    <hyperlink ref="E117" r:id="rId75" xr:uid="{DEEFB1B1-E0E5-40BF-B4FF-15669DE884F9}"/>
+    <hyperlink ref="E69" r:id="rId59" xr:uid="{DDD755CF-63DF-476F-8368-DCF07DCD4609}"/>
+    <hyperlink ref="E70" r:id="rId60" xr:uid="{2FBCBAC4-D205-410D-8C00-8356A8ECB67E}"/>
+    <hyperlink ref="E75" r:id="rId61" xr:uid="{AA939156-F9E5-43B8-8761-6EE0951EA9FF}"/>
+    <hyperlink ref="E76" r:id="rId62" xr:uid="{B5798FB4-C1E2-456D-9711-87A309BD6878}"/>
+    <hyperlink ref="E107" r:id="rId63" xr:uid="{DE574022-7D55-4097-9D55-6421929BB4D6}"/>
+    <hyperlink ref="E108" r:id="rId64" xr:uid="{17BD79E0-0F48-49EC-8C65-CB173907FEB0}"/>
+    <hyperlink ref="E104" r:id="rId65" xr:uid="{ADD3565F-8131-4C8E-BEF2-FA6062A0F466}"/>
+    <hyperlink ref="E105" r:id="rId66" xr:uid="{31F424C2-D731-4E26-ACED-E2DE4D8451E9}"/>
+    <hyperlink ref="E186" r:id="rId67" xr:uid="{8C8DD198-5284-45E6-AC60-523B30266C35}"/>
+    <hyperlink ref="E109" r:id="rId68" xr:uid="{03FFC474-5820-4AA4-BF45-21ED811B5D6B}"/>
+    <hyperlink ref="E110" r:id="rId69" xr:uid="{1D5962C8-1986-4122-8F07-ED623C46A3C9}"/>
+    <hyperlink ref="E111" r:id="rId70" xr:uid="{F572B91D-DA7D-4AB2-978B-0BA81A3AB914}"/>
+    <hyperlink ref="E112" r:id="rId71" xr:uid="{2472D891-5A22-47C0-B741-7E0E5ADD05A1}"/>
+    <hyperlink ref="E187" r:id="rId72" xr:uid="{C21B974D-1E8B-4463-8243-F86F1DB608FC}"/>
+    <hyperlink ref="E113" r:id="rId73" xr:uid="{24BB6E77-83B4-4F7F-A249-3E020A224BE1}"/>
+    <hyperlink ref="E114" r:id="rId74" xr:uid="{1DF76622-6E9B-4B29-8601-44F2E3930EB0}"/>
+    <hyperlink ref="E115" r:id="rId75" xr:uid="{DEEFB1B1-E0E5-40BF-B4FF-15669DE884F9}"/>
     <hyperlink ref="E133" r:id="rId76" xr:uid="{EB10DAA1-2581-44AA-B02F-EF7834AE0264}"/>
     <hyperlink ref="E134" r:id="rId77" xr:uid="{D3E6AEA5-E392-4135-A858-F628EB7503A4}"/>
     <hyperlink ref="E135" r:id="rId78" xr:uid="{09D7B138-477C-45D9-85FE-90663A1056C9}"/>
@@ -11466,22 +11770,22 @@
     <hyperlink ref="E153" r:id="rId96" xr:uid="{4E72F6FF-E359-403E-8C10-899982A46106}"/>
     <hyperlink ref="E154" r:id="rId97" xr:uid="{DC29AC1A-C353-42E1-A92B-B169D3D58EA9}"/>
     <hyperlink ref="E156" r:id="rId98" xr:uid="{3C1A7911-DFEA-4653-9C41-4CCA8D4B0F7E}"/>
-    <hyperlink ref="E163" r:id="rId99" xr:uid="{2B9BE5C8-7021-4253-97F8-0AF75D476D51}"/>
-    <hyperlink ref="E162" r:id="rId100" xr:uid="{71B9EE24-F9E3-47B0-9DB1-DE809D668D49}"/>
-    <hyperlink ref="E164" r:id="rId101" xr:uid="{8B5F072C-581E-4B93-A107-047F4E567BD3}"/>
-    <hyperlink ref="E166" r:id="rId102" xr:uid="{CC0CACD1-E193-4320-BA06-AD19994EB98E}"/>
-    <hyperlink ref="E165" r:id="rId103" xr:uid="{E48C6228-D60E-464A-B72D-6345D0E3CC68}"/>
+    <hyperlink ref="E164" r:id="rId99" xr:uid="{2B9BE5C8-7021-4253-97F8-0AF75D476D51}"/>
+    <hyperlink ref="E163" r:id="rId100" xr:uid="{71B9EE24-F9E3-47B0-9DB1-DE809D668D49}"/>
+    <hyperlink ref="E165" r:id="rId101" xr:uid="{8B5F072C-581E-4B93-A107-047F4E567BD3}"/>
+    <hyperlink ref="E167" r:id="rId102" xr:uid="{CC0CACD1-E193-4320-BA06-AD19994EB98E}"/>
+    <hyperlink ref="E166" r:id="rId103" xr:uid="{E48C6228-D60E-464A-B72D-6345D0E3CC68}"/>
     <hyperlink ref="E157" r:id="rId104" xr:uid="{E5167E91-C797-4BC7-BB2F-6598B43FEF38}"/>
     <hyperlink ref="E127" r:id="rId105" xr:uid="{5D0C387C-6BF9-4CCF-8CDD-27709B01C265}"/>
     <hyperlink ref="E158" r:id="rId106" xr:uid="{7A2DC4C0-FF36-43BA-A189-3BD54D156058}"/>
     <hyperlink ref="E132" r:id="rId107" xr:uid="{116340D2-01CC-4E5D-8CFC-C2B1A68AE3F6}"/>
     <hyperlink ref="E130" r:id="rId108" xr:uid="{B4D0E8D6-7F8E-449B-8D1F-8D7EBCF17B93}"/>
     <hyperlink ref="E131" r:id="rId109" xr:uid="{04C0BD6E-A059-46D2-BDE2-26C5AC6A938D}"/>
-    <hyperlink ref="E159" r:id="rId110" xr:uid="{8342F021-8D39-4131-8F90-D524FB7AEA9D}"/>
+    <hyperlink ref="E160" r:id="rId110" xr:uid="{8342F021-8D39-4131-8F90-D524FB7AEA9D}"/>
     <hyperlink ref="E149" r:id="rId111" xr:uid="{86B132C5-CB3B-447C-926A-7EF611C31616}"/>
     <hyperlink ref="E143" r:id="rId112" xr:uid="{EA253D54-3F1D-4A03-A0D3-7F679CF9F47E}"/>
     <hyperlink ref="E145" r:id="rId113" xr:uid="{5BD6299F-0EC3-4F51-AC82-FF124DBC4020}"/>
-    <hyperlink ref="E167" r:id="rId114" xr:uid="{3B84E3E9-7F9C-4F1F-B4B3-A52D4EEFB917}"/>
+    <hyperlink ref="E168" r:id="rId114" xr:uid="{3B84E3E9-7F9C-4F1F-B4B3-A52D4EEFB917}"/>
     <hyperlink ref="E2" r:id="rId115" xr:uid="{11C9A353-3E3E-4A5B-A149-F9DCD5EAC942}"/>
     <hyperlink ref="E4" r:id="rId116" xr:uid="{FA0452B0-82F7-471E-90D4-A2F200486D8C}"/>
     <hyperlink ref="E3" r:id="rId117" xr:uid="{17585C18-58AC-4CE7-9578-2F63696D867B}"/>
@@ -11493,37 +11797,30 @@
     <hyperlink ref="E147" r:id="rId123" xr:uid="{899DE784-1FB2-4A3F-BA67-B60FD0ED9C31}"/>
     <hyperlink ref="E148" r:id="rId124" xr:uid="{416E9179-6A41-4C5A-955D-4A8B6488BC03}"/>
     <hyperlink ref="E144" r:id="rId125" xr:uid="{ED6FE160-7585-48D5-BE73-72E0F12618ED}"/>
-    <hyperlink ref="E161" r:id="rId126" xr:uid="{863E8587-1A74-4216-A533-FD4D1FD293D3}"/>
-    <hyperlink ref="E160" r:id="rId127" xr:uid="{860D846A-19A6-4ED3-A227-165BA48AAE60}"/>
-    <hyperlink ref="E168" r:id="rId128" xr:uid="{29CE548D-B2B4-4587-A753-C066B1AFBF82}"/>
+    <hyperlink ref="E162" r:id="rId126" xr:uid="{863E8587-1A74-4216-A533-FD4D1FD293D3}"/>
+    <hyperlink ref="E161" r:id="rId127" xr:uid="{860D846A-19A6-4ED3-A227-165BA48AAE60}"/>
+    <hyperlink ref="E170" r:id="rId128" xr:uid="{29CE548D-B2B4-4587-A753-C066B1AFBF82}"/>
     <hyperlink ref="E61" r:id="rId129" xr:uid="{7D63EDBD-9486-4D70-A8EB-EC35CE324B2B}"/>
-    <hyperlink ref="E118" r:id="rId130" xr:uid="{A98A24AB-1380-4DE0-A6F4-00B837BDCB8A}"/>
+    <hyperlink ref="E116" r:id="rId130" xr:uid="{A98A24AB-1380-4DE0-A6F4-00B837BDCB8A}"/>
     <hyperlink ref="H17" r:id="rId131" display="Bulk Link" xr:uid="{F82FB24D-F456-4AD0-A18C-EFB9462C2336}"/>
     <hyperlink ref="E15" r:id="rId132" xr:uid="{9B908FEE-C2B6-4B01-873F-1D31646DA108}"/>
     <hyperlink ref="E24" r:id="rId133" xr:uid="{648BFDEF-0776-40CB-96BD-3105232BF7C5}"/>
-    <hyperlink ref="E119" r:id="rId134" xr:uid="{E8DEB348-3B00-41C7-85D4-7BD6198F40E2}"/>
+    <hyperlink ref="E117" r:id="rId134" xr:uid="{E8DEB348-3B00-41C7-85D4-7BD6198F40E2}"/>
     <hyperlink ref="E26" r:id="rId135" xr:uid="{365853CB-05CC-49D9-935A-4155641501C2}"/>
     <hyperlink ref="E20" r:id="rId136" xr:uid="{1434FB4A-AD21-4365-A9D6-F5C278481092}"/>
-    <hyperlink ref="E102" r:id="rId137" xr:uid="{C14C2209-5B5B-49C3-803B-A85A1210574C}"/>
+    <hyperlink ref="E101" r:id="rId137" xr:uid="{C14C2209-5B5B-49C3-803B-A85A1210574C}"/>
     <hyperlink ref="E36" r:id="rId138" xr:uid="{3F170435-BC60-4CD0-85D5-AB822CAD5955}"/>
+    <hyperlink ref="E169" r:id="rId139" xr:uid="{792BF035-BBA1-4EB3-B614-DCA9990A42C4}"/>
+    <hyperlink ref="E118" r:id="rId140" xr:uid="{439405A6-C063-4FCA-B4EC-EC73BF273123}"/>
+    <hyperlink ref="E119" r:id="rId141" xr:uid="{32E6CB73-CB22-4831-BA9B-31BA5269C4ED}"/>
+    <hyperlink ref="E120" r:id="rId142" xr:uid="{BB2B7640-97E7-4C45-875F-001470775177}"/>
+    <hyperlink ref="E59" r:id="rId143" xr:uid="{75CE5656-EFCC-41EF-B490-7E580549526F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId139"/>
+  <pageSetup orientation="portrait" r:id="rId144"/>
   <tableParts count="1">
-    <tablePart r:id="rId140"/>
+    <tablePart r:id="rId145"/>
   </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE3AEE9E-D21D-4ECD-BA1D-6BDD55688F9A}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Restored camera stand; BOM work
## 2022-03-04

- Continuing model and BOM verification. Working on kinematic components today.
- Restored PN088, the camera base.
- Added a linear rail plug that can be printed in TPU in case they are lost (I need them right now; figured they can't hurt).
- Lot of corrections to fastener sizes.
</commit_message>
<xml_diff>
--- a/BOM/General Part List.xlsx
+++ b/BOM/General Part List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\Documents\3D Print\Clockmaker\clock-3\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{951FBBC7-BC86-4D54-8ABC-8E656E0010FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{599F8DC8-2B37-446D-8B99-9320B08A93D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25500" yWindow="3195" windowWidth="23250" windowHeight="12480" firstSheet="6" activeTab="8" xr2:uid="{6EB0A7B6-C6D7-4759-8B58-841D5EFF92F5}"/>
   </bookViews>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2593" uniqueCount="631">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2601" uniqueCount="635">
   <si>
     <t>ID</t>
   </si>
@@ -1971,6 +1971,18 @@
   </si>
   <si>
     <t>Thermistor, NTC 100K, E3D V6 cartridge</t>
+  </si>
+  <si>
+    <t>PN557</t>
+  </si>
+  <si>
+    <t>Screw, M4-0.7 x 8mm BHCS</t>
+  </si>
+  <si>
+    <t>PN536</t>
+  </si>
+  <si>
+    <t>Screw, M5-0.8 x 20mm BHCS</t>
   </si>
 </sst>
 </file>
@@ -2469,10 +2481,10 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BCCEB002-6247-475F-8E59-4D3290F5D0AB}" name="Table13" displayName="Table13" ref="A1:H192" totalsRowShown="0">
-  <autoFilter ref="A1:H192" xr:uid="{BCCEB002-6247-475F-8E59-4D3290F5D0AB}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H192">
-    <sortCondition ref="A1:A192"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BCCEB002-6247-475F-8E59-4D3290F5D0AB}" name="Table13" displayName="Table13" ref="A1:H194" totalsRowShown="0">
+  <autoFilter ref="A1:H194" xr:uid="{BCCEB002-6247-475F-8E59-4D3290F5D0AB}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H194">
+    <sortCondition ref="A1:A194"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{5013DA2C-AE55-4442-B536-8693A638A779}" name="ID"/>
@@ -7586,10 +7598,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D318B5EB-87D8-4D97-AE82-574AF33D7DA4}">
-  <dimension ref="A1:H192"/>
+  <dimension ref="A1:H194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="F163" sqref="F163"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8084,39 +8096,30 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>54</v>
+        <v>633</v>
       </c>
       <c r="B21" t="s">
         <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>55</v>
+        <v>634</v>
       </c>
       <c r="D21" t="s">
         <v>479</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21" t="s">
-        <v>56</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="H21" t="s">
-        <v>58</v>
-      </c>
+      <c r="E21" s="3"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B22" t="s">
         <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>626</v>
+        <v>55</v>
       </c>
       <c r="D22" t="s">
         <v>479</v>
@@ -8125,22 +8128,24 @@
         <v>10</v>
       </c>
       <c r="F22" t="s">
-        <v>61</v>
-      </c>
-      <c r="G22" s="5"/>
+        <v>56</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="H22" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B23" t="s">
         <v>8</v>
       </c>
       <c r="C23" t="s">
-        <v>516</v>
+        <v>626</v>
       </c>
       <c r="D23" t="s">
         <v>479</v>
@@ -8149,22 +8154,22 @@
         <v>10</v>
       </c>
       <c r="F23" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="G23" s="5"/>
       <c r="H23" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>417</v>
+        <v>63</v>
       </c>
       <c r="B24" t="s">
         <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="D24" t="s">
         <v>479</v>
@@ -8173,136 +8178,134 @@
         <v>10</v>
       </c>
       <c r="F24" t="s">
-        <v>11</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>509</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="G24" s="5"/>
       <c r="H24" t="s">
-        <v>508</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="B25" t="s">
         <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>422</v>
+        <v>515</v>
       </c>
       <c r="D25" t="s">
         <v>479</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>424</v>
+        <v>10</v>
       </c>
       <c r="F25" t="s">
-        <v>425</v>
-      </c>
-      <c r="G25" s="5"/>
+        <v>11</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>509</v>
+      </c>
       <c r="H25" t="s">
-        <v>423</v>
+        <v>508</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>513</v>
+        <v>421</v>
       </c>
       <c r="B26" t="s">
         <v>8</v>
       </c>
       <c r="C26" t="s">
-        <v>514</v>
+        <v>422</v>
       </c>
       <c r="D26" t="s">
         <v>479</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>10</v>
+        <v>424</v>
       </c>
       <c r="F26" t="s">
-        <v>67</v>
+        <v>425</v>
       </c>
       <c r="G26" s="5"/>
       <c r="H26" t="s">
-        <v>517</v>
+        <v>423</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>625</v>
+        <v>513</v>
       </c>
       <c r="B27" t="s">
         <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>626</v>
+        <v>514</v>
       </c>
       <c r="D27" t="s">
         <v>479</v>
       </c>
-      <c r="E27" s="1"/>
+      <c r="E27" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="F27" t="s">
         <v>67</v>
       </c>
       <c r="G27" s="5"/>
       <c r="H27" t="s">
-        <v>627</v>
+        <v>517</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>65</v>
+        <v>625</v>
       </c>
       <c r="B28" t="s">
         <v>8</v>
       </c>
       <c r="C28" t="s">
-        <v>66</v>
+        <v>626</v>
       </c>
       <c r="D28" t="s">
         <v>479</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="E28" s="1"/>
       <c r="F28" t="s">
         <v>67</v>
       </c>
       <c r="G28" s="5"/>
+      <c r="H28" t="s">
+        <v>627</v>
+      </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>68</v>
+        <v>631</v>
       </c>
       <c r="B29" t="s">
         <v>8</v>
       </c>
       <c r="C29" t="s">
-        <v>69</v>
+        <v>632</v>
       </c>
       <c r="D29" t="s">
         <v>479</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F29" t="s">
-        <v>67</v>
-      </c>
+      <c r="E29" s="1"/>
       <c r="G29" s="5"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B30" t="s">
         <v>8</v>
       </c>
       <c r="C30" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D30" t="s">
         <v>479</v>
@@ -8317,13 +8320,13 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B31" t="s">
         <v>8</v>
       </c>
       <c r="C31" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D31" t="s">
         <v>479</v>
@@ -8338,13 +8341,13 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B32" t="s">
         <v>8</v>
       </c>
       <c r="C32" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D32" t="s">
         <v>479</v>
@@ -8359,13 +8362,13 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B33" t="s">
         <v>8</v>
       </c>
       <c r="C33" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D33" t="s">
         <v>479</v>
@@ -8380,13 +8383,13 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B34" t="s">
         <v>8</v>
       </c>
       <c r="C34" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D34" t="s">
         <v>479</v>
@@ -8401,13 +8404,13 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B35" t="s">
         <v>8</v>
       </c>
       <c r="C35" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D35" t="s">
         <v>479</v>
@@ -8422,13 +8425,13 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B36" t="s">
         <v>8</v>
       </c>
       <c r="C36" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D36" t="s">
         <v>479</v>
@@ -8443,13 +8446,13 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>530</v>
+        <v>80</v>
       </c>
       <c r="B37" t="s">
         <v>8</v>
       </c>
       <c r="C37" t="s">
-        <v>595</v>
+        <v>81</v>
       </c>
       <c r="D37" t="s">
         <v>479</v>
@@ -8461,19 +8464,16 @@
         <v>67</v>
       </c>
       <c r="G37" s="5"/>
-      <c r="H37" t="s">
-        <v>531</v>
-      </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B38" t="s">
         <v>8</v>
       </c>
       <c r="C38" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D38" t="s">
         <v>479</v>
@@ -8485,19 +8485,16 @@
         <v>67</v>
       </c>
       <c r="G38" s="5"/>
-      <c r="H38" t="s">
-        <v>86</v>
-      </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>87</v>
+        <v>530</v>
       </c>
       <c r="B39" t="s">
         <v>8</v>
       </c>
       <c r="C39" t="s">
-        <v>88</v>
+        <v>595</v>
       </c>
       <c r="D39" t="s">
         <v>479</v>
@@ -8506,22 +8503,22 @@
         <v>10</v>
       </c>
       <c r="F39" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="G39" s="5"/>
       <c r="H39" t="s">
-        <v>89</v>
+        <v>531</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B40" t="s">
         <v>8</v>
       </c>
       <c r="C40" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D40" t="s">
         <v>479</v>
@@ -8530,19 +8527,22 @@
         <v>10</v>
       </c>
       <c r="F40" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="G40" s="5"/>
+      <c r="H40" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B41" t="s">
         <v>8</v>
       </c>
       <c r="C41" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D41" t="s">
         <v>479</v>
@@ -8551,19 +8551,22 @@
         <v>10</v>
       </c>
       <c r="F41" t="s">
-        <v>94</v>
+        <v>56</v>
       </c>
       <c r="G41" s="5"/>
+      <c r="H41" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B42" t="s">
         <v>8</v>
       </c>
       <c r="C42" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D42" t="s">
         <v>479</v>
@@ -8572,19 +8575,19 @@
         <v>10</v>
       </c>
       <c r="F42" t="s">
-        <v>97</v>
+        <v>56</v>
       </c>
       <c r="G42" s="5"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B43" t="s">
-        <v>99</v>
+        <v>8</v>
       </c>
       <c r="C43" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="D43" t="s">
         <v>479</v>
@@ -8593,21 +8596,19 @@
         <v>10</v>
       </c>
       <c r="F43" t="s">
-        <v>101</v>
-      </c>
-      <c r="G43" s="5" t="s">
-        <v>102</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="G43" s="5"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B44" t="s">
-        <v>99</v>
+        <v>8</v>
       </c>
       <c r="C44" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D44" t="s">
         <v>479</v>
@@ -8616,21 +8617,19 @@
         <v>10</v>
       </c>
       <c r="F44" t="s">
-        <v>101</v>
-      </c>
-      <c r="G44" s="5" t="s">
-        <v>105</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="G44" s="5"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B45" t="s">
         <v>99</v>
       </c>
       <c r="C45" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D45" t="s">
         <v>479</v>
@@ -8642,18 +8641,18 @@
         <v>101</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B46" t="s">
         <v>99</v>
       </c>
       <c r="C46" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D46" t="s">
         <v>479</v>
@@ -8662,21 +8661,21 @@
         <v>10</v>
       </c>
       <c r="F46" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B47" t="s">
         <v>99</v>
       </c>
       <c r="C47" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="D47" t="s">
         <v>479</v>
@@ -8685,45 +8684,44 @@
         <v>10</v>
       </c>
       <c r="F47" t="s">
-        <v>67</v>
-      </c>
-      <c r="G47" s="5"/>
+        <v>101</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B48" t="s">
         <v>99</v>
       </c>
       <c r="C48" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D48" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F48" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="H48" t="s">
-        <v>476</v>
+        <v>112</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B49" t="s">
         <v>99</v>
       </c>
       <c r="C49" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D49" t="s">
         <v>479</v>
@@ -8732,44 +8730,45 @@
         <v>10</v>
       </c>
       <c r="F49" t="s">
-        <v>101</v>
-      </c>
-      <c r="G49" s="5" t="s">
-        <v>121</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="G49" s="5"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B50" t="s">
         <v>99</v>
       </c>
       <c r="C50" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="D50" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F50" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>125</v>
+        <v>118</v>
+      </c>
+      <c r="H50" t="s">
+        <v>476</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B51" t="s">
         <v>99</v>
       </c>
       <c r="C51" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="D51" t="s">
         <v>479</v>
@@ -8778,21 +8777,21 @@
         <v>10</v>
       </c>
       <c r="F51" t="s">
-        <v>128</v>
+        <v>101</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="B52" t="s">
         <v>99</v>
       </c>
       <c r="C52" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="D52" t="s">
         <v>479</v>
@@ -8801,21 +8800,21 @@
         <v>10</v>
       </c>
       <c r="F52" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B53" t="s">
         <v>99</v>
       </c>
       <c r="C53" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D53" t="s">
         <v>479</v>
@@ -8824,21 +8823,21 @@
         <v>10</v>
       </c>
       <c r="F53" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B54" t="s">
         <v>99</v>
       </c>
       <c r="C54" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D54" t="s">
         <v>479</v>
@@ -8847,44 +8846,44 @@
         <v>10</v>
       </c>
       <c r="F54" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B55" t="s">
-        <v>139</v>
+        <v>99</v>
       </c>
       <c r="C55" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="D55" t="s">
         <v>479</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>141</v>
+        <v>10</v>
       </c>
       <c r="F55" t="s">
-        <v>37</v>
+        <v>124</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="B56" t="s">
-        <v>139</v>
+        <v>99</v>
       </c>
       <c r="C56" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="D56" t="s">
         <v>479</v>
@@ -8893,19 +8892,21 @@
         <v>10</v>
       </c>
       <c r="F56" t="s">
-        <v>61</v>
-      </c>
-      <c r="G56" s="5"/>
+        <v>124</v>
+      </c>
+      <c r="G56" s="5" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B57" t="s">
         <v>139</v>
       </c>
       <c r="C57" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D57" t="s">
         <v>479</v>
@@ -8917,41 +8918,39 @@
         <v>37</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B58" t="s">
         <v>139</v>
       </c>
       <c r="C58" t="s">
-        <v>618</v>
+        <v>144</v>
       </c>
       <c r="D58" t="s">
         <v>479</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>141</v>
+        <v>10</v>
       </c>
       <c r="F58" t="s">
-        <v>37</v>
-      </c>
-      <c r="G58" s="5" t="s">
-        <v>150</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="G58" s="5"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B59" t="s">
         <v>139</v>
       </c>
       <c r="C59" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="D59" t="s">
         <v>479</v>
@@ -8963,18 +8962,18 @@
         <v>37</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="B60" t="s">
         <v>139</v>
       </c>
       <c r="C60" t="s">
-        <v>416</v>
+        <v>618</v>
       </c>
       <c r="D60" t="s">
         <v>479</v>
@@ -8986,21 +8985,18 @@
         <v>37</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="H60" t="s">
-        <v>475</v>
+        <v>150</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>414</v>
+        <v>151</v>
       </c>
       <c r="B61" t="s">
         <v>139</v>
       </c>
       <c r="C61" t="s">
-        <v>415</v>
+        <v>152</v>
       </c>
       <c r="D61" t="s">
         <v>479</v>
@@ -9012,40 +9008,44 @@
         <v>37</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="H61" t="s">
-        <v>475</v>
+        <v>153</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>418</v>
+        <v>156</v>
       </c>
       <c r="B62" t="s">
         <v>139</v>
       </c>
       <c r="C62" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="D62" t="s">
         <v>479</v>
       </c>
-      <c r="E62" s="1"/>
-      <c r="G62" s="5"/>
+      <c r="E62" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F62" t="s">
+        <v>37</v>
+      </c>
+      <c r="G62" s="5" t="s">
+        <v>157</v>
+      </c>
       <c r="H62" t="s">
-        <v>420</v>
+        <v>475</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>158</v>
+        <v>414</v>
       </c>
       <c r="B63" t="s">
         <v>139</v>
       </c>
       <c r="C63" t="s">
-        <v>159</v>
+        <v>415</v>
       </c>
       <c r="D63" t="s">
         <v>479</v>
@@ -9057,47 +9057,40 @@
         <v>37</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="H63" t="s">
-        <v>161</v>
+        <v>475</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>162</v>
+        <v>418</v>
       </c>
       <c r="B64" t="s">
         <v>139</v>
       </c>
       <c r="C64" t="s">
-        <v>163</v>
+        <v>419</v>
       </c>
       <c r="D64" t="s">
         <v>479</v>
       </c>
-      <c r="E64" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="F64" t="s">
-        <v>37</v>
-      </c>
-      <c r="G64" s="5" t="s">
-        <v>164</v>
-      </c>
+      <c r="E64" s="1"/>
+      <c r="G64" s="5"/>
       <c r="H64" t="s">
-        <v>165</v>
+        <v>420</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B65" t="s">
         <v>139</v>
       </c>
       <c r="C65" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="D65" t="s">
         <v>479</v>
@@ -9109,21 +9102,21 @@
         <v>37</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="H65" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="B66" t="s">
         <v>139</v>
       </c>
       <c r="C66" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="D66" t="s">
         <v>479</v>
@@ -9135,21 +9128,21 @@
         <v>37</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="H66" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="B67" t="s">
         <v>139</v>
       </c>
       <c r="C67" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="D67" t="s">
         <v>479</v>
@@ -9161,21 +9154,21 @@
         <v>37</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="H67" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="B68" t="s">
         <v>139</v>
       </c>
       <c r="C68" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="D68" t="s">
         <v>479</v>
@@ -9187,21 +9180,21 @@
         <v>37</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="H68" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="B69" t="s">
         <v>139</v>
       </c>
       <c r="C69" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="D69" t="s">
         <v>479</v>
@@ -9213,21 +9206,21 @@
         <v>37</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="H69" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="B70" t="s">
         <v>139</v>
       </c>
       <c r="C70" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D70" t="s">
         <v>479</v>
@@ -9239,21 +9232,21 @@
         <v>37</v>
       </c>
       <c r="G70" s="5" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="H70" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="B71" t="s">
         <v>139</v>
       </c>
       <c r="C71" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="D71" t="s">
         <v>479</v>
@@ -9265,21 +9258,21 @@
         <v>37</v>
       </c>
       <c r="G71" s="5" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="H71" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B72" t="s">
         <v>139</v>
       </c>
       <c r="C72" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="D72" t="s">
         <v>479</v>
@@ -9291,21 +9284,21 @@
         <v>37</v>
       </c>
       <c r="G72" s="5" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="H72" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="B73" t="s">
         <v>139</v>
       </c>
       <c r="C73" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="D73" t="s">
         <v>479</v>
@@ -9317,21 +9310,21 @@
         <v>37</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="H73" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="B74" t="s">
         <v>139</v>
       </c>
       <c r="C74" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="D74" t="s">
         <v>479</v>
@@ -9343,21 +9336,21 @@
         <v>37</v>
       </c>
       <c r="G74" s="5" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="H74" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="B75" t="s">
         <v>139</v>
       </c>
       <c r="C75" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="D75" t="s">
         <v>479</v>
@@ -9369,21 +9362,21 @@
         <v>37</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="H75" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="B76" t="s">
         <v>139</v>
       </c>
       <c r="C76" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="D76" t="s">
         <v>479</v>
@@ -9395,69 +9388,73 @@
         <v>37</v>
       </c>
       <c r="G76" s="5" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="H76" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="B77" t="s">
         <v>139</v>
       </c>
       <c r="C77" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="D77" t="s">
         <v>479</v>
       </c>
-      <c r="E77" t="s">
-        <v>215</v>
+      <c r="E77" s="1" t="s">
+        <v>141</v>
       </c>
       <c r="F77" t="s">
-        <v>215</v>
-      </c>
-      <c r="G77" s="5"/>
+        <v>37</v>
+      </c>
+      <c r="G77" s="5" t="s">
+        <v>207</v>
+      </c>
       <c r="H77" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="B78" t="s">
         <v>139</v>
       </c>
       <c r="C78" t="s">
-        <v>619</v>
+        <v>210</v>
       </c>
       <c r="D78" t="s">
         <v>479</v>
       </c>
-      <c r="E78" t="s">
-        <v>215</v>
+      <c r="E78" s="1" t="s">
+        <v>141</v>
       </c>
       <c r="F78" t="s">
-        <v>215</v>
-      </c>
-      <c r="G78" s="5"/>
+        <v>37</v>
+      </c>
+      <c r="G78" s="5" t="s">
+        <v>211</v>
+      </c>
       <c r="H78" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>620</v>
+        <v>213</v>
       </c>
       <c r="B79" t="s">
         <v>139</v>
       </c>
       <c r="C79" t="s">
-        <v>610</v>
+        <v>214</v>
       </c>
       <c r="D79" t="s">
         <v>479</v>
@@ -9469,16 +9466,19 @@
         <v>215</v>
       </c>
       <c r="G79" s="5"/>
+      <c r="H79" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B80" t="s">
         <v>139</v>
       </c>
       <c r="C80" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="D80" t="s">
         <v>479</v>
@@ -9490,16 +9490,19 @@
         <v>215</v>
       </c>
       <c r="G80" s="5"/>
+      <c r="H80" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>222</v>
+        <v>620</v>
       </c>
       <c r="B81" t="s">
         <v>139</v>
       </c>
       <c r="C81" t="s">
-        <v>622</v>
+        <v>610</v>
       </c>
       <c r="D81" t="s">
         <v>479</v>
@@ -9514,13 +9517,13 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B82" t="s">
         <v>139</v>
       </c>
       <c r="C82" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="D82" t="s">
         <v>479</v>
@@ -9535,13 +9538,13 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B83" t="s">
         <v>139</v>
       </c>
       <c r="C83" t="s">
-        <v>605</v>
+        <v>622</v>
       </c>
       <c r="D83" t="s">
         <v>479</v>
@@ -9556,13 +9559,13 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B84" t="s">
         <v>139</v>
       </c>
       <c r="C84" t="s">
-        <v>606</v>
+        <v>623</v>
       </c>
       <c r="D84" t="s">
         <v>479</v>
@@ -9577,13 +9580,13 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B85" t="s">
         <v>139</v>
       </c>
       <c r="C85" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="D85" t="s">
         <v>479</v>
@@ -9598,13 +9601,13 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B86" t="s">
         <v>139</v>
       </c>
       <c r="C86" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="D86" t="s">
         <v>479</v>
@@ -9619,13 +9622,13 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B87" t="s">
         <v>139</v>
       </c>
       <c r="C87" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="D87" t="s">
         <v>479</v>
@@ -9640,13 +9643,13 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>467</v>
+        <v>229</v>
       </c>
       <c r="B88" t="s">
         <v>139</v>
       </c>
       <c r="C88" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
       <c r="D88" t="s">
         <v>479</v>
@@ -9661,13 +9664,13 @@
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>469</v>
+        <v>230</v>
       </c>
       <c r="B89" t="s">
         <v>139</v>
       </c>
       <c r="C89" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="D89" t="s">
         <v>479</v>
@@ -9682,13 +9685,13 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="B90" t="s">
         <v>139</v>
       </c>
       <c r="C90" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c r="D90" t="s">
         <v>479</v>
@@ -9703,13 +9706,13 @@
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="B91" t="s">
         <v>139</v>
       </c>
       <c r="C91" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
       <c r="D91" t="s">
         <v>479</v>
@@ -9724,13 +9727,13 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>518</v>
+        <v>470</v>
       </c>
       <c r="B92" t="s">
         <v>139</v>
       </c>
       <c r="C92" t="s">
-        <v>624</v>
+        <v>612</v>
       </c>
       <c r="D92" t="s">
         <v>479</v>
@@ -9742,55 +9745,61 @@
         <v>215</v>
       </c>
       <c r="G92" s="5"/>
-      <c r="H92" t="s">
-        <v>519</v>
-      </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>490</v>
+        <v>473</v>
       </c>
       <c r="B93" t="s">
         <v>139</v>
       </c>
       <c r="C93" t="s">
-        <v>571</v>
+        <v>611</v>
       </c>
       <c r="D93" t="s">
         <v>479</v>
       </c>
+      <c r="E93" t="s">
+        <v>215</v>
+      </c>
+      <c r="F93" t="s">
+        <v>215</v>
+      </c>
       <c r="G93" s="5"/>
-      <c r="H93" t="s">
-        <v>497</v>
-      </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>491</v>
+        <v>518</v>
       </c>
       <c r="B94" t="s">
         <v>139</v>
       </c>
       <c r="C94" t="s">
-        <v>603</v>
+        <v>624</v>
       </c>
       <c r="D94" t="s">
         <v>479</v>
+      </c>
+      <c r="E94" t="s">
+        <v>215</v>
+      </c>
+      <c r="F94" t="s">
+        <v>215</v>
       </c>
       <c r="G94" s="5"/>
       <c r="H94" t="s">
-        <v>497</v>
+        <v>519</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B95" t="s">
         <v>139</v>
       </c>
       <c r="C95" t="s">
-        <v>604</v>
+        <v>571</v>
       </c>
       <c r="D95" t="s">
         <v>479</v>
@@ -9802,49 +9811,49 @@
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="B96" t="s">
         <v>139</v>
       </c>
       <c r="C96" t="s">
-        <v>493</v>
+        <v>603</v>
       </c>
       <c r="D96" t="s">
         <v>479</v>
       </c>
       <c r="G96" s="5"/>
       <c r="H96" t="s">
-        <v>504</v>
+        <v>497</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="B97" t="s">
         <v>139</v>
       </c>
       <c r="C97" t="s">
-        <v>496</v>
+        <v>604</v>
       </c>
       <c r="D97" t="s">
         <v>479</v>
       </c>
       <c r="G97" s="5"/>
       <c r="H97" t="s">
-        <v>504</v>
+        <v>497</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="B98" t="s">
         <v>139</v>
       </c>
       <c r="C98" t="s">
-        <v>502</v>
+        <v>493</v>
       </c>
       <c r="D98" t="s">
         <v>479</v>
@@ -9856,31 +9865,31 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="B99" t="s">
         <v>139</v>
       </c>
       <c r="C99" t="s">
-        <v>503</v>
+        <v>496</v>
       </c>
       <c r="D99" t="s">
         <v>479</v>
       </c>
       <c r="G99" s="5"/>
       <c r="H99" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B100" t="s">
         <v>139</v>
       </c>
       <c r="C100" t="s">
-        <v>572</v>
+        <v>502</v>
       </c>
       <c r="D100" t="s">
         <v>479</v>
@@ -9892,154 +9901,145 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B101" t="s">
         <v>139</v>
       </c>
       <c r="C101" t="s">
-        <v>573</v>
+        <v>503</v>
       </c>
       <c r="D101" t="s">
         <v>479</v>
       </c>
       <c r="G101" s="5"/>
       <c r="H101" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>521</v>
+        <v>500</v>
       </c>
       <c r="B102" t="s">
         <v>139</v>
       </c>
       <c r="C102" t="s">
-        <v>602</v>
+        <v>572</v>
       </c>
       <c r="D102" t="s">
         <v>479</v>
       </c>
       <c r="G102" s="5"/>
       <c r="H102" t="s">
-        <v>524</v>
+        <v>504</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>560</v>
+        <v>501</v>
       </c>
       <c r="B103" t="s">
         <v>139</v>
       </c>
       <c r="C103" t="s">
-        <v>615</v>
+        <v>573</v>
       </c>
       <c r="D103" t="s">
         <v>479</v>
       </c>
-      <c r="E103" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="F103" s="6" t="s">
-        <v>215</v>
-      </c>
       <c r="G103" s="5"/>
+      <c r="H103" t="s">
+        <v>504</v>
+      </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>561</v>
+        <v>521</v>
       </c>
       <c r="B104" t="s">
         <v>139</v>
       </c>
       <c r="C104" t="s">
-        <v>616</v>
+        <v>602</v>
       </c>
       <c r="D104" t="s">
         <v>479</v>
       </c>
-      <c r="E104" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="F104" s="6" t="s">
-        <v>215</v>
-      </c>
       <c r="G104" s="5"/>
+      <c r="H104" t="s">
+        <v>524</v>
+      </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>596</v>
+        <v>560</v>
       </c>
       <c r="B105" t="s">
         <v>139</v>
       </c>
       <c r="C105" t="s">
-        <v>617</v>
-      </c>
-      <c r="E105" s="1" t="s">
-        <v>424</v>
+        <v>615</v>
+      </c>
+      <c r="D105" t="s">
+        <v>479</v>
+      </c>
+      <c r="E105" s="6" t="s">
+        <v>215</v>
       </c>
       <c r="F105" s="6" t="s">
-        <v>67</v>
+        <v>215</v>
       </c>
       <c r="G105" s="5"/>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>231</v>
+        <v>561</v>
       </c>
       <c r="B106" t="s">
-        <v>232</v>
+        <v>139</v>
       </c>
       <c r="C106" t="s">
-        <v>233</v>
+        <v>616</v>
       </c>
       <c r="D106" t="s">
         <v>479</v>
       </c>
-      <c r="E106" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F106" t="s">
-        <v>234</v>
+      <c r="E106" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="F106" s="6" t="s">
+        <v>215</v>
       </c>
       <c r="G106" s="5"/>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>235</v>
+        <v>596</v>
       </c>
       <c r="B107" t="s">
-        <v>232</v>
+        <v>139</v>
       </c>
       <c r="C107" t="s">
-        <v>236</v>
-      </c>
-      <c r="D107" t="s">
-        <v>479</v>
+        <v>617</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F107" t="s">
-        <v>234</v>
+        <v>424</v>
+      </c>
+      <c r="F107" s="6" t="s">
+        <v>67</v>
       </c>
       <c r="G107" s="5"/>
-      <c r="H107" t="s">
-        <v>574</v>
-      </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="B108" t="s">
         <v>232</v>
       </c>
       <c r="C108" t="s">
-        <v>579</v>
+        <v>233</v>
       </c>
       <c r="D108" t="s">
         <v>479</v>
@@ -10048,22 +10048,19 @@
         <v>10</v>
       </c>
       <c r="F108" t="s">
-        <v>67</v>
+        <v>234</v>
       </c>
       <c r="G108" s="5"/>
-      <c r="H108" t="s">
-        <v>580</v>
-      </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="B109" t="s">
         <v>232</v>
       </c>
       <c r="C109" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="D109" t="s">
         <v>479</v>
@@ -10072,24 +10069,22 @@
         <v>10</v>
       </c>
       <c r="F109" t="s">
-        <v>56</v>
-      </c>
-      <c r="G109" s="5" t="s">
-        <v>57</v>
-      </c>
+        <v>234</v>
+      </c>
+      <c r="G109" s="5"/>
       <c r="H109" t="s">
-        <v>244</v>
+        <v>574</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="B110" t="s">
         <v>232</v>
       </c>
       <c r="C110" t="s">
-        <v>243</v>
+        <v>579</v>
       </c>
       <c r="D110" t="s">
         <v>479</v>
@@ -10098,24 +10093,22 @@
         <v>10</v>
       </c>
       <c r="F110" t="s">
-        <v>56</v>
-      </c>
-      <c r="G110" s="5" t="s">
-        <v>57</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="G110" s="5"/>
       <c r="H110" t="s">
-        <v>244</v>
+        <v>580</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="B111" t="s">
         <v>232</v>
       </c>
       <c r="C111" t="s">
-        <v>576</v>
+        <v>241</v>
       </c>
       <c r="D111" t="s">
         <v>479</v>
@@ -10124,50 +10117,50 @@
         <v>10</v>
       </c>
       <c r="F111" t="s">
-        <v>246</v>
+        <v>56</v>
       </c>
       <c r="G111" s="5" t="s">
-        <v>247</v>
+        <v>57</v>
       </c>
       <c r="H111" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="B112" t="s">
         <v>232</v>
       </c>
       <c r="C112" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="D112" t="s">
         <v>479</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>251</v>
+        <v>10</v>
       </c>
       <c r="F112" t="s">
-        <v>251</v>
-      </c>
-      <c r="G112" s="5">
-        <v>570</v>
+        <v>56</v>
+      </c>
+      <c r="G112" s="5" t="s">
+        <v>57</v>
       </c>
       <c r="H112" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="B113" t="s">
         <v>232</v>
       </c>
       <c r="C113" t="s">
-        <v>520</v>
+        <v>576</v>
       </c>
       <c r="D113" t="s">
         <v>479</v>
@@ -10176,45 +10169,50 @@
         <v>10</v>
       </c>
       <c r="F113" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="G113" s="5" t="s">
-        <v>255</v>
+        <v>247</v>
+      </c>
+      <c r="H113" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="B114" t="s">
         <v>232</v>
       </c>
       <c r="C114" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="D114" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>10</v>
+        <v>251</v>
       </c>
       <c r="F114" t="s">
-        <v>67</v>
-      </c>
-      <c r="G114" s="5"/>
+        <v>251</v>
+      </c>
+      <c r="G114" s="5">
+        <v>570</v>
+      </c>
       <c r="H114" t="s">
-        <v>488</v>
+        <v>252</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="B115" t="s">
         <v>232</v>
       </c>
       <c r="C115" t="s">
-        <v>259</v>
+        <v>520</v>
       </c>
       <c r="D115" t="s">
         <v>479</v>
@@ -10223,19 +10221,21 @@
         <v>10</v>
       </c>
       <c r="F115" t="s">
-        <v>67</v>
-      </c>
-      <c r="G115" s="5"/>
+        <v>254</v>
+      </c>
+      <c r="G115" s="5" t="s">
+        <v>255</v>
+      </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="B116" t="s">
         <v>232</v>
       </c>
       <c r="C116" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="D116" t="s">
         <v>480</v>
@@ -10248,18 +10248,18 @@
       </c>
       <c r="G116" s="5"/>
       <c r="H116" t="s">
-        <v>264</v>
+        <v>488</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="B117" t="s">
         <v>232</v>
       </c>
       <c r="C117" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="D117" t="s">
         <v>479</v>
@@ -10271,22 +10271,19 @@
         <v>67</v>
       </c>
       <c r="G117" s="5"/>
-      <c r="H117" t="s">
-        <v>267</v>
-      </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="B118" t="s">
         <v>232</v>
       </c>
       <c r="C118" t="s">
-        <v>589</v>
+        <v>263</v>
       </c>
       <c r="D118" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="E118" s="1" t="s">
         <v>10</v>
@@ -10295,16 +10292,19 @@
         <v>67</v>
       </c>
       <c r="G118" s="5"/>
+      <c r="H118" t="s">
+        <v>264</v>
+      </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>511</v>
+        <v>265</v>
       </c>
       <c r="B119" t="s">
         <v>232</v>
       </c>
       <c r="C119" t="s">
-        <v>510</v>
+        <v>266</v>
       </c>
       <c r="D119" t="s">
         <v>479</v>
@@ -10317,18 +10317,18 @@
       </c>
       <c r="G119" s="5"/>
       <c r="H119" t="s">
-        <v>512</v>
+        <v>267</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>526</v>
+        <v>268</v>
       </c>
       <c r="B120" t="s">
         <v>232</v>
       </c>
       <c r="C120" t="s">
-        <v>527</v>
+        <v>589</v>
       </c>
       <c r="D120" t="s">
         <v>479</v>
@@ -10340,19 +10340,16 @@
         <v>67</v>
       </c>
       <c r="G120" s="5"/>
-      <c r="H120" t="s">
-        <v>528</v>
-      </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>581</v>
+        <v>511</v>
       </c>
       <c r="B121" t="s">
         <v>232</v>
       </c>
       <c r="C121" t="s">
-        <v>584</v>
+        <v>510</v>
       </c>
       <c r="D121" t="s">
         <v>479</v>
@@ -10361,24 +10358,25 @@
         <v>10</v>
       </c>
       <c r="F121" t="s">
-        <v>592</v>
-      </c>
-      <c r="G121" s="5" t="s">
-        <v>593</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="G121" s="5"/>
       <c r="H121" t="s">
-        <v>585</v>
+        <v>512</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>582</v>
+        <v>526</v>
       </c>
       <c r="B122" t="s">
         <v>232</v>
       </c>
       <c r="C122" t="s">
-        <v>583</v>
+        <v>527</v>
+      </c>
+      <c r="D122" t="s">
+        <v>479</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>10</v>
@@ -10388,70 +10386,65 @@
       </c>
       <c r="G122" s="5"/>
       <c r="H122" t="s">
-        <v>594</v>
+        <v>528</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>269</v>
+        <v>581</v>
       </c>
       <c r="B123" t="s">
-        <v>270</v>
+        <v>232</v>
       </c>
       <c r="C123" t="s">
-        <v>271</v>
+        <v>584</v>
       </c>
       <c r="D123" t="s">
         <v>479</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>272</v>
+        <v>10</v>
       </c>
       <c r="F123" t="s">
-        <v>273</v>
+        <v>592</v>
       </c>
       <c r="G123" s="5" t="s">
-        <v>274</v>
+        <v>593</v>
       </c>
       <c r="H123" t="s">
-        <v>275</v>
+        <v>585</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>276</v>
+        <v>582</v>
       </c>
       <c r="B124" t="s">
-        <v>270</v>
+        <v>232</v>
       </c>
       <c r="C124" t="s">
-        <v>277</v>
-      </c>
-      <c r="D124" t="s">
-        <v>479</v>
+        <v>583</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>272</v>
+        <v>10</v>
       </c>
       <c r="F124" t="s">
-        <v>273</v>
-      </c>
-      <c r="G124" s="5" t="s">
-        <v>278</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="G124" s="5"/>
       <c r="H124" t="s">
-        <v>279</v>
+        <v>594</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="B125" t="s">
         <v>270</v>
       </c>
       <c r="C125" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="D125" t="s">
         <v>479</v>
@@ -10463,93 +10456,96 @@
         <v>273</v>
       </c>
       <c r="G125" s="5" t="s">
-        <v>282</v>
+        <v>274</v>
+      </c>
+      <c r="H125" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="B126" t="s">
         <v>270</v>
       </c>
       <c r="C126" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="D126" t="s">
         <v>479</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>10</v>
+        <v>272</v>
       </c>
       <c r="F126" t="s">
-        <v>246</v>
+        <v>273</v>
       </c>
       <c r="G126" s="5" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="H126" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="B127" t="s">
         <v>270</v>
       </c>
       <c r="C127" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="D127" t="s">
         <v>479</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="F127" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="G127" s="10" t="s">
-        <v>291</v>
-      </c>
-      <c r="H127" t="s">
-        <v>292</v>
+        <v>272</v>
+      </c>
+      <c r="F127" t="s">
+        <v>273</v>
+      </c>
+      <c r="G127" s="5" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="B128" t="s">
         <v>270</v>
       </c>
       <c r="C128" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="D128" t="s">
         <v>479</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>289</v>
+        <v>10</v>
       </c>
       <c r="F128" t="s">
-        <v>295</v>
+        <v>246</v>
       </c>
       <c r="G128" s="5" t="s">
-        <v>296</v>
+        <v>285</v>
+      </c>
+      <c r="H128" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="B129" t="s">
         <v>270</v>
       </c>
       <c r="C129" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="D129" t="s">
         <v>479</v>
@@ -10557,70 +10553,71 @@
       <c r="E129" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="F129" t="s">
-        <v>299</v>
-      </c>
-      <c r="G129" s="5" t="s">
-        <v>300</v>
+      <c r="F129" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="G129" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="H129" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="B130" t="s">
         <v>270</v>
       </c>
       <c r="C130" t="s">
-        <v>427</v>
+        <v>294</v>
       </c>
       <c r="D130" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>10</v>
+        <v>289</v>
       </c>
       <c r="F130" t="s">
-        <v>67</v>
-      </c>
-      <c r="G130" s="5"/>
-      <c r="H130" t="s">
-        <v>429</v>
+        <v>295</v>
+      </c>
+      <c r="G130" s="5" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="B131" t="s">
         <v>270</v>
       </c>
       <c r="C131" t="s">
-        <v>426</v>
+        <v>298</v>
       </c>
       <c r="D131" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>10</v>
+        <v>289</v>
       </c>
       <c r="F131" t="s">
-        <v>67</v>
-      </c>
-      <c r="G131" s="5"/>
-      <c r="H131" t="s">
-        <v>428</v>
+        <v>299</v>
+      </c>
+      <c r="G131" s="5" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B132" t="s">
         <v>270</v>
       </c>
       <c r="C132" t="s">
-        <v>306</v>
+        <v>427</v>
       </c>
       <c r="D132" t="s">
         <v>480</v>
@@ -10633,18 +10630,18 @@
       </c>
       <c r="G132" s="5"/>
       <c r="H132" t="s">
-        <v>487</v>
+        <v>429</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="B133" t="s">
         <v>270</v>
       </c>
       <c r="C133" t="s">
-        <v>308</v>
+        <v>426</v>
       </c>
       <c r="D133" t="s">
         <v>480</v>
@@ -10656,19 +10653,19 @@
         <v>67</v>
       </c>
       <c r="G133" s="5"/>
-      <c r="H133" s="4" t="s">
-        <v>486</v>
+      <c r="H133" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="B134" t="s">
         <v>270</v>
       </c>
       <c r="C134" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="D134" t="s">
         <v>480</v>
@@ -10681,64 +10678,66 @@
       </c>
       <c r="G134" s="5"/>
       <c r="H134" t="s">
-        <v>304</v>
+        <v>487</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="B135" t="s">
         <v>270</v>
       </c>
       <c r="C135" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="D135" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>289</v>
+        <v>10</v>
       </c>
       <c r="F135" t="s">
-        <v>312</v>
-      </c>
-      <c r="G135" s="8" t="s">
-        <v>313</v>
+        <v>67</v>
+      </c>
+      <c r="G135" s="5"/>
+      <c r="H135" s="4" t="s">
+        <v>486</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="B136" t="s">
         <v>270</v>
       </c>
       <c r="C136" t="s">
-        <v>315</v>
+        <v>303</v>
       </c>
       <c r="D136" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>289</v>
+        <v>10</v>
       </c>
       <c r="F136" t="s">
-        <v>312</v>
-      </c>
-      <c r="G136" s="8" t="s">
-        <v>316</v>
+        <v>67</v>
+      </c>
+      <c r="G136" s="5"/>
+      <c r="H136" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="B137" t="s">
         <v>270</v>
       </c>
       <c r="C137" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="D137" t="s">
         <v>479</v>
@@ -10749,19 +10748,19 @@
       <c r="F137" t="s">
         <v>312</v>
       </c>
-      <c r="G137" s="5" t="s">
-        <v>319</v>
+      <c r="G137" s="8" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="B138" t="s">
         <v>270</v>
       </c>
       <c r="C138" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="D138" t="s">
         <v>479</v>
@@ -10772,19 +10771,19 @@
       <c r="F138" t="s">
         <v>312</v>
       </c>
-      <c r="G138" s="5" t="s">
-        <v>322</v>
+      <c r="G138" s="8" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="B139" t="s">
         <v>270</v>
       </c>
       <c r="C139" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="D139" t="s">
         <v>479</v>
@@ -10796,18 +10795,18 @@
         <v>312</v>
       </c>
       <c r="G139" s="5" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="B140" t="s">
         <v>270</v>
       </c>
       <c r="C140" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="D140" t="s">
         <v>479</v>
@@ -10819,18 +10818,18 @@
         <v>312</v>
       </c>
       <c r="G140" s="5" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="B141" t="s">
         <v>270</v>
       </c>
       <c r="C141" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="D141" t="s">
         <v>479</v>
@@ -10842,18 +10841,18 @@
         <v>312</v>
       </c>
       <c r="G141" s="5" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="B142" t="s">
         <v>270</v>
       </c>
       <c r="C142" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="D142" t="s">
         <v>479</v>
@@ -10865,18 +10864,18 @@
         <v>312</v>
       </c>
       <c r="G142" s="5" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="B143" t="s">
         <v>270</v>
       </c>
       <c r="C143" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="D143" t="s">
         <v>479</v>
@@ -10888,44 +10887,41 @@
         <v>312</v>
       </c>
       <c r="G143" s="5" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="B144" t="s">
         <v>270</v>
       </c>
       <c r="C144" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="D144" t="s">
         <v>479</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>141</v>
+        <v>289</v>
       </c>
       <c r="F144" t="s">
         <v>312</v>
       </c>
       <c r="G144" s="5" t="s">
-        <v>340</v>
-      </c>
-      <c r="H144" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="B145" t="s">
         <v>270</v>
       </c>
       <c r="C145" t="s">
-        <v>436</v>
+        <v>336</v>
       </c>
       <c r="D145" t="s">
         <v>479</v>
@@ -10937,41 +10933,44 @@
         <v>312</v>
       </c>
       <c r="G145" s="5" t="s">
-        <v>442</v>
+        <v>337</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="B146" t="s">
         <v>270</v>
       </c>
       <c r="C146" t="s">
-        <v>437</v>
+        <v>339</v>
       </c>
       <c r="D146" t="s">
         <v>479</v>
       </c>
-      <c r="E146" s="3" t="s">
-        <v>289</v>
+      <c r="E146" s="1" t="s">
+        <v>141</v>
       </c>
       <c r="F146" t="s">
         <v>312</v>
       </c>
       <c r="G146" s="5" t="s">
-        <v>440</v>
+        <v>340</v>
+      </c>
+      <c r="H146" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B147" t="s">
         <v>270</v>
       </c>
       <c r="C147" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="D147" t="s">
         <v>479</v>
@@ -10983,18 +10982,18 @@
         <v>312</v>
       </c>
       <c r="G147" s="5" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>430</v>
+        <v>343</v>
       </c>
       <c r="B148" t="s">
         <v>270</v>
       </c>
       <c r="C148" t="s">
-        <v>483</v>
+        <v>437</v>
       </c>
       <c r="D148" t="s">
         <v>479</v>
@@ -11006,21 +11005,18 @@
         <v>312</v>
       </c>
       <c r="G148" s="5" t="s">
-        <v>434</v>
-      </c>
-      <c r="H148" t="s">
-        <v>485</v>
+        <v>440</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>431</v>
+        <v>344</v>
       </c>
       <c r="B149" t="s">
         <v>270</v>
       </c>
       <c r="C149" t="s">
-        <v>484</v>
+        <v>438</v>
       </c>
       <c r="D149" t="s">
         <v>479</v>
@@ -11032,88 +11028,93 @@
         <v>312</v>
       </c>
       <c r="G149" s="5" t="s">
-        <v>435</v>
-      </c>
-      <c r="H149" t="s">
-        <v>485</v>
+        <v>441</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B150" t="s">
         <v>270</v>
       </c>
       <c r="C150" t="s">
-        <v>433</v>
+        <v>483</v>
       </c>
       <c r="D150" t="s">
         <v>479</v>
       </c>
-      <c r="E150" s="1" t="s">
+      <c r="E150" s="3" t="s">
         <v>289</v>
       </c>
       <c r="F150" t="s">
         <v>312</v>
       </c>
-      <c r="G150" s="10" t="s">
-        <v>439</v>
+      <c r="G150" s="5" t="s">
+        <v>434</v>
+      </c>
+      <c r="H150" t="s">
+        <v>485</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>345</v>
+        <v>431</v>
       </c>
       <c r="B151" t="s">
         <v>270</v>
       </c>
       <c r="C151" t="s">
-        <v>346</v>
+        <v>484</v>
       </c>
       <c r="D151" t="s">
         <v>479</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>10</v>
+        <v>289</v>
       </c>
       <c r="F151" t="s">
-        <v>347</v>
+        <v>312</v>
       </c>
       <c r="G151" s="5" t="s">
-        <v>348</v>
+        <v>435</v>
+      </c>
+      <c r="H151" t="s">
+        <v>485</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>349</v>
+        <v>432</v>
       </c>
       <c r="B152" t="s">
         <v>270</v>
       </c>
       <c r="C152" t="s">
-        <v>350</v>
+        <v>433</v>
       </c>
       <c r="D152" t="s">
         <v>479</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>10</v>
+        <v>289</v>
       </c>
       <c r="F152" t="s">
-        <v>67</v>
-      </c>
-      <c r="G152" s="5"/>
+        <v>312</v>
+      </c>
+      <c r="G152" s="10" t="s">
+        <v>439</v>
+      </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="B153" t="s">
         <v>270</v>
       </c>
       <c r="C153" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="D153" t="s">
         <v>479</v>
@@ -11122,21 +11123,21 @@
         <v>10</v>
       </c>
       <c r="F153" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="G153" s="5" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="B154" t="s">
         <v>270</v>
       </c>
       <c r="C154" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="D154" t="s">
         <v>479</v>
@@ -11145,22 +11146,19 @@
         <v>10</v>
       </c>
       <c r="F154" t="s">
-        <v>357</v>
+        <v>67</v>
       </c>
       <c r="G154" s="5"/>
-      <c r="H154" t="s">
-        <v>358</v>
-      </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="B155" t="s">
         <v>270</v>
       </c>
       <c r="C155" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="D155" t="s">
         <v>479</v>
@@ -11169,19 +11167,21 @@
         <v>10</v>
       </c>
       <c r="F155" t="s">
-        <v>67</v>
-      </c>
-      <c r="G155" s="5"/>
+        <v>353</v>
+      </c>
+      <c r="G155" s="5" t="s">
+        <v>354</v>
+      </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="B156" t="s">
         <v>270</v>
       </c>
       <c r="C156" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="D156" t="s">
         <v>479</v>
@@ -11190,19 +11190,22 @@
         <v>10</v>
       </c>
       <c r="F156" t="s">
-        <v>67</v>
+        <v>357</v>
       </c>
       <c r="G156" s="5"/>
+      <c r="H156" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="B157" t="s">
         <v>270</v>
       </c>
       <c r="C157" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="D157" t="s">
         <v>479</v>
@@ -11214,19 +11217,16 @@
         <v>67</v>
       </c>
       <c r="G157" s="5"/>
-      <c r="H157" t="s">
-        <v>365</v>
-      </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="B158" t="s">
         <v>270</v>
       </c>
       <c r="C158" t="s">
-        <v>578</v>
+        <v>362</v>
       </c>
       <c r="D158" t="s">
         <v>479</v>
@@ -11235,50 +11235,43 @@
         <v>10</v>
       </c>
       <c r="F158" t="s">
-        <v>367</v>
-      </c>
-      <c r="G158" s="5" t="s">
-        <v>368</v>
-      </c>
-      <c r="H158" t="s">
-        <v>369</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="G158" s="5"/>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="B159" t="s">
         <v>270</v>
       </c>
       <c r="C159" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="D159" t="s">
         <v>479</v>
       </c>
       <c r="E159" s="1" t="s">
-        <v>141</v>
+        <v>10</v>
       </c>
       <c r="F159" t="s">
-        <v>37</v>
-      </c>
-      <c r="G159" s="5" t="s">
-        <v>372</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="G159" s="5"/>
       <c r="H159" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="B160" t="s">
         <v>270</v>
       </c>
       <c r="C160" t="s">
-        <v>525</v>
+        <v>578</v>
       </c>
       <c r="D160" t="s">
         <v>479</v>
@@ -11287,41 +11280,50 @@
         <v>10</v>
       </c>
       <c r="F160" t="s">
-        <v>67</v>
-      </c>
-      <c r="G160" s="5"/>
+        <v>367</v>
+      </c>
+      <c r="G160" s="5" t="s">
+        <v>368</v>
+      </c>
       <c r="H160" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>568</v>
+        <v>370</v>
       </c>
       <c r="B161" t="s">
         <v>270</v>
       </c>
       <c r="C161" t="s">
-        <v>569</v>
+        <v>371</v>
       </c>
       <c r="D161" t="s">
         <v>479</v>
       </c>
-      <c r="E161" s="1"/>
+      <c r="E161" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="F161" t="s">
-        <v>67</v>
-      </c>
-      <c r="G161" s="5"/>
+        <v>37</v>
+      </c>
+      <c r="G161" s="5" t="s">
+        <v>372</v>
+      </c>
+      <c r="H161" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B162" t="s">
         <v>270</v>
       </c>
       <c r="C162" t="s">
-        <v>377</v>
+        <v>525</v>
       </c>
       <c r="D162" t="s">
         <v>479</v>
@@ -11334,80 +11336,79 @@
       </c>
       <c r="G162" s="5"/>
       <c r="H162" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>379</v>
+        <v>568</v>
       </c>
       <c r="B163" t="s">
         <v>270</v>
       </c>
       <c r="C163" t="s">
-        <v>630</v>
+        <v>569</v>
       </c>
       <c r="D163" t="s">
         <v>479</v>
       </c>
-      <c r="E163" t="s">
-        <v>10</v>
+      <c r="E163" s="1"/>
+      <c r="F163" t="s">
+        <v>67</v>
       </c>
       <c r="G163" s="5"/>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="B164" t="s">
         <v>270</v>
       </c>
       <c r="C164" t="s">
-        <v>445</v>
+        <v>377</v>
       </c>
       <c r="D164" t="s">
         <v>479</v>
       </c>
       <c r="E164" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="F164" t="s">
+        <v>67</v>
       </c>
       <c r="G164" s="5"/>
       <c r="H164" t="s">
-        <v>446</v>
+        <v>378</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B165" t="s">
         <v>270</v>
       </c>
       <c r="C165" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="D165" t="s">
         <v>479</v>
       </c>
-      <c r="E165" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F165" t="s">
-        <v>117</v>
-      </c>
-      <c r="G165" s="5" t="s">
-        <v>447</v>
-      </c>
+      <c r="E165" t="s">
+        <v>10</v>
+      </c>
+      <c r="G165" s="5"/>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B166" t="s">
         <v>270</v>
       </c>
       <c r="C166" t="s">
-        <v>462</v>
+        <v>445</v>
       </c>
       <c r="D166" t="s">
         <v>479</v>
@@ -11415,22 +11416,20 @@
       <c r="E166" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F166" t="s">
-        <v>234</v>
-      </c>
-      <c r="G166" s="5" t="s">
-        <v>383</v>
+      <c r="G166" s="5"/>
+      <c r="H166" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="B167" t="s">
         <v>270</v>
       </c>
       <c r="C167" t="s">
-        <v>385</v>
+        <v>629</v>
       </c>
       <c r="D167" t="s">
         <v>479</v>
@@ -11439,21 +11438,21 @@
         <v>10</v>
       </c>
       <c r="F167" t="s">
-        <v>234</v>
+        <v>117</v>
       </c>
       <c r="G167" s="5" t="s">
-        <v>386</v>
+        <v>447</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="B168" t="s">
         <v>270</v>
       </c>
       <c r="C168" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="D168" t="s">
         <v>479</v>
@@ -11465,41 +11464,41 @@
         <v>234</v>
       </c>
       <c r="G168" s="5" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="B169" t="s">
         <v>270</v>
       </c>
       <c r="C169" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="D169" t="s">
         <v>479</v>
       </c>
       <c r="E169" s="1" t="s">
-        <v>289</v>
+        <v>10</v>
       </c>
       <c r="F169" t="s">
-        <v>391</v>
+        <v>234</v>
       </c>
       <c r="G169" s="5" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="B170" t="s">
         <v>270</v>
       </c>
       <c r="C170" t="s">
-        <v>394</v>
+        <v>461</v>
       </c>
       <c r="D170" t="s">
         <v>479</v>
@@ -11508,44 +11507,44 @@
         <v>10</v>
       </c>
       <c r="F170" t="s">
-        <v>395</v>
+        <v>234</v>
       </c>
       <c r="G170" s="5" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="B171" t="s">
         <v>270</v>
       </c>
       <c r="C171" t="s">
-        <v>444</v>
+        <v>390</v>
       </c>
       <c r="D171" t="s">
         <v>479</v>
       </c>
       <c r="E171" s="1" t="s">
-        <v>10</v>
+        <v>289</v>
       </c>
       <c r="F171" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="G171" s="5" t="s">
-        <v>443</v>
+        <v>392</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>586</v>
+        <v>393</v>
       </c>
       <c r="B172" t="s">
         <v>270</v>
       </c>
       <c r="C172" t="s">
-        <v>587</v>
+        <v>394</v>
       </c>
       <c r="D172" t="s">
         <v>479</v>
@@ -11554,93 +11553,109 @@
         <v>10</v>
       </c>
       <c r="F172" t="s">
-        <v>67</v>
-      </c>
-      <c r="G172" s="5"/>
-      <c r="H172" t="s">
-        <v>588</v>
+        <v>395</v>
+      </c>
+      <c r="G172" s="5" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>532</v>
+        <v>397</v>
       </c>
       <c r="B173" t="s">
-        <v>448</v>
+        <v>270</v>
       </c>
       <c r="C173" t="s">
-        <v>477</v>
+        <v>444</v>
       </c>
       <c r="D173" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="E173" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F173" t="s">
-        <v>464</v>
-      </c>
-      <c r="G173" s="5">
-        <v>92003</v>
+        <v>398</v>
+      </c>
+      <c r="G173" s="5" t="s">
+        <v>443</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>533</v>
+        <v>586</v>
       </c>
       <c r="B174" t="s">
-        <v>448</v>
+        <v>270</v>
       </c>
       <c r="C174" t="s">
-        <v>449</v>
+        <v>587</v>
       </c>
       <c r="D174" t="s">
-        <v>482</v>
+        <v>479</v>
+      </c>
+      <c r="E174" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F174" t="s">
+        <v>67</v>
       </c>
       <c r="G174" s="5"/>
       <c r="H174" t="s">
-        <v>463</v>
+        <v>588</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B175" t="s">
         <v>448</v>
       </c>
       <c r="C175" t="s">
-        <v>450</v>
+        <v>477</v>
       </c>
       <c r="D175" t="s">
-        <v>479</v>
-      </c>
-      <c r="G175" s="5"/>
+        <v>482</v>
+      </c>
+      <c r="E175" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F175" t="s">
+        <v>464</v>
+      </c>
+      <c r="G175" s="5">
+        <v>92003</v>
+      </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="B176" t="s">
         <v>448</v>
       </c>
       <c r="C176" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D176" t="s">
-        <v>479</v>
+        <v>482</v>
       </c>
       <c r="G176" s="5"/>
+      <c r="H176" t="s">
+        <v>463</v>
+      </c>
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B177" t="s">
         <v>448</v>
       </c>
       <c r="C177" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D177" t="s">
         <v>479</v>
@@ -11649,13 +11664,13 @@
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B178" t="s">
         <v>448</v>
       </c>
       <c r="C178" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D178" t="s">
         <v>479</v>
@@ -11664,13 +11679,13 @@
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B179" t="s">
         <v>448</v>
       </c>
       <c r="C179" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="D179" t="s">
         <v>479</v>
@@ -11679,13 +11694,13 @@
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="B180" t="s">
         <v>448</v>
       </c>
       <c r="C180" t="s">
-        <v>540</v>
+        <v>453</v>
       </c>
       <c r="D180" t="s">
         <v>479</v>
@@ -11694,13 +11709,13 @@
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="B181" t="s">
         <v>448</v>
       </c>
       <c r="C181" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
       <c r="D181" t="s">
         <v>479</v>
@@ -11709,13 +11724,13 @@
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="B182" t="s">
         <v>448</v>
       </c>
       <c r="C182" t="s">
-        <v>455</v>
+        <v>540</v>
       </c>
       <c r="D182" t="s">
         <v>479</v>
@@ -11724,13 +11739,13 @@
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="B183" t="s">
         <v>448</v>
       </c>
       <c r="C183" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D183" t="s">
         <v>479</v>
@@ -11739,43 +11754,43 @@
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="B184" t="s">
         <v>448</v>
       </c>
       <c r="C184" t="s">
-        <v>545</v>
+        <v>455</v>
       </c>
       <c r="D184" t="s">
-        <v>554</v>
+        <v>479</v>
       </c>
       <c r="G184" s="5"/>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="B185" t="s">
         <v>448</v>
       </c>
       <c r="C185" t="s">
-        <v>548</v>
+        <v>456</v>
       </c>
       <c r="D185" t="s">
-        <v>554</v>
+        <v>479</v>
       </c>
       <c r="G185" s="5"/>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
       <c r="B186" t="s">
         <v>448</v>
       </c>
       <c r="C186" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="D186" t="s">
         <v>554</v>
@@ -11784,13 +11799,13 @@
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="B187" t="s">
         <v>448</v>
       </c>
       <c r="C187" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="D187" t="s">
         <v>554</v>
@@ -11799,99 +11814,129 @@
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>564</v>
+        <v>549</v>
       </c>
       <c r="B188" t="s">
         <v>448</v>
       </c>
       <c r="C188" t="s">
-        <v>567</v>
+        <v>551</v>
       </c>
       <c r="D188" t="s">
-        <v>482</v>
-      </c>
-      <c r="F188" t="s">
-        <v>565</v>
-      </c>
-      <c r="G188" s="5" t="s">
-        <v>566</v>
-      </c>
+        <v>554</v>
+      </c>
+      <c r="G188" s="5"/>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>575</v>
+        <v>550</v>
       </c>
       <c r="B189" t="s">
         <v>448</v>
       </c>
       <c r="C189" t="s">
-        <v>238</v>
+        <v>552</v>
       </c>
       <c r="D189" t="s">
-        <v>479</v>
-      </c>
-      <c r="E189" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F189" t="s">
-        <v>239</v>
+        <v>554</v>
       </c>
       <c r="G189" s="5"/>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>577</v>
+        <v>564</v>
       </c>
       <c r="B190" t="s">
-        <v>232</v>
+        <v>448</v>
       </c>
       <c r="C190" t="s">
-        <v>260</v>
+        <v>567</v>
       </c>
       <c r="D190" t="s">
-        <v>481</v>
-      </c>
-      <c r="E190" s="1" t="s">
-        <v>10</v>
+        <v>482</v>
       </c>
       <c r="F190" t="s">
-        <v>261</v>
-      </c>
-      <c r="G190" s="5"/>
-      <c r="H190" t="s">
-        <v>489</v>
+        <v>565</v>
+      </c>
+      <c r="G190" s="5" t="s">
+        <v>566</v>
       </c>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>546</v>
+        <v>575</v>
       </c>
       <c r="B191" t="s">
         <v>448</v>
       </c>
       <c r="C191" t="s">
-        <v>460</v>
+        <v>238</v>
       </c>
       <c r="D191" t="s">
-        <v>554</v>
+        <v>479</v>
+      </c>
+      <c r="E191" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F191" t="s">
+        <v>239</v>
       </c>
       <c r="G191" s="5"/>
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>553</v>
+        <v>577</v>
       </c>
       <c r="B192" t="s">
-        <v>448</v>
+        <v>232</v>
       </c>
       <c r="C192" t="s">
-        <v>458</v>
+        <v>260</v>
       </c>
       <c r="D192" t="s">
-        <v>554</v>
+        <v>481</v>
+      </c>
+      <c r="E192" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F192" t="s">
+        <v>261</v>
       </c>
       <c r="G192" s="5"/>
       <c r="H192" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>546</v>
+      </c>
+      <c r="B193" t="s">
+        <v>448</v>
+      </c>
+      <c r="C193" t="s">
+        <v>460</v>
+      </c>
+      <c r="D193" t="s">
+        <v>554</v>
+      </c>
+      <c r="G193" s="5"/>
+    </row>
+    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>553</v>
+      </c>
+      <c r="B194" t="s">
+        <v>448</v>
+      </c>
+      <c r="C194" t="s">
+        <v>458</v>
+      </c>
+      <c r="D194" t="s">
+        <v>554</v>
+      </c>
+      <c r="G194" s="5"/>
+      <c r="H194" t="s">
         <v>459</v>
       </c>
     </row>
@@ -11910,135 +11955,135 @@
     <hyperlink ref="E17" r:id="rId11" xr:uid="{91220B8C-C348-46A7-9967-EA4ACCF1D647}"/>
     <hyperlink ref="E18" r:id="rId12" xr:uid="{E0C9C4C1-D641-42A9-9B56-D4029F8CDFB4}"/>
     <hyperlink ref="E19" r:id="rId13" xr:uid="{6F28E518-974F-44BE-AE42-EFB20B3D76D1}"/>
-    <hyperlink ref="E21" r:id="rId14" xr:uid="{FDFF675B-FC08-4216-96E8-3B56FF5D770B}"/>
-    <hyperlink ref="E22" r:id="rId15" xr:uid="{9AA29EF8-A2F8-4925-94F2-B4F7AFD478E4}"/>
-    <hyperlink ref="E23" r:id="rId16" xr:uid="{F8F2BC0E-05CC-4628-BC90-BD98AA4895FF}"/>
-    <hyperlink ref="E39" r:id="rId17" xr:uid="{39BD6409-DC00-4BD4-A017-E05A3D15C7D2}"/>
-    <hyperlink ref="E38" r:id="rId18" xr:uid="{596DAA04-792B-42F8-A9FD-267B1B9A7CA2}"/>
-    <hyperlink ref="E40" r:id="rId19" xr:uid="{350F1ACC-8E41-4389-A6CC-B674D554D429}"/>
-    <hyperlink ref="E33" r:id="rId20" xr:uid="{FD8A9DE2-3E2E-4637-98CE-3B6829E5180D}"/>
-    <hyperlink ref="E34" r:id="rId21" xr:uid="{E1CF8E83-D2FD-48D2-9376-DEF821C49C6B}"/>
-    <hyperlink ref="E35" r:id="rId22" xr:uid="{FAADABC4-EEAC-40E9-84C7-A287145C9636}"/>
-    <hyperlink ref="E36" r:id="rId23" xr:uid="{E5415A8F-88D4-4C5E-8446-3D99783FDFEA}"/>
-    <hyperlink ref="E28" r:id="rId24" xr:uid="{07F96DB7-0AE9-408F-8C42-5EB2CEA3C026}"/>
-    <hyperlink ref="E29" r:id="rId25" xr:uid="{FC3F4CA2-FD7B-4D09-B4DB-01317A6C73D7}"/>
-    <hyperlink ref="E30" r:id="rId26" xr:uid="{90BB934F-F0FC-4443-BBC9-32BB27A75129}"/>
-    <hyperlink ref="E41" r:id="rId27" xr:uid="{C4691E01-6037-4385-B104-AF195A8A8C59}"/>
-    <hyperlink ref="E42" r:id="rId28" xr:uid="{04CA465C-BF7F-4262-A18F-7688827E5CD9}"/>
-    <hyperlink ref="E31" r:id="rId29" xr:uid="{84BD5FE8-1288-451A-A957-CE59903194BC}"/>
-    <hyperlink ref="E32" r:id="rId30" xr:uid="{1F4DF7D2-5902-4013-A667-4B6FB41385D0}"/>
-    <hyperlink ref="E43" r:id="rId31" xr:uid="{84406404-E636-4FBF-9CCA-CE4F02227EA6}"/>
-    <hyperlink ref="E44" r:id="rId32" xr:uid="{5A5E8193-A24C-47AB-8A5C-2EDBD030992D}"/>
-    <hyperlink ref="E46" r:id="rId33" xr:uid="{CA5DBEEA-29BB-480B-9D0D-DC20C8EF3FFF}"/>
-    <hyperlink ref="E47" r:id="rId34" xr:uid="{517E1C9A-3E42-46EA-8F09-E65EFA2D199B}"/>
-    <hyperlink ref="E49" r:id="rId35" xr:uid="{3A9135AA-ABF0-47BA-82C6-0F54E4AD8456}"/>
-    <hyperlink ref="E50" r:id="rId36" xr:uid="{11514DF0-7DCE-428B-ABCE-7A7F7786083C}"/>
-    <hyperlink ref="E54" r:id="rId37" xr:uid="{8474C762-2FA4-471F-88F4-9507ABBEA1D6}"/>
-    <hyperlink ref="E53" r:id="rId38" xr:uid="{B7636CDA-ED58-48B8-B4D3-9BE9C4450E9C}"/>
-    <hyperlink ref="E51" r:id="rId39" xr:uid="{467B3D48-F556-4DC3-9CD8-F58882EA0F04}"/>
-    <hyperlink ref="E52" r:id="rId40" xr:uid="{F24C1CFE-2E0B-45DB-B2E3-DB05E26885C3}"/>
-    <hyperlink ref="E48" r:id="rId41" xr:uid="{330AB8A4-8075-459A-828D-A7CA52D00C09}"/>
-    <hyperlink ref="E45" r:id="rId42" xr:uid="{AD09F005-7743-4B3F-B4FC-FB4B1F026C9B}"/>
-    <hyperlink ref="E56" r:id="rId43" xr:uid="{5415AFB7-220B-4379-BB87-BD51ABB3D173}"/>
-    <hyperlink ref="E55" r:id="rId44" xr:uid="{B4A2FA72-5FA9-438E-94C5-C7E835DB1EA2}"/>
-    <hyperlink ref="E59" r:id="rId45" xr:uid="{C60CF865-BCD8-47F6-A475-552204F4369C}"/>
-    <hyperlink ref="E58" r:id="rId46" xr:uid="{149A592E-555E-44E8-8CEE-44BCE1209AF3}"/>
-    <hyperlink ref="E60" r:id="rId47" xr:uid="{2658F9E0-0265-434E-BBB5-B98967B5B007}"/>
-    <hyperlink ref="E57" r:id="rId48" xr:uid="{7DF445B3-1872-486D-B99F-3EDA65B82488}"/>
-    <hyperlink ref="E63" r:id="rId49" xr:uid="{7EC7E37C-7549-40C8-81DE-8ACFDE03437C}"/>
-    <hyperlink ref="E65" r:id="rId50" xr:uid="{B5DAC180-9B3B-41CB-82EB-134E54507853}"/>
-    <hyperlink ref="E66" r:id="rId51" xr:uid="{FCD67149-1EF3-40DA-BB29-03662DB0E615}"/>
-    <hyperlink ref="E64" r:id="rId52" xr:uid="{85A32931-0A6D-4FED-BFFA-62A12F314D92}"/>
-    <hyperlink ref="E71" r:id="rId53" xr:uid="{B5C2A792-3025-4E08-BFB9-61ECF51B374D}"/>
-    <hyperlink ref="E72" r:id="rId54" xr:uid="{97CED2FD-9F84-464D-9342-72A124A363BC}"/>
-    <hyperlink ref="E74" r:id="rId55" xr:uid="{980BBB81-A1C1-4ACA-8663-5B0460438D1D}"/>
-    <hyperlink ref="E73" r:id="rId56" xr:uid="{02868430-C4CD-4A7F-88A2-39B6B75D371E}"/>
-    <hyperlink ref="E67" r:id="rId57" xr:uid="{1E13D856-EEFD-4ABB-A5C0-5D1E0BF95A82}"/>
-    <hyperlink ref="E68" r:id="rId58" xr:uid="{5FB21DD1-70AF-4D29-A5BB-7D9EB3DA55F6}"/>
-    <hyperlink ref="E69" r:id="rId59" xr:uid="{DDD755CF-63DF-476F-8368-DCF07DCD4609}"/>
-    <hyperlink ref="E70" r:id="rId60" xr:uid="{2FBCBAC4-D205-410D-8C00-8356A8ECB67E}"/>
-    <hyperlink ref="E75" r:id="rId61" xr:uid="{AA939156-F9E5-43B8-8761-6EE0951EA9FF}"/>
-    <hyperlink ref="E76" r:id="rId62" xr:uid="{B5798FB4-C1E2-456D-9711-87A309BD6878}"/>
-    <hyperlink ref="E109" r:id="rId63" xr:uid="{DE574022-7D55-4097-9D55-6421929BB4D6}"/>
-    <hyperlink ref="E110" r:id="rId64" xr:uid="{17BD79E0-0F48-49EC-8C65-CB173907FEB0}"/>
-    <hyperlink ref="E106" r:id="rId65" xr:uid="{ADD3565F-8131-4C8E-BEF2-FA6062A0F466}"/>
-    <hyperlink ref="E107" r:id="rId66" xr:uid="{31F424C2-D731-4E26-ACED-E2DE4D8451E9}"/>
-    <hyperlink ref="E189" r:id="rId67" xr:uid="{8C8DD198-5284-45E6-AC60-523B30266C35}"/>
-    <hyperlink ref="E111" r:id="rId68" xr:uid="{03FFC474-5820-4AA4-BF45-21ED811B5D6B}"/>
-    <hyperlink ref="E112" r:id="rId69" xr:uid="{1D5962C8-1986-4122-8F07-ED623C46A3C9}"/>
-    <hyperlink ref="E113" r:id="rId70" xr:uid="{F572B91D-DA7D-4AB2-978B-0BA81A3AB914}"/>
-    <hyperlink ref="E114" r:id="rId71" xr:uid="{2472D891-5A22-47C0-B741-7E0E5ADD05A1}"/>
-    <hyperlink ref="E190" r:id="rId72" xr:uid="{C21B974D-1E8B-4463-8243-F86F1DB608FC}"/>
-    <hyperlink ref="E115" r:id="rId73" xr:uid="{24BB6E77-83B4-4F7F-A249-3E020A224BE1}"/>
-    <hyperlink ref="E116" r:id="rId74" xr:uid="{1DF76622-6E9B-4B29-8601-44F2E3930EB0}"/>
-    <hyperlink ref="E117" r:id="rId75" xr:uid="{DEEFB1B1-E0E5-40BF-B4FF-15669DE884F9}"/>
-    <hyperlink ref="E135" r:id="rId76" xr:uid="{EB10DAA1-2581-44AA-B02F-EF7834AE0264}"/>
-    <hyperlink ref="E136" r:id="rId77" xr:uid="{D3E6AEA5-E392-4135-A858-F628EB7503A4}"/>
-    <hyperlink ref="E137" r:id="rId78" xr:uid="{09D7B138-477C-45D9-85FE-90663A1056C9}"/>
-    <hyperlink ref="E138" r:id="rId79" xr:uid="{631945C2-34E1-4750-8BEA-BDABAE971896}"/>
-    <hyperlink ref="E139" r:id="rId80" xr:uid="{BA1F0E6D-1DBE-4A90-A33F-469C641718DF}"/>
-    <hyperlink ref="E140" r:id="rId81" xr:uid="{F9D86F45-D9C9-4538-B341-DF5A33CC0EFC}"/>
-    <hyperlink ref="E141" r:id="rId82" xr:uid="{2AADD4A8-A263-428A-A5BF-8C42D2AABE5D}"/>
-    <hyperlink ref="E142" r:id="rId83" xr:uid="{946C6856-98BA-4E8A-B829-4FEE05381A8D}"/>
-    <hyperlink ref="E143" r:id="rId84" xr:uid="{57D85244-0DAF-4BB8-9EEE-D9FCFDD83C97}"/>
-    <hyperlink ref="E144" r:id="rId85" display="MISUMI" xr:uid="{4B5CAC98-6580-4911-9884-A5ED64A6DCB4}"/>
-    <hyperlink ref="E128" r:id="rId86" xr:uid="{1446C3F8-F3D9-455E-BC26-48F648FA30AE}"/>
-    <hyperlink ref="E127" r:id="rId87" xr:uid="{8B07067C-5948-45DF-8DF6-8C7211AB660D}"/>
-    <hyperlink ref="E123" r:id="rId88" xr:uid="{8F38FC91-B580-4FD2-8ECB-343E24FAA585}"/>
-    <hyperlink ref="E124" r:id="rId89" xr:uid="{36201AD7-A1AD-4E30-98D6-22A498A00BA9}"/>
-    <hyperlink ref="E125" r:id="rId90" xr:uid="{72BC9AEB-CD73-4EFE-BF72-603FA37D26EB}"/>
-    <hyperlink ref="E126" r:id="rId91" xr:uid="{6EB20256-2B70-4154-9BFB-63BC557C9FF7}"/>
-    <hyperlink ref="E153" r:id="rId92" xr:uid="{70213BBC-D94D-4352-81EE-65753DC5766C}"/>
-    <hyperlink ref="E154" r:id="rId93" xr:uid="{27BD824A-A22E-4944-9DEC-9A48AB945C46}"/>
-    <hyperlink ref="E152" r:id="rId94" xr:uid="{C8E0C7B3-F9AE-4EC8-9761-C357883B19EB}"/>
-    <hyperlink ref="E157" r:id="rId95" xr:uid="{7305F7C5-B953-4BBB-A644-B36EF58D00F8}"/>
-    <hyperlink ref="E155" r:id="rId96" xr:uid="{4E72F6FF-E359-403E-8C10-899982A46106}"/>
-    <hyperlink ref="E156" r:id="rId97" xr:uid="{DC29AC1A-C353-42E1-A92B-B169D3D58EA9}"/>
-    <hyperlink ref="E158" r:id="rId98" xr:uid="{3C1A7911-DFEA-4653-9C41-4CCA8D4B0F7E}"/>
-    <hyperlink ref="E167" r:id="rId99" xr:uid="{2B9BE5C8-7021-4253-97F8-0AF75D476D51}"/>
-    <hyperlink ref="E166" r:id="rId100" xr:uid="{71B9EE24-F9E3-47B0-9DB1-DE809D668D49}"/>
-    <hyperlink ref="E168" r:id="rId101" xr:uid="{8B5F072C-581E-4B93-A107-047F4E567BD3}"/>
-    <hyperlink ref="E170" r:id="rId102" xr:uid="{CC0CACD1-E193-4320-BA06-AD19994EB98E}"/>
-    <hyperlink ref="E169" r:id="rId103" xr:uid="{E48C6228-D60E-464A-B72D-6345D0E3CC68}"/>
-    <hyperlink ref="E159" r:id="rId104" xr:uid="{E5167E91-C797-4BC7-BB2F-6598B43FEF38}"/>
-    <hyperlink ref="E129" r:id="rId105" xr:uid="{5D0C387C-6BF9-4CCF-8CDD-27709B01C265}"/>
-    <hyperlink ref="E160" r:id="rId106" xr:uid="{7A2DC4C0-FF36-43BA-A189-3BD54D156058}"/>
-    <hyperlink ref="E134" r:id="rId107" xr:uid="{116340D2-01CC-4E5D-8CFC-C2B1A68AE3F6}"/>
-    <hyperlink ref="E132" r:id="rId108" xr:uid="{B4D0E8D6-7F8E-449B-8D1F-8D7EBCF17B93}"/>
-    <hyperlink ref="E133" r:id="rId109" xr:uid="{04C0BD6E-A059-46D2-BDE2-26C5AC6A938D}"/>
-    <hyperlink ref="E162" r:id="rId110" xr:uid="{8342F021-8D39-4131-8F90-D524FB7AEA9D}"/>
-    <hyperlink ref="E151" r:id="rId111" xr:uid="{86B132C5-CB3B-447C-926A-7EF611C31616}"/>
-    <hyperlink ref="E145" r:id="rId112" xr:uid="{EA253D54-3F1D-4A03-A0D3-7F679CF9F47E}"/>
-    <hyperlink ref="E147" r:id="rId113" xr:uid="{5BD6299F-0EC3-4F51-AC82-FF124DBC4020}"/>
-    <hyperlink ref="E171" r:id="rId114" xr:uid="{3B84E3E9-7F9C-4F1F-B4B3-A52D4EEFB917}"/>
+    <hyperlink ref="E22" r:id="rId14" xr:uid="{FDFF675B-FC08-4216-96E8-3B56FF5D770B}"/>
+    <hyperlink ref="E23" r:id="rId15" xr:uid="{9AA29EF8-A2F8-4925-94F2-B4F7AFD478E4}"/>
+    <hyperlink ref="E24" r:id="rId16" xr:uid="{F8F2BC0E-05CC-4628-BC90-BD98AA4895FF}"/>
+    <hyperlink ref="E41" r:id="rId17" xr:uid="{39BD6409-DC00-4BD4-A017-E05A3D15C7D2}"/>
+    <hyperlink ref="E40" r:id="rId18" xr:uid="{596DAA04-792B-42F8-A9FD-267B1B9A7CA2}"/>
+    <hyperlink ref="E42" r:id="rId19" xr:uid="{350F1ACC-8E41-4389-A6CC-B674D554D429}"/>
+    <hyperlink ref="E35" r:id="rId20" xr:uid="{FD8A9DE2-3E2E-4637-98CE-3B6829E5180D}"/>
+    <hyperlink ref="E36" r:id="rId21" xr:uid="{E1CF8E83-D2FD-48D2-9376-DEF821C49C6B}"/>
+    <hyperlink ref="E37" r:id="rId22" xr:uid="{FAADABC4-EEAC-40E9-84C7-A287145C9636}"/>
+    <hyperlink ref="E38" r:id="rId23" xr:uid="{E5415A8F-88D4-4C5E-8446-3D99783FDFEA}"/>
+    <hyperlink ref="E30" r:id="rId24" xr:uid="{07F96DB7-0AE9-408F-8C42-5EB2CEA3C026}"/>
+    <hyperlink ref="E31" r:id="rId25" xr:uid="{FC3F4CA2-FD7B-4D09-B4DB-01317A6C73D7}"/>
+    <hyperlink ref="E32" r:id="rId26" xr:uid="{90BB934F-F0FC-4443-BBC9-32BB27A75129}"/>
+    <hyperlink ref="E43" r:id="rId27" xr:uid="{C4691E01-6037-4385-B104-AF195A8A8C59}"/>
+    <hyperlink ref="E44" r:id="rId28" xr:uid="{04CA465C-BF7F-4262-A18F-7688827E5CD9}"/>
+    <hyperlink ref="E33" r:id="rId29" xr:uid="{84BD5FE8-1288-451A-A957-CE59903194BC}"/>
+    <hyperlink ref="E34" r:id="rId30" xr:uid="{1F4DF7D2-5902-4013-A667-4B6FB41385D0}"/>
+    <hyperlink ref="E45" r:id="rId31" xr:uid="{84406404-E636-4FBF-9CCA-CE4F02227EA6}"/>
+    <hyperlink ref="E46" r:id="rId32" xr:uid="{5A5E8193-A24C-47AB-8A5C-2EDBD030992D}"/>
+    <hyperlink ref="E48" r:id="rId33" xr:uid="{CA5DBEEA-29BB-480B-9D0D-DC20C8EF3FFF}"/>
+    <hyperlink ref="E49" r:id="rId34" xr:uid="{517E1C9A-3E42-46EA-8F09-E65EFA2D199B}"/>
+    <hyperlink ref="E51" r:id="rId35" xr:uid="{3A9135AA-ABF0-47BA-82C6-0F54E4AD8456}"/>
+    <hyperlink ref="E52" r:id="rId36" xr:uid="{11514DF0-7DCE-428B-ABCE-7A7F7786083C}"/>
+    <hyperlink ref="E56" r:id="rId37" xr:uid="{8474C762-2FA4-471F-88F4-9507ABBEA1D6}"/>
+    <hyperlink ref="E55" r:id="rId38" xr:uid="{B7636CDA-ED58-48B8-B4D3-9BE9C4450E9C}"/>
+    <hyperlink ref="E53" r:id="rId39" xr:uid="{467B3D48-F556-4DC3-9CD8-F58882EA0F04}"/>
+    <hyperlink ref="E54" r:id="rId40" xr:uid="{F24C1CFE-2E0B-45DB-B2E3-DB05E26885C3}"/>
+    <hyperlink ref="E50" r:id="rId41" xr:uid="{330AB8A4-8075-459A-828D-A7CA52D00C09}"/>
+    <hyperlink ref="E47" r:id="rId42" xr:uid="{AD09F005-7743-4B3F-B4FC-FB4B1F026C9B}"/>
+    <hyperlink ref="E58" r:id="rId43" xr:uid="{5415AFB7-220B-4379-BB87-BD51ABB3D173}"/>
+    <hyperlink ref="E57" r:id="rId44" xr:uid="{B4A2FA72-5FA9-438E-94C5-C7E835DB1EA2}"/>
+    <hyperlink ref="E61" r:id="rId45" xr:uid="{C60CF865-BCD8-47F6-A475-552204F4369C}"/>
+    <hyperlink ref="E60" r:id="rId46" xr:uid="{149A592E-555E-44E8-8CEE-44BCE1209AF3}"/>
+    <hyperlink ref="E62" r:id="rId47" xr:uid="{2658F9E0-0265-434E-BBB5-B98967B5B007}"/>
+    <hyperlink ref="E59" r:id="rId48" xr:uid="{7DF445B3-1872-486D-B99F-3EDA65B82488}"/>
+    <hyperlink ref="E65" r:id="rId49" xr:uid="{7EC7E37C-7549-40C8-81DE-8ACFDE03437C}"/>
+    <hyperlink ref="E67" r:id="rId50" xr:uid="{B5DAC180-9B3B-41CB-82EB-134E54507853}"/>
+    <hyperlink ref="E68" r:id="rId51" xr:uid="{FCD67149-1EF3-40DA-BB29-03662DB0E615}"/>
+    <hyperlink ref="E66" r:id="rId52" xr:uid="{85A32931-0A6D-4FED-BFFA-62A12F314D92}"/>
+    <hyperlink ref="E73" r:id="rId53" xr:uid="{B5C2A792-3025-4E08-BFB9-61ECF51B374D}"/>
+    <hyperlink ref="E74" r:id="rId54" xr:uid="{97CED2FD-9F84-464D-9342-72A124A363BC}"/>
+    <hyperlink ref="E76" r:id="rId55" xr:uid="{980BBB81-A1C1-4ACA-8663-5B0460438D1D}"/>
+    <hyperlink ref="E75" r:id="rId56" xr:uid="{02868430-C4CD-4A7F-88A2-39B6B75D371E}"/>
+    <hyperlink ref="E69" r:id="rId57" xr:uid="{1E13D856-EEFD-4ABB-A5C0-5D1E0BF95A82}"/>
+    <hyperlink ref="E70" r:id="rId58" xr:uid="{5FB21DD1-70AF-4D29-A5BB-7D9EB3DA55F6}"/>
+    <hyperlink ref="E71" r:id="rId59" xr:uid="{DDD755CF-63DF-476F-8368-DCF07DCD4609}"/>
+    <hyperlink ref="E72" r:id="rId60" xr:uid="{2FBCBAC4-D205-410D-8C00-8356A8ECB67E}"/>
+    <hyperlink ref="E77" r:id="rId61" xr:uid="{AA939156-F9E5-43B8-8761-6EE0951EA9FF}"/>
+    <hyperlink ref="E78" r:id="rId62" xr:uid="{B5798FB4-C1E2-456D-9711-87A309BD6878}"/>
+    <hyperlink ref="E111" r:id="rId63" xr:uid="{DE574022-7D55-4097-9D55-6421929BB4D6}"/>
+    <hyperlink ref="E112" r:id="rId64" xr:uid="{17BD79E0-0F48-49EC-8C65-CB173907FEB0}"/>
+    <hyperlink ref="E108" r:id="rId65" xr:uid="{ADD3565F-8131-4C8E-BEF2-FA6062A0F466}"/>
+    <hyperlink ref="E109" r:id="rId66" xr:uid="{31F424C2-D731-4E26-ACED-E2DE4D8451E9}"/>
+    <hyperlink ref="E191" r:id="rId67" xr:uid="{8C8DD198-5284-45E6-AC60-523B30266C35}"/>
+    <hyperlink ref="E113" r:id="rId68" xr:uid="{03FFC474-5820-4AA4-BF45-21ED811B5D6B}"/>
+    <hyperlink ref="E114" r:id="rId69" xr:uid="{1D5962C8-1986-4122-8F07-ED623C46A3C9}"/>
+    <hyperlink ref="E115" r:id="rId70" xr:uid="{F572B91D-DA7D-4AB2-978B-0BA81A3AB914}"/>
+    <hyperlink ref="E116" r:id="rId71" xr:uid="{2472D891-5A22-47C0-B741-7E0E5ADD05A1}"/>
+    <hyperlink ref="E192" r:id="rId72" xr:uid="{C21B974D-1E8B-4463-8243-F86F1DB608FC}"/>
+    <hyperlink ref="E117" r:id="rId73" xr:uid="{24BB6E77-83B4-4F7F-A249-3E020A224BE1}"/>
+    <hyperlink ref="E118" r:id="rId74" xr:uid="{1DF76622-6E9B-4B29-8601-44F2E3930EB0}"/>
+    <hyperlink ref="E119" r:id="rId75" xr:uid="{DEEFB1B1-E0E5-40BF-B4FF-15669DE884F9}"/>
+    <hyperlink ref="E137" r:id="rId76" xr:uid="{EB10DAA1-2581-44AA-B02F-EF7834AE0264}"/>
+    <hyperlink ref="E138" r:id="rId77" xr:uid="{D3E6AEA5-E392-4135-A858-F628EB7503A4}"/>
+    <hyperlink ref="E139" r:id="rId78" xr:uid="{09D7B138-477C-45D9-85FE-90663A1056C9}"/>
+    <hyperlink ref="E140" r:id="rId79" xr:uid="{631945C2-34E1-4750-8BEA-BDABAE971896}"/>
+    <hyperlink ref="E141" r:id="rId80" xr:uid="{BA1F0E6D-1DBE-4A90-A33F-469C641718DF}"/>
+    <hyperlink ref="E142" r:id="rId81" xr:uid="{F9D86F45-D9C9-4538-B341-DF5A33CC0EFC}"/>
+    <hyperlink ref="E143" r:id="rId82" xr:uid="{2AADD4A8-A263-428A-A5BF-8C42D2AABE5D}"/>
+    <hyperlink ref="E144" r:id="rId83" xr:uid="{946C6856-98BA-4E8A-B829-4FEE05381A8D}"/>
+    <hyperlink ref="E145" r:id="rId84" xr:uid="{57D85244-0DAF-4BB8-9EEE-D9FCFDD83C97}"/>
+    <hyperlink ref="E146" r:id="rId85" display="MISUMI" xr:uid="{4B5CAC98-6580-4911-9884-A5ED64A6DCB4}"/>
+    <hyperlink ref="E130" r:id="rId86" xr:uid="{1446C3F8-F3D9-455E-BC26-48F648FA30AE}"/>
+    <hyperlink ref="E129" r:id="rId87" xr:uid="{8B07067C-5948-45DF-8DF6-8C7211AB660D}"/>
+    <hyperlink ref="E125" r:id="rId88" xr:uid="{8F38FC91-B580-4FD2-8ECB-343E24FAA585}"/>
+    <hyperlink ref="E126" r:id="rId89" xr:uid="{36201AD7-A1AD-4E30-98D6-22A498A00BA9}"/>
+    <hyperlink ref="E127" r:id="rId90" xr:uid="{72BC9AEB-CD73-4EFE-BF72-603FA37D26EB}"/>
+    <hyperlink ref="E128" r:id="rId91" xr:uid="{6EB20256-2B70-4154-9BFB-63BC557C9FF7}"/>
+    <hyperlink ref="E155" r:id="rId92" xr:uid="{70213BBC-D94D-4352-81EE-65753DC5766C}"/>
+    <hyperlink ref="E156" r:id="rId93" xr:uid="{27BD824A-A22E-4944-9DEC-9A48AB945C46}"/>
+    <hyperlink ref="E154" r:id="rId94" xr:uid="{C8E0C7B3-F9AE-4EC8-9761-C357883B19EB}"/>
+    <hyperlink ref="E159" r:id="rId95" xr:uid="{7305F7C5-B953-4BBB-A644-B36EF58D00F8}"/>
+    <hyperlink ref="E157" r:id="rId96" xr:uid="{4E72F6FF-E359-403E-8C10-899982A46106}"/>
+    <hyperlink ref="E158" r:id="rId97" xr:uid="{DC29AC1A-C353-42E1-A92B-B169D3D58EA9}"/>
+    <hyperlink ref="E160" r:id="rId98" xr:uid="{3C1A7911-DFEA-4653-9C41-4CCA8D4B0F7E}"/>
+    <hyperlink ref="E169" r:id="rId99" xr:uid="{2B9BE5C8-7021-4253-97F8-0AF75D476D51}"/>
+    <hyperlink ref="E168" r:id="rId100" xr:uid="{71B9EE24-F9E3-47B0-9DB1-DE809D668D49}"/>
+    <hyperlink ref="E170" r:id="rId101" xr:uid="{8B5F072C-581E-4B93-A107-047F4E567BD3}"/>
+    <hyperlink ref="E172" r:id="rId102" xr:uid="{CC0CACD1-E193-4320-BA06-AD19994EB98E}"/>
+    <hyperlink ref="E171" r:id="rId103" xr:uid="{E48C6228-D60E-464A-B72D-6345D0E3CC68}"/>
+    <hyperlink ref="E161" r:id="rId104" xr:uid="{E5167E91-C797-4BC7-BB2F-6598B43FEF38}"/>
+    <hyperlink ref="E131" r:id="rId105" xr:uid="{5D0C387C-6BF9-4CCF-8CDD-27709B01C265}"/>
+    <hyperlink ref="E162" r:id="rId106" xr:uid="{7A2DC4C0-FF36-43BA-A189-3BD54D156058}"/>
+    <hyperlink ref="E136" r:id="rId107" xr:uid="{116340D2-01CC-4E5D-8CFC-C2B1A68AE3F6}"/>
+    <hyperlink ref="E134" r:id="rId108" xr:uid="{B4D0E8D6-7F8E-449B-8D1F-8D7EBCF17B93}"/>
+    <hyperlink ref="E135" r:id="rId109" xr:uid="{04C0BD6E-A059-46D2-BDE2-26C5AC6A938D}"/>
+    <hyperlink ref="E164" r:id="rId110" xr:uid="{8342F021-8D39-4131-8F90-D524FB7AEA9D}"/>
+    <hyperlink ref="E153" r:id="rId111" xr:uid="{86B132C5-CB3B-447C-926A-7EF611C31616}"/>
+    <hyperlink ref="E147" r:id="rId112" xr:uid="{EA253D54-3F1D-4A03-A0D3-7F679CF9F47E}"/>
+    <hyperlink ref="E149" r:id="rId113" xr:uid="{5BD6299F-0EC3-4F51-AC82-FF124DBC4020}"/>
+    <hyperlink ref="E173" r:id="rId114" xr:uid="{3B84E3E9-7F9C-4F1F-B4B3-A52D4EEFB917}"/>
     <hyperlink ref="E2" r:id="rId115" xr:uid="{11C9A353-3E3E-4A5B-A149-F9DCD5EAC942}"/>
     <hyperlink ref="E4" r:id="rId116" xr:uid="{FA0452B0-82F7-471E-90D4-A2F200486D8C}"/>
     <hyperlink ref="E3" r:id="rId117" xr:uid="{17585C18-58AC-4CE7-9578-2F63696D867B}"/>
     <hyperlink ref="E5" r:id="rId118" xr:uid="{09D76B63-3F40-48F7-95B0-49AFA9753495}"/>
-    <hyperlink ref="E25" r:id="rId119" xr:uid="{32F8939F-DC89-4273-A80E-CFFEF0ECCF60}"/>
-    <hyperlink ref="E130" r:id="rId120" xr:uid="{FF03F29F-526A-43E5-81D3-97BE750C5878}"/>
-    <hyperlink ref="E131" r:id="rId121" xr:uid="{488FC55A-8C05-4264-9AFB-1BE9A4D762DC}"/>
-    <hyperlink ref="E148" r:id="rId122" xr:uid="{369738BB-65CA-4CEA-AE2F-C5D3D903F148}"/>
-    <hyperlink ref="E149" r:id="rId123" xr:uid="{899DE784-1FB2-4A3F-BA67-B60FD0ED9C31}"/>
-    <hyperlink ref="E150" r:id="rId124" xr:uid="{416E9179-6A41-4C5A-955D-4A8B6488BC03}"/>
-    <hyperlink ref="E146" r:id="rId125" xr:uid="{ED6FE160-7585-48D5-BE73-72E0F12618ED}"/>
-    <hyperlink ref="E164" r:id="rId126" xr:uid="{863E8587-1A74-4216-A533-FD4D1FD293D3}"/>
-    <hyperlink ref="E173" r:id="rId127" xr:uid="{29CE548D-B2B4-4587-A753-C066B1AFBF82}"/>
-    <hyperlink ref="E61" r:id="rId128" xr:uid="{7D63EDBD-9486-4D70-A8EB-EC35CE324B2B}"/>
-    <hyperlink ref="E118" r:id="rId129" xr:uid="{A98A24AB-1380-4DE0-A6F4-00B837BDCB8A}"/>
+    <hyperlink ref="E26" r:id="rId119" xr:uid="{32F8939F-DC89-4273-A80E-CFFEF0ECCF60}"/>
+    <hyperlink ref="E132" r:id="rId120" xr:uid="{FF03F29F-526A-43E5-81D3-97BE750C5878}"/>
+    <hyperlink ref="E133" r:id="rId121" xr:uid="{488FC55A-8C05-4264-9AFB-1BE9A4D762DC}"/>
+    <hyperlink ref="E150" r:id="rId122" xr:uid="{369738BB-65CA-4CEA-AE2F-C5D3D903F148}"/>
+    <hyperlink ref="E151" r:id="rId123" xr:uid="{899DE784-1FB2-4A3F-BA67-B60FD0ED9C31}"/>
+    <hyperlink ref="E152" r:id="rId124" xr:uid="{416E9179-6A41-4C5A-955D-4A8B6488BC03}"/>
+    <hyperlink ref="E148" r:id="rId125" xr:uid="{ED6FE160-7585-48D5-BE73-72E0F12618ED}"/>
+    <hyperlink ref="E166" r:id="rId126" xr:uid="{863E8587-1A74-4216-A533-FD4D1FD293D3}"/>
+    <hyperlink ref="E175" r:id="rId127" xr:uid="{29CE548D-B2B4-4587-A753-C066B1AFBF82}"/>
+    <hyperlink ref="E63" r:id="rId128" xr:uid="{7D63EDBD-9486-4D70-A8EB-EC35CE324B2B}"/>
+    <hyperlink ref="E120" r:id="rId129" xr:uid="{A98A24AB-1380-4DE0-A6F4-00B837BDCB8A}"/>
     <hyperlink ref="H17" r:id="rId130" display="Bulk Link" xr:uid="{F82FB24D-F456-4AD0-A18C-EFB9462C2336}"/>
     <hyperlink ref="E15" r:id="rId131" xr:uid="{9B908FEE-C2B6-4B01-873F-1D31646DA108}"/>
-    <hyperlink ref="E24" r:id="rId132" xr:uid="{648BFDEF-0776-40CB-96BD-3105232BF7C5}"/>
-    <hyperlink ref="E119" r:id="rId133" xr:uid="{E8DEB348-3B00-41C7-85D4-7BD6198F40E2}"/>
-    <hyperlink ref="E26" r:id="rId134" xr:uid="{365853CB-05CC-49D9-935A-4155641501C2}"/>
+    <hyperlink ref="E25" r:id="rId132" xr:uid="{648BFDEF-0776-40CB-96BD-3105232BF7C5}"/>
+    <hyperlink ref="E121" r:id="rId133" xr:uid="{E8DEB348-3B00-41C7-85D4-7BD6198F40E2}"/>
+    <hyperlink ref="E27" r:id="rId134" xr:uid="{365853CB-05CC-49D9-935A-4155641501C2}"/>
     <hyperlink ref="E20" r:id="rId135" xr:uid="{1434FB4A-AD21-4365-A9D6-F5C278481092}"/>
-    <hyperlink ref="E37" r:id="rId136" xr:uid="{3F170435-BC60-4CD0-85D5-AB822CAD5955}"/>
-    <hyperlink ref="E172" r:id="rId137" xr:uid="{792BF035-BBA1-4EB3-B614-DCA9990A42C4}"/>
-    <hyperlink ref="E120" r:id="rId138" xr:uid="{439405A6-C063-4FCA-B4EC-EC73BF273123}"/>
-    <hyperlink ref="E121" r:id="rId139" xr:uid="{32E6CB73-CB22-4831-BA9B-31BA5269C4ED}"/>
-    <hyperlink ref="E122" r:id="rId140" xr:uid="{BB2B7640-97E7-4C45-875F-001470775177}"/>
-    <hyperlink ref="E105" r:id="rId141" xr:uid="{7941F873-0C16-46F4-AD41-77D42F7F1889}"/>
-    <hyperlink ref="E165" r:id="rId142" xr:uid="{C2C174FC-F9AD-4008-B396-2B912B550A9A}"/>
+    <hyperlink ref="E39" r:id="rId136" xr:uid="{3F170435-BC60-4CD0-85D5-AB822CAD5955}"/>
+    <hyperlink ref="E174" r:id="rId137" xr:uid="{792BF035-BBA1-4EB3-B614-DCA9990A42C4}"/>
+    <hyperlink ref="E122" r:id="rId138" xr:uid="{439405A6-C063-4FCA-B4EC-EC73BF273123}"/>
+    <hyperlink ref="E123" r:id="rId139" xr:uid="{32E6CB73-CB22-4831-BA9B-31BA5269C4ED}"/>
+    <hyperlink ref="E124" r:id="rId140" xr:uid="{BB2B7640-97E7-4C45-875F-001470775177}"/>
+    <hyperlink ref="E107" r:id="rId141" xr:uid="{7941F873-0C16-46F4-AD41-77D42F7F1889}"/>
+    <hyperlink ref="E167" r:id="rId142" xr:uid="{C2C174FC-F9AD-4008-B396-2B912B550A9A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId143"/>

</xml_diff>

<commit_message>
Updated stepper mount; added laser cut paths for paneling.
## 2022-03-18

- Laid out panels for laser cutting on 4'x5' sheets.
- Now have both engineering sketches and laser cut paths in the `BOM` folder; closing #33

## 2022-03-17

- Finished draft of engineering sketches.
- Several more renders of the panels for the fabricator to see.
- Re-export PN016, the stepper mounts, as I forgot on the 16th.
</commit_message>
<xml_diff>
--- a/BOM/General Part List.xlsx
+++ b/BOM/General Part List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\Documents\3D Print\Clockmaker\clock-3\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0922E5F-BECD-4E96-83DE-FDF829026C71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D652E0-B198-404F-97A4-D1C08FBA8F52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{6EB0A7B6-C6D7-4759-8B58-841D5EFF92F5}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="8" xr2:uid="{6EB0A7B6-C6D7-4759-8B58-841D5EFF92F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Electrical" sheetId="4" r:id="rId1"/>
@@ -33,6 +33,7 @@
     <definedName name="ExternalData_6" localSheetId="7" hidden="1">Transmission!$A$1:$H$13</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -78,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2837" uniqueCount="797">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2831" uniqueCount="798">
   <si>
     <t>ID</t>
   </si>
@@ -2465,10 +2466,13 @@
     <t>For piano hinge</t>
   </si>
   <si>
-    <t>Screw, Wood, #8 x 5/8", Truss Head</t>
-  </si>
-  <si>
     <t>https://www.amazon.com/100Pcs-Standard-Tapping-SG-TZH/dp/B09955NQ43</t>
+  </si>
+  <si>
+    <t>Screw, Wood, #8 x 3/4", Truss Head</t>
+  </si>
+  <si>
+    <t>Wood Panel, Front Center</t>
   </si>
 </sst>
 </file>
@@ -2952,10 +2956,10 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BCCEB002-6247-475F-8E59-4D3290F5D0AB}" name="Table13" displayName="Table13" ref="A1:J202" totalsRowShown="0">
-  <autoFilter ref="A1:J202" xr:uid="{BCCEB002-6247-475F-8E59-4D3290F5D0AB}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J198">
-    <sortCondition ref="A1:A198"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BCCEB002-6247-475F-8E59-4D3290F5D0AB}" name="Table13" displayName="Table13" ref="A1:J201" totalsRowShown="0">
+  <autoFilter ref="A1:J201" xr:uid="{BCCEB002-6247-475F-8E59-4D3290F5D0AB}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J197">
+    <sortCondition ref="A1:A197"/>
   </sortState>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{5013DA2C-AE55-4442-B536-8693A638A779}" name="ID"/>
@@ -8039,10 +8043,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D318B5EB-87D8-4D97-AE82-574AF33D7DA4}">
-  <dimension ref="A1:J202"/>
+  <dimension ref="A1:J201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="C100" sqref="C100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8870,16 +8874,16 @@
         <v>8</v>
       </c>
       <c r="C31" t="s">
+        <v>796</v>
+      </c>
+      <c r="D31" t="s">
+        <v>463</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G31" s="1" t="s">
         <v>795</v>
-      </c>
-      <c r="D31" t="s">
-        <v>463</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>796</v>
       </c>
       <c r="H31" t="s">
         <v>65</v>
@@ -10480,7 +10484,7 @@
         <v>137</v>
       </c>
       <c r="C94" t="s">
-        <v>581</v>
+        <v>797</v>
       </c>
       <c r="D94" t="s">
         <v>463</v>
@@ -10495,13 +10499,13 @@
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>458</v>
+        <v>502</v>
       </c>
       <c r="B95" t="s">
         <v>137</v>
       </c>
       <c r="C95" t="s">
-        <v>580</v>
+        <v>792</v>
       </c>
       <c r="D95" t="s">
         <v>463</v>
@@ -10513,40 +10517,37 @@
         <v>210</v>
       </c>
       <c r="I95" s="5"/>
+      <c r="J95" t="s">
+        <v>503</v>
+      </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>502</v>
+        <v>474</v>
       </c>
       <c r="B96" t="s">
         <v>137</v>
       </c>
       <c r="C96" t="s">
-        <v>792</v>
+        <v>547</v>
       </c>
       <c r="D96" t="s">
         <v>463</v>
-      </c>
-      <c r="F96" t="s">
-        <v>210</v>
-      </c>
-      <c r="H96" t="s">
-        <v>210</v>
       </c>
       <c r="I96" s="5"/>
       <c r="J96" t="s">
-        <v>503</v>
+        <v>481</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B97" t="s">
         <v>137</v>
       </c>
       <c r="C97" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="D97" t="s">
         <v>463</v>
@@ -10558,13 +10559,13 @@
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="B98" t="s">
         <v>137</v>
       </c>
       <c r="C98" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="D98" t="s">
         <v>463</v>
@@ -10576,31 +10577,31 @@
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="B99" t="s">
         <v>137</v>
       </c>
       <c r="C99" t="s">
-        <v>573</v>
+        <v>477</v>
       </c>
       <c r="D99" t="s">
         <v>463</v>
       </c>
       <c r="I99" s="5"/>
       <c r="J99" t="s">
-        <v>481</v>
+        <v>488</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="B100" t="s">
         <v>137</v>
       </c>
       <c r="C100" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
       <c r="D100" t="s">
         <v>463</v>
@@ -10612,13 +10613,13 @@
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>479</v>
+        <v>482</v>
       </c>
       <c r="B101" t="s">
         <v>137</v>
       </c>
       <c r="C101" t="s">
-        <v>480</v>
+        <v>486</v>
       </c>
       <c r="D101" t="s">
         <v>463</v>
@@ -10630,49 +10631,49 @@
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="B102" t="s">
         <v>137</v>
       </c>
       <c r="C102" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="D102" t="s">
         <v>463</v>
       </c>
       <c r="I102" s="5"/>
       <c r="J102" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B103" t="s">
         <v>137</v>
       </c>
       <c r="C103" t="s">
-        <v>487</v>
+        <v>548</v>
       </c>
       <c r="D103" t="s">
         <v>463</v>
       </c>
       <c r="I103" s="5"/>
       <c r="J103" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B104" t="s">
         <v>137</v>
       </c>
       <c r="C104" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="D104" t="s">
         <v>463</v>
@@ -10684,49 +10685,53 @@
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>485</v>
+        <v>505</v>
       </c>
       <c r="B105" t="s">
         <v>137</v>
       </c>
       <c r="C105" t="s">
-        <v>549</v>
+        <v>571</v>
       </c>
       <c r="D105" t="s">
         <v>463</v>
       </c>
       <c r="I105" s="5"/>
       <c r="J105" t="s">
-        <v>488</v>
+        <v>506</v>
       </c>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>505</v>
+        <v>539</v>
       </c>
       <c r="B106" t="s">
         <v>137</v>
       </c>
       <c r="C106" t="s">
-        <v>571</v>
+        <v>584</v>
       </c>
       <c r="D106" t="s">
         <v>463</v>
       </c>
+      <c r="F106" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="G106" s="6"/>
+      <c r="H106" s="6" t="s">
+        <v>210</v>
+      </c>
       <c r="I106" s="5"/>
-      <c r="J106" t="s">
-        <v>506</v>
-      </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="B107" t="s">
         <v>137</v>
       </c>
       <c r="C107" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="D107" t="s">
         <v>463</v>
@@ -10742,59 +10747,61 @@
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>540</v>
+        <v>570</v>
       </c>
       <c r="B108" t="s">
         <v>137</v>
       </c>
       <c r="C108" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="D108" t="s">
         <v>463</v>
       </c>
-      <c r="F108" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="G108" s="6"/>
+      <c r="F108" t="s">
+        <v>414</v>
+      </c>
+      <c r="G108" s="1" t="s">
+        <v>734</v>
+      </c>
       <c r="H108" s="6" t="s">
-        <v>210</v>
+        <v>65</v>
       </c>
       <c r="I108" s="5"/>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>570</v>
+        <v>222</v>
       </c>
       <c r="B109" t="s">
-        <v>137</v>
+        <v>223</v>
       </c>
       <c r="C109" t="s">
-        <v>586</v>
+        <v>224</v>
       </c>
       <c r="D109" t="s">
         <v>463</v>
       </c>
       <c r="F109" t="s">
-        <v>414</v>
+        <v>10</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>734</v>
-      </c>
-      <c r="H109" s="6" t="s">
-        <v>65</v>
+        <v>735</v>
+      </c>
+      <c r="H109" t="s">
+        <v>225</v>
       </c>
       <c r="I109" s="5"/>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="B110" t="s">
         <v>223</v>
       </c>
       <c r="C110" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="D110" t="s">
         <v>463</v>
@@ -10809,68 +10816,73 @@
         <v>225</v>
       </c>
       <c r="I110" s="5"/>
+      <c r="J110" t="s">
+        <v>550</v>
+      </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B111" t="s">
         <v>223</v>
       </c>
       <c r="C111" t="s">
-        <v>227</v>
+        <v>555</v>
       </c>
       <c r="D111" t="s">
         <v>463</v>
       </c>
-      <c r="F111" t="s">
-        <v>10</v>
-      </c>
-      <c r="G111" s="1" t="s">
-        <v>735</v>
-      </c>
+      <c r="F111" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G111" s="1"/>
       <c r="H111" t="s">
-        <v>225</v>
+        <v>65</v>
       </c>
       <c r="I111" s="5"/>
       <c r="J111" t="s">
-        <v>550</v>
+        <v>736</v>
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="B112" t="s">
         <v>223</v>
       </c>
       <c r="C112" t="s">
-        <v>555</v>
+        <v>232</v>
       </c>
       <c r="D112" t="s">
         <v>463</v>
       </c>
-      <c r="F112" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G112" s="1"/>
+      <c r="F112" t="s">
+        <v>10</v>
+      </c>
+      <c r="G112" s="1" t="s">
+        <v>682</v>
+      </c>
       <c r="H112" t="s">
-        <v>65</v>
-      </c>
-      <c r="I112" s="5"/>
+        <v>55</v>
+      </c>
+      <c r="I112" s="5" t="s">
+        <v>56</v>
+      </c>
       <c r="J112" t="s">
-        <v>736</v>
+        <v>235</v>
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B113" t="s">
         <v>223</v>
       </c>
       <c r="C113" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="D113" t="s">
         <v>463</v>
@@ -10893,13 +10905,13 @@
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="B114" t="s">
         <v>223</v>
       </c>
       <c r="C114" t="s">
-        <v>234</v>
+        <v>552</v>
       </c>
       <c r="D114" t="s">
         <v>463</v>
@@ -10908,195 +10920,193 @@
         <v>10</v>
       </c>
       <c r="G114" s="1" t="s">
-        <v>682</v>
+        <v>737</v>
       </c>
       <c r="H114" t="s">
-        <v>55</v>
+        <v>237</v>
       </c>
       <c r="I114" s="5" t="s">
-        <v>56</v>
+        <v>238</v>
       </c>
       <c r="J114" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="B115" t="s">
         <v>223</v>
       </c>
       <c r="C115" t="s">
-        <v>552</v>
+        <v>241</v>
       </c>
       <c r="D115" t="s">
         <v>463</v>
       </c>
       <c r="F115" t="s">
-        <v>10</v>
+        <v>242</v>
       </c>
       <c r="G115" s="1" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="H115" t="s">
-        <v>237</v>
-      </c>
-      <c r="I115" s="5" t="s">
-        <v>238</v>
+        <v>242</v>
+      </c>
+      <c r="I115" s="5">
+        <v>570</v>
       </c>
       <c r="J115" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="B116" t="s">
         <v>223</v>
       </c>
       <c r="C116" t="s">
-        <v>241</v>
+        <v>504</v>
       </c>
       <c r="D116" t="s">
         <v>463</v>
       </c>
       <c r="F116" t="s">
-        <v>242</v>
+        <v>10</v>
       </c>
       <c r="G116" s="1" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="H116" t="s">
-        <v>242</v>
-      </c>
-      <c r="I116" s="5">
-        <v>570</v>
-      </c>
-      <c r="J116" t="s">
-        <v>243</v>
+        <v>245</v>
+      </c>
+      <c r="I116" s="5" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="B117" t="s">
         <v>223</v>
       </c>
       <c r="C117" t="s">
-        <v>504</v>
+        <v>248</v>
       </c>
       <c r="D117" t="s">
-        <v>463</v>
+        <v>770</v>
+      </c>
+      <c r="E117">
+        <v>120</v>
       </c>
       <c r="F117" t="s">
         <v>10</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="H117" t="s">
-        <v>245</v>
-      </c>
-      <c r="I117" s="5" t="s">
-        <v>246</v>
+        <v>65</v>
+      </c>
+      <c r="I117" s="5"/>
+      <c r="J117" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B118" t="s">
         <v>223</v>
       </c>
       <c r="C118" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="D118" t="s">
-        <v>770</v>
-      </c>
-      <c r="E118">
-        <v>120</v>
+        <v>463</v>
       </c>
       <c r="F118" t="s">
         <v>10</v>
       </c>
       <c r="G118" s="1" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="H118" t="s">
         <v>65</v>
       </c>
       <c r="I118" s="5"/>
-      <c r="J118" t="s">
-        <v>472</v>
-      </c>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="B119" t="s">
         <v>223</v>
       </c>
       <c r="C119" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="D119" t="s">
-        <v>463</v>
+        <v>464</v>
+      </c>
+      <c r="E119">
+        <v>1</v>
       </c>
       <c r="F119" t="s">
         <v>10</v>
       </c>
       <c r="G119" s="1" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="H119" t="s">
         <v>65</v>
       </c>
       <c r="I119" s="5"/>
+      <c r="J119" t="s">
+        <v>255</v>
+      </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="B120" t="s">
         <v>223</v>
       </c>
       <c r="C120" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="D120" t="s">
-        <v>464</v>
-      </c>
-      <c r="E120">
-        <v>1</v>
+        <v>463</v>
       </c>
       <c r="F120" t="s">
         <v>10</v>
       </c>
       <c r="G120" s="1" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="H120" t="s">
         <v>65</v>
       </c>
       <c r="I120" s="5"/>
       <c r="J120" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="B121" t="s">
         <v>223</v>
       </c>
       <c r="C121" t="s">
-        <v>257</v>
+        <v>565</v>
       </c>
       <c r="D121" t="s">
         <v>463</v>
@@ -11105,25 +11115,22 @@
         <v>10</v>
       </c>
       <c r="G121" s="1" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="H121" t="s">
         <v>65</v>
       </c>
       <c r="I121" s="5"/>
-      <c r="J121" t="s">
-        <v>258</v>
-      </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>259</v>
+        <v>495</v>
       </c>
       <c r="B122" t="s">
         <v>223</v>
       </c>
       <c r="C122" t="s">
-        <v>565</v>
+        <v>494</v>
       </c>
       <c r="D122" t="s">
         <v>463</v>
@@ -11132,22 +11139,25 @@
         <v>10</v>
       </c>
       <c r="G122" s="1" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="H122" t="s">
         <v>65</v>
       </c>
       <c r="I122" s="5"/>
+      <c r="J122" t="s">
+        <v>496</v>
+      </c>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>495</v>
+        <v>508</v>
       </c>
       <c r="B123" t="s">
         <v>223</v>
       </c>
       <c r="C123" t="s">
-        <v>494</v>
+        <v>509</v>
       </c>
       <c r="D123" t="s">
         <v>463</v>
@@ -11156,25 +11166,25 @@
         <v>10</v>
       </c>
       <c r="G123" s="1" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="H123" t="s">
         <v>65</v>
       </c>
       <c r="I123" s="5"/>
       <c r="J123" t="s">
-        <v>496</v>
+        <v>510</v>
       </c>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>508</v>
+        <v>557</v>
       </c>
       <c r="B124" t="s">
         <v>223</v>
       </c>
       <c r="C124" t="s">
-        <v>509</v>
+        <v>560</v>
       </c>
       <c r="D124" t="s">
         <v>463</v>
@@ -11183,25 +11193,27 @@
         <v>10</v>
       </c>
       <c r="G124" s="1" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="H124" t="s">
-        <v>65</v>
-      </c>
-      <c r="I124" s="5"/>
+        <v>566</v>
+      </c>
+      <c r="I124" s="5" t="s">
+        <v>567</v>
+      </c>
       <c r="J124" t="s">
-        <v>510</v>
+        <v>561</v>
       </c>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="B125" t="s">
         <v>223</v>
       </c>
       <c r="C125" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D125" t="s">
         <v>463</v>
@@ -11210,54 +11222,54 @@
         <v>10</v>
       </c>
       <c r="G125" s="1" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="H125" t="s">
-        <v>566</v>
-      </c>
-      <c r="I125" s="5" t="s">
-        <v>567</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="I125" s="5"/>
       <c r="J125" t="s">
-        <v>561</v>
+        <v>568</v>
       </c>
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>558</v>
+        <v>260</v>
       </c>
       <c r="B126" t="s">
-        <v>223</v>
+        <v>261</v>
       </c>
       <c r="C126" t="s">
-        <v>559</v>
+        <v>262</v>
       </c>
       <c r="D126" t="s">
         <v>463</v>
       </c>
       <c r="F126" t="s">
-        <v>10</v>
+        <v>263</v>
       </c>
       <c r="G126" s="1" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="H126" t="s">
-        <v>65</v>
-      </c>
-      <c r="I126" s="5"/>
+        <v>264</v>
+      </c>
+      <c r="I126" s="5" t="s">
+        <v>265</v>
+      </c>
       <c r="J126" t="s">
-        <v>568</v>
+        <v>266</v>
       </c>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>260</v>
+        <v>267</v>
       </c>
       <c r="B127" t="s">
         <v>261</v>
       </c>
       <c r="C127" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="D127" t="s">
         <v>463</v>
@@ -11266,27 +11278,27 @@
         <v>263</v>
       </c>
       <c r="G127" s="1" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="H127" t="s">
         <v>264</v>
       </c>
       <c r="I127" s="5" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="J127" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="B128" t="s">
         <v>261</v>
       </c>
       <c r="C128" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="D128" t="s">
         <v>463</v>
@@ -11295,82 +11307,82 @@
         <v>263</v>
       </c>
       <c r="G128" s="1" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="H128" t="s">
         <v>264</v>
       </c>
       <c r="I128" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="J128" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="B129" t="s">
         <v>261</v>
       </c>
       <c r="C129" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="D129" t="s">
         <v>463</v>
       </c>
       <c r="F129" t="s">
-        <v>263</v>
+        <v>10</v>
       </c>
       <c r="G129" s="1" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="H129" t="s">
-        <v>264</v>
+        <v>237</v>
       </c>
       <c r="I129" s="5" t="s">
-        <v>273</v>
+        <v>276</v>
+      </c>
+      <c r="J129" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="B130" t="s">
         <v>261</v>
       </c>
       <c r="C130" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="D130" t="s">
         <v>463</v>
       </c>
       <c r="F130" t="s">
-        <v>10</v>
+        <v>280</v>
       </c>
       <c r="G130" s="1" t="s">
-        <v>752</v>
-      </c>
-      <c r="H130" t="s">
-        <v>237</v>
-      </c>
-      <c r="I130" s="5" t="s">
-        <v>276</v>
+        <v>753</v>
+      </c>
+      <c r="H130" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="I130" s="10" t="s">
+        <v>282</v>
       </c>
       <c r="J130" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="B131" t="s">
         <v>261</v>
       </c>
       <c r="C131" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="D131" t="s">
         <v>463</v>
@@ -11379,27 +11391,24 @@
         <v>280</v>
       </c>
       <c r="G131" s="1" t="s">
-        <v>753</v>
-      </c>
-      <c r="H131" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="I131" s="10" t="s">
-        <v>282</v>
-      </c>
-      <c r="J131" t="s">
-        <v>283</v>
+        <v>754</v>
+      </c>
+      <c r="H131" t="s">
+        <v>286</v>
+      </c>
+      <c r="I131" s="5" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="B132" t="s">
         <v>261</v>
       </c>
       <c r="C132" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="D132" t="s">
         <v>463</v>
@@ -11408,56 +11417,60 @@
         <v>280</v>
       </c>
       <c r="G132" s="1" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="H132" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="I132" s="5" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="B133" t="s">
         <v>261</v>
       </c>
       <c r="C133" t="s">
-        <v>289</v>
+        <v>417</v>
       </c>
       <c r="D133" t="s">
-        <v>463</v>
+        <v>770</v>
+      </c>
+      <c r="E133">
+        <v>200</v>
       </c>
       <c r="F133" t="s">
-        <v>280</v>
+        <v>10</v>
       </c>
       <c r="G133" s="1" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="H133" t="s">
-        <v>290</v>
-      </c>
-      <c r="I133" s="5" t="s">
-        <v>291</v>
+        <v>65</v>
+      </c>
+      <c r="I133" s="5"/>
+      <c r="J133" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B134" t="s">
         <v>261</v>
       </c>
       <c r="C134" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D134" t="s">
         <v>770</v>
       </c>
       <c r="E134">
-        <v>200</v>
+        <v>120</v>
       </c>
       <c r="F134" t="s">
         <v>10</v>
@@ -11470,48 +11483,45 @@
       </c>
       <c r="I134" s="5"/>
       <c r="J134" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="B135" t="s">
         <v>261</v>
       </c>
       <c r="C135" t="s">
-        <v>416</v>
+        <v>297</v>
       </c>
       <c r="D135" t="s">
         <v>770</v>
       </c>
-      <c r="E135">
-        <v>120</v>
-      </c>
       <c r="F135" t="s">
         <v>10</v>
       </c>
       <c r="G135" s="1" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="H135" t="s">
         <v>65</v>
       </c>
       <c r="I135" s="5"/>
       <c r="J135" t="s">
-        <v>418</v>
+        <v>471</v>
       </c>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="B136" t="s">
         <v>261</v>
       </c>
       <c r="C136" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="D136" t="s">
         <v>770</v>
@@ -11520,25 +11530,25 @@
         <v>10</v>
       </c>
       <c r="G136" s="1" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="H136" t="s">
         <v>65</v>
       </c>
       <c r="I136" s="5"/>
-      <c r="J136" t="s">
-        <v>471</v>
+      <c r="J136" s="4" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="B137" t="s">
         <v>261</v>
       </c>
       <c r="C137" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="D137" t="s">
         <v>770</v>
@@ -11547,52 +11557,51 @@
         <v>10</v>
       </c>
       <c r="G137" s="1" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="H137" t="s">
         <v>65</v>
       </c>
       <c r="I137" s="5"/>
-      <c r="J137" s="4" t="s">
-        <v>470</v>
+      <c r="J137" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B138" t="s">
         <v>261</v>
       </c>
       <c r="C138" t="s">
-        <v>294</v>
+        <v>302</v>
       </c>
       <c r="D138" t="s">
-        <v>770</v>
+        <v>463</v>
       </c>
       <c r="F138" t="s">
-        <v>10</v>
+        <v>280</v>
       </c>
       <c r="G138" s="1" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="H138" t="s">
-        <v>65</v>
-      </c>
-      <c r="I138" s="5"/>
-      <c r="J138" t="s">
-        <v>295</v>
+        <v>303</v>
+      </c>
+      <c r="I138" s="8" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="B139" t="s">
         <v>261</v>
       </c>
       <c r="C139" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="D139" t="s">
         <v>463</v>
@@ -11601,24 +11610,24 @@
         <v>280</v>
       </c>
       <c r="G139" s="1" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="H139" t="s">
         <v>303</v>
       </c>
       <c r="I139" s="8" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="B140" t="s">
         <v>261</v>
       </c>
       <c r="C140" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="D140" t="s">
         <v>463</v>
@@ -11627,24 +11636,24 @@
         <v>280</v>
       </c>
       <c r="G140" s="1" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="H140" t="s">
         <v>303</v>
       </c>
-      <c r="I140" s="8" t="s">
-        <v>307</v>
+      <c r="I140" s="5" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="B141" t="s">
         <v>261</v>
       </c>
       <c r="C141" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="D141" t="s">
         <v>463</v>
@@ -11653,24 +11662,24 @@
         <v>280</v>
       </c>
       <c r="G141" s="1" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="H141" t="s">
         <v>303</v>
       </c>
       <c r="I141" s="5" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="B142" t="s">
         <v>261</v>
       </c>
       <c r="C142" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="D142" t="s">
         <v>463</v>
@@ -11679,24 +11688,24 @@
         <v>280</v>
       </c>
       <c r="G142" s="1" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="H142" t="s">
         <v>303</v>
       </c>
       <c r="I142" s="5" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="B143" t="s">
         <v>261</v>
       </c>
       <c r="C143" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="D143" t="s">
         <v>463</v>
@@ -11705,24 +11714,24 @@
         <v>280</v>
       </c>
       <c r="G143" s="1" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="H143" t="s">
         <v>303</v>
       </c>
       <c r="I143" s="5" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="B144" t="s">
         <v>261</v>
       </c>
       <c r="C144" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="D144" t="s">
         <v>463</v>
@@ -11731,24 +11740,24 @@
         <v>280</v>
       </c>
       <c r="G144" s="1" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="H144" t="s">
         <v>303</v>
       </c>
       <c r="I144" s="5" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="B145" t="s">
         <v>261</v>
       </c>
       <c r="C145" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="D145" t="s">
         <v>463</v>
@@ -11757,24 +11766,24 @@
         <v>280</v>
       </c>
       <c r="G145" s="1" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="H145" t="s">
         <v>303</v>
       </c>
       <c r="I145" s="5" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="B146" t="s">
         <v>261</v>
       </c>
       <c r="C146" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="D146" t="s">
         <v>463</v>
@@ -11783,79 +11792,79 @@
         <v>280</v>
       </c>
       <c r="G146" s="1" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="H146" t="s">
         <v>303</v>
       </c>
       <c r="I146" s="5" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="B147" t="s">
         <v>261</v>
       </c>
       <c r="C147" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="D147" t="s">
         <v>463</v>
       </c>
       <c r="F147" t="s">
-        <v>280</v>
+        <v>139</v>
       </c>
       <c r="G147" s="1" t="s">
-        <v>768</v>
+        <v>664</v>
       </c>
       <c r="H147" t="s">
         <v>303</v>
       </c>
       <c r="I147" s="5" t="s">
-        <v>328</v>
+        <v>331</v>
+      </c>
+      <c r="J147" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="B148" t="s">
         <v>261</v>
       </c>
       <c r="C148" t="s">
-        <v>330</v>
+        <v>426</v>
       </c>
       <c r="D148" t="s">
         <v>463</v>
       </c>
       <c r="F148" t="s">
-        <v>139</v>
+        <v>280</v>
       </c>
       <c r="G148" s="1" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="H148" t="s">
         <v>303</v>
       </c>
       <c r="I148" s="5" t="s">
-        <v>331</v>
-      </c>
-      <c r="J148" t="s">
-        <v>332</v>
+        <v>432</v>
       </c>
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B149" t="s">
         <v>261</v>
       </c>
       <c r="C149" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="D149" t="s">
         <v>463</v>
@@ -11863,25 +11872,25 @@
       <c r="F149" t="s">
         <v>280</v>
       </c>
-      <c r="G149" s="1" t="s">
-        <v>665</v>
+      <c r="G149" s="3" t="s">
+        <v>666</v>
       </c>
       <c r="H149" t="s">
         <v>303</v>
       </c>
       <c r="I149" s="5" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B150" t="s">
         <v>261</v>
       </c>
       <c r="C150" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="D150" t="s">
         <v>463</v>
@@ -11889,25 +11898,25 @@
       <c r="F150" t="s">
         <v>280</v>
       </c>
-      <c r="G150" s="3" t="s">
-        <v>666</v>
+      <c r="G150" s="1" t="s">
+        <v>667</v>
       </c>
       <c r="H150" t="s">
         <v>303</v>
       </c>
       <c r="I150" s="5" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>335</v>
+        <v>420</v>
       </c>
       <c r="B151" t="s">
         <v>261</v>
       </c>
       <c r="C151" t="s">
-        <v>428</v>
+        <v>467</v>
       </c>
       <c r="D151" t="s">
         <v>463</v>
@@ -11915,25 +11924,28 @@
       <c r="F151" t="s">
         <v>280</v>
       </c>
-      <c r="G151" s="1" t="s">
-        <v>667</v>
+      <c r="G151" s="3" t="s">
+        <v>668</v>
       </c>
       <c r="H151" t="s">
         <v>303</v>
       </c>
       <c r="I151" s="5" t="s">
-        <v>431</v>
+        <v>424</v>
+      </c>
+      <c r="J151" t="s">
+        <v>469</v>
       </c>
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B152" t="s">
         <v>261</v>
       </c>
       <c r="C152" t="s">
-        <v>467</v>
+        <v>677</v>
       </c>
       <c r="D152" t="s">
         <v>463</v>
@@ -11941,14 +11953,14 @@
       <c r="F152" t="s">
         <v>280</v>
       </c>
-      <c r="G152" s="3" t="s">
+      <c r="G152" s="1" t="s">
         <v>668</v>
       </c>
       <c r="H152" t="s">
         <v>303</v>
       </c>
       <c r="I152" s="5" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="J152" t="s">
         <v>469</v>
@@ -11956,13 +11968,13 @@
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="B153" t="s">
         <v>261</v>
       </c>
       <c r="C153" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="D153" t="s">
         <v>463</v>
@@ -11971,53 +11983,50 @@
         <v>280</v>
       </c>
       <c r="G153" s="1" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="H153" t="s">
         <v>303</v>
       </c>
-      <c r="I153" s="5" t="s">
-        <v>425</v>
-      </c>
-      <c r="J153" t="s">
-        <v>469</v>
+      <c r="I153" s="10" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>422</v>
+        <v>336</v>
       </c>
       <c r="B154" t="s">
         <v>261</v>
       </c>
       <c r="C154" t="s">
-        <v>676</v>
+        <v>337</v>
       </c>
       <c r="D154" t="s">
         <v>463</v>
       </c>
       <c r="F154" t="s">
-        <v>280</v>
+        <v>10</v>
       </c>
       <c r="G154" s="1" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="H154" t="s">
-        <v>303</v>
-      </c>
-      <c r="I154" s="10" t="s">
-        <v>429</v>
+        <v>338</v>
+      </c>
+      <c r="I154" s="5" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="B155" t="s">
         <v>261</v>
       </c>
       <c r="C155" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="D155" t="s">
         <v>463</v>
@@ -12026,24 +12035,22 @@
         <v>10</v>
       </c>
       <c r="G155" s="1" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="H155" t="s">
-        <v>338</v>
-      </c>
-      <c r="I155" s="5" t="s">
-        <v>339</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="I155" s="5"/>
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="B156" t="s">
         <v>261</v>
       </c>
       <c r="C156" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="D156" t="s">
         <v>463</v>
@@ -12052,22 +12059,24 @@
         <v>10</v>
       </c>
       <c r="G156" s="1" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="H156" t="s">
-        <v>65</v>
-      </c>
-      <c r="I156" s="5"/>
+        <v>344</v>
+      </c>
+      <c r="I156" s="5" t="s">
+        <v>345</v>
+      </c>
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="B157" t="s">
         <v>261</v>
       </c>
       <c r="C157" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="D157" t="s">
         <v>463</v>
@@ -12076,24 +12085,25 @@
         <v>10</v>
       </c>
       <c r="G157" s="1" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="H157" t="s">
-        <v>344</v>
-      </c>
-      <c r="I157" s="5" t="s">
-        <v>345</v>
+        <v>348</v>
+      </c>
+      <c r="I157" s="5"/>
+      <c r="J157" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="B158" t="s">
         <v>261</v>
       </c>
       <c r="C158" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="D158" t="s">
         <v>463</v>
@@ -12102,25 +12112,22 @@
         <v>10</v>
       </c>
       <c r="G158" s="1" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="H158" t="s">
-        <v>348</v>
+        <v>65</v>
       </c>
       <c r="I158" s="5"/>
-      <c r="J158" t="s">
-        <v>349</v>
-      </c>
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="B159" t="s">
         <v>261</v>
       </c>
       <c r="C159" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="D159" t="s">
         <v>463</v>
@@ -12129,7 +12136,7 @@
         <v>10</v>
       </c>
       <c r="G159" s="1" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="H159" t="s">
         <v>65</v>
@@ -12138,13 +12145,13 @@
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="B160" t="s">
         <v>261</v>
       </c>
       <c r="C160" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="D160" t="s">
         <v>463</v>
@@ -12153,22 +12160,25 @@
         <v>10</v>
       </c>
       <c r="G160" s="1" t="s">
-        <v>675</v>
+        <v>663</v>
       </c>
       <c r="H160" t="s">
         <v>65</v>
       </c>
       <c r="I160" s="5"/>
+      <c r="J160" t="s">
+        <v>356</v>
+      </c>
     </row>
     <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="B161" t="s">
         <v>261</v>
       </c>
       <c r="C161" t="s">
-        <v>355</v>
+        <v>554</v>
       </c>
       <c r="D161" t="s">
         <v>463</v>
@@ -12177,110 +12187,110 @@
         <v>10</v>
       </c>
       <c r="G161" s="1" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="H161" t="s">
-        <v>65</v>
-      </c>
-      <c r="I161" s="5"/>
+        <v>358</v>
+      </c>
+      <c r="I161" s="5" t="s">
+        <v>359</v>
+      </c>
       <c r="J161" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
     </row>
     <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="B162" t="s">
         <v>261</v>
       </c>
       <c r="C162" t="s">
-        <v>554</v>
+        <v>362</v>
       </c>
       <c r="D162" t="s">
         <v>463</v>
       </c>
       <c r="F162" t="s">
-        <v>10</v>
+        <v>139</v>
       </c>
       <c r="G162" s="1" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="H162" t="s">
-        <v>358</v>
+        <v>36</v>
       </c>
       <c r="I162" s="5" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="J162" t="s">
-        <v>360</v>
+        <v>790</v>
       </c>
     </row>
     <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="B163" t="s">
         <v>261</v>
       </c>
       <c r="C163" t="s">
-        <v>362</v>
+        <v>507</v>
       </c>
       <c r="D163" t="s">
         <v>463</v>
       </c>
       <c r="F163" t="s">
-        <v>139</v>
+        <v>10</v>
       </c>
       <c r="G163" s="1" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="H163" t="s">
-        <v>36</v>
-      </c>
-      <c r="I163" s="5" t="s">
-        <v>363</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="I163" s="5"/>
       <c r="J163" t="s">
-        <v>790</v>
+        <v>366</v>
       </c>
     </row>
     <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>365</v>
+        <v>545</v>
       </c>
       <c r="B164" t="s">
         <v>261</v>
       </c>
       <c r="C164" t="s">
-        <v>507</v>
+        <v>546</v>
       </c>
       <c r="D164" t="s">
         <v>463</v>
       </c>
-      <c r="F164" t="s">
+      <c r="E164">
+        <v>1</v>
+      </c>
+      <c r="F164" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G164" s="1" t="s">
-        <v>660</v>
+        <v>789</v>
       </c>
       <c r="H164" t="s">
         <v>65</v>
       </c>
       <c r="I164" s="5"/>
-      <c r="J164" t="s">
-        <v>366</v>
-      </c>
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>545</v>
+        <v>612</v>
       </c>
       <c r="B165" t="s">
         <v>261</v>
       </c>
       <c r="C165" t="s">
-        <v>546</v>
+        <v>613</v>
       </c>
       <c r="D165" t="s">
         <v>463</v>
@@ -12288,11 +12298,11 @@
       <c r="E165">
         <v>1</v>
       </c>
-      <c r="F165" s="6" t="s">
+      <c r="F165" t="s">
         <v>10</v>
       </c>
       <c r="G165" s="1" t="s">
-        <v>789</v>
+        <v>659</v>
       </c>
       <c r="H165" t="s">
         <v>65</v>
@@ -12301,16 +12311,16 @@
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c r="B166" t="s">
         <v>261</v>
       </c>
       <c r="C166" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
       <c r="D166" t="s">
-        <v>463</v>
+        <v>535</v>
       </c>
       <c r="E166">
         <v>1</v>
@@ -12319,7 +12329,7 @@
         <v>10</v>
       </c>
       <c r="G166" s="1" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="H166" t="s">
         <v>65</v>
@@ -12328,40 +12338,40 @@
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>614</v>
+        <v>367</v>
       </c>
       <c r="B167" t="s">
         <v>261</v>
       </c>
       <c r="C167" t="s">
-        <v>615</v>
+        <v>368</v>
       </c>
       <c r="D167" t="s">
-        <v>535</v>
-      </c>
-      <c r="E167">
-        <v>1</v>
+        <v>463</v>
       </c>
       <c r="F167" t="s">
         <v>10</v>
       </c>
       <c r="G167" s="1" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="H167" t="s">
         <v>65</v>
       </c>
       <c r="I167" s="5"/>
+      <c r="J167" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="B168" t="s">
         <v>261</v>
       </c>
       <c r="C168" t="s">
-        <v>368</v>
+        <v>599</v>
       </c>
       <c r="D168" t="s">
         <v>463</v>
@@ -12370,25 +12380,22 @@
         <v>10</v>
       </c>
       <c r="G168" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="H168" t="s">
         <v>65</v>
       </c>
       <c r="I168" s="5"/>
-      <c r="J168" t="s">
-        <v>369</v>
-      </c>
     </row>
     <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B169" t="s">
         <v>261</v>
       </c>
       <c r="C169" t="s">
-        <v>599</v>
+        <v>435</v>
       </c>
       <c r="D169" t="s">
         <v>463</v>
@@ -12397,12 +12404,15 @@
         <v>10</v>
       </c>
       <c r="G169" s="1" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="H169" t="s">
         <v>65</v>
       </c>
       <c r="I169" s="5"/>
+      <c r="J169" t="s">
+        <v>436</v>
+      </c>
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
@@ -12412,7 +12422,7 @@
         <v>261</v>
       </c>
       <c r="C170" t="s">
-        <v>435</v>
+        <v>598</v>
       </c>
       <c r="D170" t="s">
         <v>463</v>
@@ -12421,25 +12431,24 @@
         <v>10</v>
       </c>
       <c r="G170" s="1" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="H170" t="s">
-        <v>65</v>
-      </c>
-      <c r="I170" s="5"/>
-      <c r="J170" t="s">
-        <v>436</v>
+        <v>115</v>
+      </c>
+      <c r="I170" s="5" t="s">
+        <v>437</v>
       </c>
     </row>
     <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B171" t="s">
         <v>261</v>
       </c>
       <c r="C171" t="s">
-        <v>598</v>
+        <v>452</v>
       </c>
       <c r="D171" t="s">
         <v>463</v>
@@ -12448,24 +12457,24 @@
         <v>10</v>
       </c>
       <c r="G171" s="1" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="H171" t="s">
-        <v>115</v>
+        <v>225</v>
       </c>
       <c r="I171" s="5" t="s">
-        <v>437</v>
+        <v>373</v>
       </c>
     </row>
     <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="B172" t="s">
         <v>261</v>
       </c>
       <c r="C172" t="s">
-        <v>452</v>
+        <v>375</v>
       </c>
       <c r="D172" t="s">
         <v>463</v>
@@ -12474,24 +12483,24 @@
         <v>10</v>
       </c>
       <c r="G172" s="1" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="H172" t="s">
         <v>225</v>
       </c>
       <c r="I172" s="5" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
     </row>
     <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="B173" t="s">
         <v>261</v>
       </c>
       <c r="C173" t="s">
-        <v>375</v>
+        <v>451</v>
       </c>
       <c r="D173" t="s">
         <v>463</v>
@@ -12500,76 +12509,76 @@
         <v>10</v>
       </c>
       <c r="G173" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="H173" t="s">
         <v>225</v>
       </c>
       <c r="I173" s="5" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
     </row>
     <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="B174" t="s">
         <v>261</v>
       </c>
       <c r="C174" t="s">
-        <v>451</v>
+        <v>380</v>
       </c>
       <c r="D174" t="s">
         <v>463</v>
       </c>
       <c r="F174" t="s">
-        <v>10</v>
+        <v>280</v>
       </c>
       <c r="G174" s="1" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="H174" t="s">
-        <v>225</v>
+        <v>381</v>
       </c>
       <c r="I174" s="5" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
     </row>
     <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
       <c r="B175" t="s">
         <v>261</v>
       </c>
       <c r="C175" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="D175" t="s">
         <v>463</v>
       </c>
       <c r="F175" t="s">
-        <v>280</v>
+        <v>10</v>
       </c>
       <c r="G175" s="1" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="H175" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="I175" s="5" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
     </row>
     <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="B176" t="s">
         <v>261</v>
       </c>
       <c r="C176" t="s">
-        <v>384</v>
+        <v>434</v>
       </c>
       <c r="D176" t="s">
         <v>463</v>
@@ -12578,24 +12587,24 @@
         <v>10</v>
       </c>
       <c r="G176" s="1" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="H176" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="I176" s="5" t="s">
-        <v>386</v>
+        <v>433</v>
       </c>
     </row>
     <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>387</v>
+        <v>562</v>
       </c>
       <c r="B177" t="s">
         <v>261</v>
       </c>
       <c r="C177" t="s">
-        <v>434</v>
+        <v>563</v>
       </c>
       <c r="D177" t="s">
         <v>463</v>
@@ -12604,51 +12613,54 @@
         <v>10</v>
       </c>
       <c r="G177" s="1" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="H177" t="s">
-        <v>388</v>
-      </c>
-      <c r="I177" s="5" t="s">
-        <v>433</v>
+        <v>65</v>
+      </c>
+      <c r="I177" s="5"/>
+      <c r="J177" t="s">
+        <v>564</v>
       </c>
     </row>
     <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>562</v>
+        <v>513</v>
       </c>
       <c r="B178" t="s">
-        <v>261</v>
+        <v>438</v>
       </c>
       <c r="C178" t="s">
-        <v>563</v>
+        <v>461</v>
       </c>
       <c r="D178" t="s">
         <v>463</v>
       </c>
+      <c r="E178">
+        <v>1</v>
+      </c>
       <c r="F178" t="s">
         <v>10</v>
       </c>
       <c r="G178" s="1" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="H178" t="s">
-        <v>65</v>
-      </c>
-      <c r="I178" s="5"/>
-      <c r="J178" t="s">
-        <v>564</v>
+        <v>454</v>
+      </c>
+      <c r="I178" s="5">
+        <v>92003</v>
       </c>
     </row>
     <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="B179" t="s">
         <v>438</v>
       </c>
       <c r="C179" t="s">
-        <v>461</v>
+        <v>439</v>
       </c>
       <c r="D179" t="s">
         <v>463</v>
@@ -12657,57 +12669,55 @@
         <v>1</v>
       </c>
       <c r="F179" t="s">
-        <v>10</v>
-      </c>
-      <c r="G179" s="1" t="s">
-        <v>645</v>
+        <v>210</v>
       </c>
       <c r="H179" t="s">
-        <v>454</v>
-      </c>
-      <c r="I179" s="5">
-        <v>92003</v>
+        <v>65</v>
+      </c>
+      <c r="I179" s="5"/>
+      <c r="J179" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="B180" t="s">
         <v>438</v>
       </c>
       <c r="C180" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="D180" t="s">
-        <v>463</v>
+        <v>771</v>
       </c>
       <c r="E180">
         <v>1</v>
       </c>
       <c r="F180" t="s">
-        <v>210</v>
+        <v>10</v>
+      </c>
+      <c r="G180" t="s">
+        <v>776</v>
       </c>
       <c r="H180" t="s">
         <v>65</v>
       </c>
       <c r="I180" s="5"/>
-      <c r="J180" t="s">
-        <v>453</v>
-      </c>
     </row>
     <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="B181" t="s">
         <v>438</v>
       </c>
       <c r="C181" t="s">
-        <v>440</v>
+        <v>777</v>
       </c>
       <c r="D181" t="s">
-        <v>771</v>
+        <v>463</v>
       </c>
       <c r="E181">
         <v>1</v>
@@ -12715,8 +12725,8 @@
       <c r="F181" t="s">
         <v>10</v>
       </c>
-      <c r="G181" t="s">
-        <v>776</v>
+      <c r="G181" s="1" t="s">
+        <v>778</v>
       </c>
       <c r="H181" t="s">
         <v>65</v>
@@ -12725,13 +12735,13 @@
     </row>
     <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="B182" t="s">
         <v>438</v>
       </c>
       <c r="C182" t="s">
-        <v>777</v>
+        <v>442</v>
       </c>
       <c r="D182" t="s">
         <v>463</v>
@@ -12739,12 +12749,6 @@
       <c r="E182">
         <v>1</v>
       </c>
-      <c r="F182" t="s">
-        <v>10</v>
-      </c>
-      <c r="G182" s="1" t="s">
-        <v>778</v>
-      </c>
       <c r="H182" t="s">
         <v>65</v>
       </c>
@@ -12752,13 +12756,13 @@
     </row>
     <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="B183" t="s">
         <v>438</v>
       </c>
       <c r="C183" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="D183" t="s">
         <v>463</v>
@@ -12773,13 +12777,13 @@
     </row>
     <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="B184" t="s">
         <v>438</v>
       </c>
       <c r="C184" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
       <c r="D184" t="s">
         <v>463</v>
@@ -12787,20 +12791,29 @@
       <c r="E184">
         <v>1</v>
       </c>
+      <c r="F184" t="s">
+        <v>10</v>
+      </c>
+      <c r="G184" t="s">
+        <v>787</v>
+      </c>
       <c r="H184" t="s">
         <v>65</v>
       </c>
       <c r="I184" s="5"/>
+      <c r="J184" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="B185" t="s">
         <v>438</v>
       </c>
       <c r="C185" t="s">
-        <v>447</v>
+        <v>521</v>
       </c>
       <c r="D185" t="s">
         <v>463</v>
@@ -12808,29 +12821,17 @@
       <c r="E185">
         <v>1</v>
       </c>
-      <c r="F185" t="s">
-        <v>10</v>
-      </c>
-      <c r="G185" t="s">
-        <v>787</v>
-      </c>
-      <c r="H185" t="s">
-        <v>65</v>
-      </c>
       <c r="I185" s="5"/>
-      <c r="J185" t="s">
-        <v>788</v>
-      </c>
     </row>
     <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="B186" t="s">
         <v>438</v>
       </c>
       <c r="C186" t="s">
-        <v>521</v>
+        <v>786</v>
       </c>
       <c r="D186" t="s">
         <v>463</v>
@@ -12838,17 +12839,28 @@
       <c r="E186">
         <v>1</v>
       </c>
-      <c r="I186" s="5"/>
+      <c r="F186" t="s">
+        <v>10</v>
+      </c>
+      <c r="G186" t="s">
+        <v>783</v>
+      </c>
+      <c r="H186" t="s">
+        <v>784</v>
+      </c>
+      <c r="I186" s="5" t="s">
+        <v>785</v>
+      </c>
     </row>
     <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="B187" t="s">
         <v>438</v>
       </c>
       <c r="C187" t="s">
-        <v>786</v>
+        <v>445</v>
       </c>
       <c r="D187" t="s">
         <v>463</v>
@@ -12856,28 +12868,17 @@
       <c r="E187">
         <v>1</v>
       </c>
-      <c r="F187" t="s">
-        <v>10</v>
-      </c>
-      <c r="G187" t="s">
-        <v>783</v>
-      </c>
-      <c r="H187" t="s">
-        <v>784</v>
-      </c>
-      <c r="I187" s="5" t="s">
-        <v>785</v>
-      </c>
+      <c r="I187" s="5"/>
     </row>
     <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="B188" t="s">
         <v>438</v>
       </c>
       <c r="C188" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="D188" t="s">
         <v>463</v>
@@ -12885,17 +12886,28 @@
       <c r="E188">
         <v>1</v>
       </c>
-      <c r="I188" s="5"/>
+      <c r="F188" t="s">
+        <v>10</v>
+      </c>
+      <c r="G188" t="s">
+        <v>779</v>
+      </c>
+      <c r="H188" t="s">
+        <v>780</v>
+      </c>
+      <c r="I188" s="5" t="s">
+        <v>781</v>
+      </c>
     </row>
     <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="B189" t="s">
         <v>438</v>
       </c>
       <c r="C189" t="s">
-        <v>446</v>
+        <v>772</v>
       </c>
       <c r="D189" t="s">
         <v>463</v>
@@ -12903,49 +12915,38 @@
       <c r="E189">
         <v>1</v>
       </c>
-      <c r="F189" t="s">
-        <v>10</v>
-      </c>
-      <c r="G189" t="s">
-        <v>779</v>
-      </c>
-      <c r="H189" t="s">
-        <v>780</v>
-      </c>
-      <c r="I189" s="5" t="s">
-        <v>781</v>
+      <c r="I189" s="5"/>
+      <c r="J189" t="s">
+        <v>773</v>
       </c>
     </row>
     <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
       <c r="B190" t="s">
         <v>438</v>
       </c>
       <c r="C190" t="s">
-        <v>772</v>
+        <v>529</v>
       </c>
       <c r="D190" t="s">
-        <v>463</v>
+        <v>771</v>
       </c>
       <c r="E190">
         <v>1</v>
       </c>
       <c r="I190" s="5"/>
-      <c r="J190" t="s">
-        <v>773</v>
-      </c>
     </row>
     <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="B191" t="s">
         <v>438</v>
       </c>
       <c r="C191" t="s">
-        <v>529</v>
+        <v>532</v>
       </c>
       <c r="D191" t="s">
         <v>771</v>
@@ -12957,13 +12958,13 @@
     </row>
     <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="B192" t="s">
         <v>438</v>
       </c>
       <c r="C192" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="D192" t="s">
         <v>771</v>
@@ -12975,31 +12976,42 @@
     </row>
     <row r="193" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>531</v>
+        <v>541</v>
       </c>
       <c r="B193" t="s">
         <v>438</v>
       </c>
       <c r="C193" t="s">
-        <v>533</v>
+        <v>774</v>
       </c>
       <c r="D193" t="s">
-        <v>771</v>
+        <v>463</v>
       </c>
       <c r="E193">
         <v>1</v>
       </c>
-      <c r="I193" s="5"/>
+      <c r="F193" t="s">
+        <v>10</v>
+      </c>
+      <c r="G193" t="s">
+        <v>775</v>
+      </c>
+      <c r="H193" t="s">
+        <v>542</v>
+      </c>
+      <c r="I193" s="5" t="s">
+        <v>543</v>
+      </c>
     </row>
     <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>541</v>
+        <v>551</v>
       </c>
       <c r="B194" t="s">
         <v>438</v>
       </c>
       <c r="C194" t="s">
-        <v>774</v>
+        <v>229</v>
       </c>
       <c r="D194" t="s">
         <v>463</v>
@@ -13010,28 +13022,26 @@
       <c r="F194" t="s">
         <v>10</v>
       </c>
-      <c r="G194" t="s">
-        <v>775</v>
+      <c r="G194" s="1" t="s">
+        <v>648</v>
       </c>
       <c r="H194" t="s">
-        <v>542</v>
-      </c>
-      <c r="I194" s="5" t="s">
-        <v>543</v>
-      </c>
+        <v>230</v>
+      </c>
+      <c r="I194" s="5"/>
     </row>
     <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="B195" t="s">
-        <v>438</v>
+        <v>223</v>
       </c>
       <c r="C195" t="s">
-        <v>229</v>
+        <v>251</v>
       </c>
       <c r="D195" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="E195">
         <v>1</v>
@@ -13040,70 +13050,73 @@
         <v>10</v>
       </c>
       <c r="G195" s="1" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="H195" t="s">
-        <v>230</v>
+        <v>252</v>
       </c>
       <c r="I195" s="5"/>
+      <c r="J195" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="196" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>553</v>
+        <v>527</v>
       </c>
       <c r="B196" t="s">
-        <v>223</v>
+        <v>438</v>
       </c>
       <c r="C196" t="s">
-        <v>251</v>
+        <v>450</v>
       </c>
       <c r="D196" t="s">
-        <v>465</v>
+        <v>535</v>
       </c>
       <c r="E196">
         <v>1</v>
       </c>
-      <c r="F196" t="s">
-        <v>10</v>
-      </c>
-      <c r="G196" s="1" t="s">
-        <v>649</v>
-      </c>
-      <c r="H196" t="s">
-        <v>252</v>
-      </c>
       <c r="I196" s="5"/>
-      <c r="J196" t="s">
-        <v>473</v>
-      </c>
     </row>
     <row r="197" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>527</v>
+        <v>534</v>
       </c>
       <c r="B197" t="s">
         <v>438</v>
       </c>
       <c r="C197" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D197" t="s">
-        <v>535</v>
+        <v>463</v>
       </c>
       <c r="E197">
         <v>1</v>
       </c>
+      <c r="F197" t="s">
+        <v>10</v>
+      </c>
+      <c r="G197" t="s">
+        <v>782</v>
+      </c>
+      <c r="H197" t="s">
+        <v>65</v>
+      </c>
       <c r="I197" s="5"/>
+      <c r="J197" t="s">
+        <v>449</v>
+      </c>
     </row>
     <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>534</v>
+        <v>606</v>
       </c>
       <c r="B198" t="s">
         <v>438</v>
       </c>
       <c r="C198" t="s">
-        <v>448</v>
+        <v>607</v>
       </c>
       <c r="D198" t="s">
         <v>463</v>
@@ -13112,55 +13125,46 @@
         <v>1</v>
       </c>
       <c r="F198" t="s">
-        <v>10</v>
-      </c>
-      <c r="G198" t="s">
-        <v>782</v>
+        <v>210</v>
       </c>
       <c r="H198" t="s">
         <v>65</v>
       </c>
       <c r="I198" s="5"/>
       <c r="J198" t="s">
-        <v>449</v>
+        <v>608</v>
       </c>
     </row>
     <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>606</v>
+        <v>609</v>
       </c>
       <c r="B199" t="s">
         <v>438</v>
       </c>
       <c r="C199" t="s">
-        <v>607</v>
+        <v>610</v>
       </c>
       <c r="D199" t="s">
-        <v>463</v>
+        <v>771</v>
       </c>
       <c r="E199">
         <v>1</v>
       </c>
-      <c r="F199" t="s">
-        <v>210</v>
-      </c>
-      <c r="H199" t="s">
-        <v>65</v>
-      </c>
       <c r="I199" s="5"/>
       <c r="J199" t="s">
-        <v>608</v>
+        <v>611</v>
       </c>
     </row>
     <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>609</v>
+        <v>616</v>
       </c>
       <c r="B200" t="s">
         <v>438</v>
       </c>
       <c r="C200" t="s">
-        <v>610</v>
+        <v>619</v>
       </c>
       <c r="D200" t="s">
         <v>771</v>
@@ -13170,18 +13174,18 @@
       </c>
       <c r="I200" s="5"/>
       <c r="J200" t="s">
-        <v>611</v>
+        <v>620</v>
       </c>
     </row>
     <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="B201" t="s">
         <v>438</v>
       </c>
       <c r="C201" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="D201" t="s">
         <v>771</v>
@@ -13191,27 +13195,6 @@
       </c>
       <c r="I201" s="5"/>
       <c r="J201" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A202" t="s">
-        <v>617</v>
-      </c>
-      <c r="B202" t="s">
-        <v>438</v>
-      </c>
-      <c r="C202" t="s">
-        <v>618</v>
-      </c>
-      <c r="D202" t="s">
-        <v>771</v>
-      </c>
-      <c r="E202">
-        <v>1</v>
-      </c>
-      <c r="I202" s="5"/>
-      <c r="J202" t="s">
         <v>620</v>
       </c>
     </row>
@@ -13221,7 +13204,7 @@
     <hyperlink ref="G2" r:id="rId2" xr:uid="{EC7FA136-5E31-4921-B95C-7A464909BD66}"/>
     <hyperlink ref="G3" r:id="rId3" xr:uid="{71E787F6-211B-4241-8E76-CF22B248E3DB}"/>
     <hyperlink ref="G4" r:id="rId4" xr:uid="{3B791CF3-5818-4AE7-9B9F-37B6ECA27E60}"/>
-    <hyperlink ref="G182" r:id="rId5" xr:uid="{D022707A-EC6F-4C5C-81E7-41B5B3AD1C37}"/>
+    <hyperlink ref="G181" r:id="rId5" xr:uid="{D022707A-EC6F-4C5C-81E7-41B5B3AD1C37}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>

</xml_diff>

<commit_message>
Wiring docs, insulation dimensions
## 2022-03-20

- Working on issue #28 fairly steadily.
- All wire runs will now have an ID to aid tracking and assembly.
- Wire IDs are based on component IDs
- IDs not involving the PSU are tailed with a letter code indicating distance from MCU, e.g. HE-A is MCU->chamber panel mount, HE-B is from the right chamber panel to the tooldhead panel.
- There are a few third level connectors with a -C. The modified BLTouch wire is ABL-C and connects to ABL-B. Likewise, I included a -C for LED strips. Even though they are soldered on, they still have to be made by the builder.
- Added initial drawings for foam insulation to the `/BOM` folder
</commit_message>
<xml_diff>
--- a/BOM/General Part List.xlsx
+++ b/BOM/General Part List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\Documents\3D Print\Clockmaker\clock-3\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE3C21D0-1564-4B8C-919E-F445C3B03A9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84ED25E7-DA63-4AD1-8E9D-188427F1E172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="8" xr2:uid="{6EB0A7B6-C6D7-4759-8B58-841D5EFF92F5}"/>
   </bookViews>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2831" uniqueCount="798">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2851" uniqueCount="830">
   <si>
     <t>ID</t>
   </si>
@@ -1931,9 +1931,6 @@
     <t>UN050</t>
   </si>
   <si>
-    <t>UN151</t>
-  </si>
-  <si>
     <t>Spade Connectors, Various sizes</t>
   </si>
   <si>
@@ -2462,16 +2459,115 @@
     <t>PN558</t>
   </si>
   <si>
-    <t>For piano hinge</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/100Pcs-Standard-Tapping-SG-TZH/dp/B09955NQ43</t>
-  </si>
-  <si>
-    <t>Screw, Wood, #8 x 3/4", Truss Head</t>
-  </si>
-  <si>
     <t>Wood Panel, Front Center</t>
+  </si>
+  <si>
+    <t>Screw, #8 x 3/4", Truss Head, Sharp Point</t>
+  </si>
+  <si>
+    <t>For fasteneing metal to wood</t>
+  </si>
+  <si>
+    <t>https://www.homedepot.com/p/Everbilt-8-x-3-4-in-Phillips-Drive-Truss-Head-Lath-Sharp-Point-Screw-1-lb-Box-215-Pack-116102/205142852</t>
+  </si>
+  <si>
+    <t>200pc: https://www.amazon.com/M5-0-8-Button-Available-Stainless-Machine/dp/B07VRZYMP6</t>
+  </si>
+  <si>
+    <t>UN051</t>
+  </si>
+  <si>
+    <t>Materials</t>
+  </si>
+  <si>
+    <t>Polyisocyanurate Foam, 1/2", 4'x8' sheet</t>
+  </si>
+  <si>
+    <t>Will need a second if sheet has to be cut for transport</t>
+  </si>
+  <si>
+    <t>Plywood sheet, 12mm thickness, 4'x5'</t>
+  </si>
+  <si>
+    <t>Acrylic sheet, 5mm, 4'x5'</t>
+  </si>
+  <si>
+    <t>Wood strips, 6mmx20mm</t>
+  </si>
+  <si>
+    <t>MN100</t>
+  </si>
+  <si>
+    <t>MN101</t>
+  </si>
+  <si>
+    <t>MN102</t>
+  </si>
+  <si>
+    <t>MN103</t>
+  </si>
+  <si>
+    <t>MN104</t>
+  </si>
+  <si>
+    <t>MN105</t>
+  </si>
+  <si>
+    <t>MN112</t>
+  </si>
+  <si>
+    <t>MN111</t>
+  </si>
+  <si>
+    <t>MN110</t>
+  </si>
+  <si>
+    <t>MN220</t>
+  </si>
+  <si>
+    <t>MN201</t>
+  </si>
+  <si>
+    <t>MN221</t>
+  </si>
+  <si>
+    <t>MN222</t>
+  </si>
+  <si>
+    <t>MN230</t>
+  </si>
+  <si>
+    <t>MN223</t>
+  </si>
+  <si>
+    <t>MN240</t>
+  </si>
+  <si>
+    <t>MN202</t>
+  </si>
+  <si>
+    <t>MN203</t>
+  </si>
+  <si>
+    <t>MN204</t>
+  </si>
+  <si>
+    <t>MN205</t>
+  </si>
+  <si>
+    <t>MN210</t>
+  </si>
+  <si>
+    <t>MN211</t>
+  </si>
+  <si>
+    <t>MN212</t>
+  </si>
+  <si>
+    <t>MN213</t>
+  </si>
+  <si>
+    <t>MN001</t>
   </si>
 </sst>
 </file>
@@ -2955,10 +3051,10 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BCCEB002-6247-475F-8E59-4D3290F5D0AB}" name="Table13" displayName="Table13" ref="A1:J201" totalsRowShown="0">
-  <autoFilter ref="A1:J201" xr:uid="{BCCEB002-6247-475F-8E59-4D3290F5D0AB}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J197">
-    <sortCondition ref="A1:A197"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BCCEB002-6247-475F-8E59-4D3290F5D0AB}" name="Table13" displayName="Table13" ref="A1:J205" totalsRowShown="0">
+  <autoFilter ref="A1:J205" xr:uid="{BCCEB002-6247-475F-8E59-4D3290F5D0AB}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J175">
+    <sortCondition ref="A1:A175"/>
   </sortState>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{5013DA2C-AE55-4442-B536-8693A638A779}" name="ID"/>
@@ -8042,10 +8138,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D318B5EB-87D8-4D97-AE82-574AF33D7DA4}">
-  <dimension ref="A1:J201"/>
+  <dimension ref="A1:J205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="E84" sqref="E84"/>
+    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
+      <selection activeCell="A206" sqref="A206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8074,19 +8170,19 @@
         <v>462</v>
       </c>
       <c r="E1" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="F1" t="s">
+        <v>641</v>
+      </c>
+      <c r="G1" t="s">
+        <v>640</v>
+      </c>
+      <c r="H1" t="s">
         <v>642</v>
       </c>
-      <c r="G1" t="s">
-        <v>641</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>643</v>
-      </c>
-      <c r="I1" t="s">
-        <v>644</v>
       </c>
       <c r="J1" t="s">
         <v>6</v>
@@ -8100,7 +8196,7 @@
         <v>538</v>
       </c>
       <c r="C2" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="D2" t="s">
         <v>463</v>
@@ -8109,16 +8205,16 @@
         <v>10</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="H2" s="6" t="s">
+        <v>620</v>
+      </c>
+      <c r="I2" s="8" t="s">
         <v>621</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="J2" t="s">
         <v>622</v>
-      </c>
-      <c r="J2" t="s">
-        <v>623</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -8138,7 +8234,7 @@
         <v>10</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>394</v>
@@ -8167,7 +8263,7 @@
         <v>10</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>394</v>
@@ -8196,7 +8292,7 @@
         <v>10</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>399</v>
@@ -8223,7 +8319,7 @@
         <v>10</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="H6" t="s">
         <v>11</v>
@@ -8249,7 +8345,7 @@
         <v>10</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="H7" t="s">
         <v>11</v>
@@ -8275,7 +8371,7 @@
         <v>10</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="H8" t="s">
         <v>11</v>
@@ -8301,7 +8397,7 @@
         <v>10</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="H9" t="s">
         <v>11</v>
@@ -8327,7 +8423,7 @@
         <v>10</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="H10" t="s">
         <v>11</v>
@@ -8353,7 +8449,7 @@
         <v>10</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="H11" t="s">
         <v>11</v>
@@ -8382,7 +8478,7 @@
         <v>10</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="H12" t="s">
         <v>11</v>
@@ -8411,7 +8507,7 @@
         <v>10</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="H13" t="s">
         <v>11</v>
@@ -8440,7 +8536,7 @@
         <v>10</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="H14" t="s">
         <v>11</v>
@@ -8469,7 +8565,7 @@
         <v>36</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="H15" t="s">
         <v>37</v>
@@ -8498,7 +8594,7 @@
         <v>10</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="H16" t="s">
         <v>11</v>
@@ -8524,7 +8620,7 @@
         <v>10</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="H17" t="s">
         <v>11</v>
@@ -8532,8 +8628,8 @@
       <c r="I17" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="J17" s="1" t="s">
-        <v>490</v>
+      <c r="J17" t="s">
+        <v>797</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -8553,7 +8649,7 @@
         <v>10</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="H18" t="s">
         <v>11</v>
@@ -8579,7 +8675,7 @@
         <v>10</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="H19" t="s">
         <v>11</v>
@@ -8605,14 +8701,14 @@
         <v>10</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="H20" t="s">
         <v>65</v>
       </c>
       <c r="I20" s="5"/>
       <c r="J20" s="6" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -8641,7 +8737,7 @@
         <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="D22" t="s">
         <v>463</v>
@@ -8650,7 +8746,7 @@
       <c r="G22" s="3"/>
       <c r="I22" s="5"/>
       <c r="J22" s="6" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -8670,7 +8766,7 @@
         <v>10</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H23" t="s">
         <v>55</v>
@@ -8699,7 +8795,7 @@
         <v>10</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="H24" t="s">
         <v>59</v>
@@ -8726,7 +8822,7 @@
         <v>10</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="H25" t="s">
         <v>55</v>
@@ -8753,7 +8849,7 @@
         <v>10</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="H26" t="s">
         <v>11</v>
@@ -8782,7 +8878,7 @@
         <v>414</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="H27" t="s">
         <v>415</v>
@@ -8809,7 +8905,7 @@
         <v>10</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="H28" t="s">
         <v>65</v>
@@ -8862,34 +8958,34 @@
       </c>
       <c r="I30" s="5"/>
       <c r="J30" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="B31" t="s">
         <v>8</v>
       </c>
       <c r="C31" t="s">
+        <v>794</v>
+      </c>
+      <c r="D31" t="s">
+        <v>463</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>414</v>
+      </c>
+      <c r="G31" s="1" t="s">
         <v>796</v>
-      </c>
-      <c r="D31" t="s">
-        <v>463</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>795</v>
       </c>
       <c r="H31" t="s">
         <v>65</v>
       </c>
       <c r="I31" s="5"/>
       <c r="J31" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -8909,7 +9005,7 @@
         <v>10</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="H32" t="s">
         <v>65</v>
@@ -8933,7 +9029,7 @@
         <v>10</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="H33" t="s">
         <v>65</v>
@@ -8957,7 +9053,7 @@
         <v>10</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="H34" t="s">
         <v>65</v>
@@ -8981,7 +9077,7 @@
         <v>10</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="H35" t="s">
         <v>65</v>
@@ -9005,7 +9101,7 @@
         <v>10</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="H36" t="s">
         <v>65</v>
@@ -9029,7 +9125,7 @@
         <v>10</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H37" t="s">
         <v>65</v>
@@ -9053,7 +9149,7 @@
         <v>10</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="H38" t="s">
         <v>65</v>
@@ -9077,7 +9173,7 @@
         <v>10</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="H39" t="s">
         <v>65</v>
@@ -9101,7 +9197,7 @@
         <v>10</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="H40" t="s">
         <v>65</v>
@@ -9125,7 +9221,7 @@
         <v>10</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="H41" t="s">
         <v>65</v>
@@ -9152,7 +9248,7 @@
         <v>10</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="H42" t="s">
         <v>65</v>
@@ -9179,7 +9275,7 @@
         <v>10</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="H43" t="s">
         <v>55</v>
@@ -9206,7 +9302,7 @@
         <v>10</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="H44" t="s">
         <v>55</v>
@@ -9230,7 +9326,7 @@
         <v>10</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="H45" t="s">
         <v>92</v>
@@ -9254,7 +9350,7 @@
         <v>10</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="H46" t="s">
         <v>95</v>
@@ -9278,7 +9374,7 @@
         <v>10</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="H47" t="s">
         <v>99</v>
@@ -9304,7 +9400,7 @@
         <v>10</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="H48" t="s">
         <v>99</v>
@@ -9330,7 +9426,7 @@
         <v>10</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="H49" t="s">
         <v>99</v>
@@ -9356,7 +9452,7 @@
         <v>10</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H50" t="s">
         <v>109</v>
@@ -9382,7 +9478,7 @@
         <v>10</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="H51" t="s">
         <v>65</v>
@@ -9409,7 +9505,7 @@
         <v>10</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="H52" t="s">
         <v>115</v>
@@ -9438,7 +9534,7 @@
         <v>10</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="H53" t="s">
         <v>99</v>
@@ -9464,7 +9560,7 @@
         <v>10</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="H54" t="s">
         <v>122</v>
@@ -9490,7 +9586,7 @@
         <v>10</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="H55" t="s">
         <v>126</v>
@@ -9516,7 +9612,7 @@
         <v>10</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="H56" t="s">
         <v>126</v>
@@ -9542,7 +9638,7 @@
         <v>10</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="H57" t="s">
         <v>122</v>
@@ -9568,7 +9664,7 @@
         <v>10</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="H58" t="s">
         <v>122</v>
@@ -9594,7 +9690,7 @@
         <v>139</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="H59" t="s">
         <v>36</v>
@@ -9620,7 +9716,7 @@
         <v>10</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="H60" t="s">
         <v>59</v>
@@ -9644,7 +9740,7 @@
         <v>139</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="H61" t="s">
         <v>36</v>
@@ -9670,7 +9766,7 @@
         <v>139</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="H62" t="s">
         <v>36</v>
@@ -9696,7 +9792,7 @@
         <v>139</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="H63" t="s">
         <v>36</v>
@@ -9722,7 +9818,7 @@
         <v>139</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="H64" t="s">
         <v>36</v>
@@ -9751,7 +9847,7 @@
         <v>139</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="H65" t="s">
         <v>36</v>
@@ -9771,23 +9867,23 @@
         <v>137</v>
       </c>
       <c r="C66" t="s">
+        <v>710</v>
+      </c>
+      <c r="D66" t="s">
+        <v>463</v>
+      </c>
+      <c r="F66" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G66" s="1" t="s">
         <v>711</v>
-      </c>
-      <c r="D66" t="s">
-        <v>463</v>
-      </c>
-      <c r="F66" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G66" s="1" t="s">
-        <v>712</v>
       </c>
       <c r="H66" t="s">
         <v>65</v>
       </c>
       <c r="I66" s="5"/>
       <c r="J66" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
@@ -9807,7 +9903,7 @@
         <v>139</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="H67" t="s">
         <v>36</v>
@@ -9836,7 +9932,7 @@
         <v>139</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="H68" t="s">
         <v>36</v>
@@ -9865,7 +9961,7 @@
         <v>139</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="H69" t="s">
         <v>36</v>
@@ -9894,7 +9990,7 @@
         <v>139</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="H70" t="s">
         <v>36</v>
@@ -9923,7 +10019,7 @@
         <v>139</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="H71" t="s">
         <v>36</v>
@@ -9952,7 +10048,7 @@
         <v>139</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H72" t="s">
         <v>36</v>
@@ -9981,7 +10077,7 @@
         <v>139</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="H73" t="s">
         <v>36</v>
@@ -10010,7 +10106,7 @@
         <v>139</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="H74" t="s">
         <v>36</v>
@@ -10039,7 +10135,7 @@
         <v>139</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="H75" t="s">
         <v>36</v>
@@ -10068,7 +10164,7 @@
         <v>139</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="H76" t="s">
         <v>36</v>
@@ -10097,7 +10193,7 @@
         <v>139</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="H77" t="s">
         <v>36</v>
@@ -10126,7 +10222,7 @@
         <v>139</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="H78" t="s">
         <v>36</v>
@@ -10155,7 +10251,7 @@
         <v>139</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="H79" t="s">
         <v>36</v>
@@ -10184,7 +10280,7 @@
         <v>139</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="H80" t="s">
         <v>36</v>
@@ -10483,7 +10579,7 @@
         <v>137</v>
       </c>
       <c r="C94" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
       <c r="D94" t="s">
         <v>463</v>
@@ -10504,7 +10600,7 @@
         <v>137</v>
       </c>
       <c r="C95" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="D95" t="s">
         <v>463</v>
@@ -10761,7 +10857,7 @@
         <v>414</v>
       </c>
       <c r="G108" s="1" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="H108" s="6" t="s">
         <v>65</v>
@@ -10785,7 +10881,7 @@
         <v>10</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="H109" t="s">
         <v>225</v>
@@ -10809,7 +10905,7 @@
         <v>10</v>
       </c>
       <c r="G110" s="1" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="H110" t="s">
         <v>225</v>
@@ -10841,7 +10937,7 @@
       </c>
       <c r="I111" s="5"/>
       <c r="J111" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
@@ -10861,7 +10957,7 @@
         <v>10</v>
       </c>
       <c r="G112" s="1" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H112" t="s">
         <v>55</v>
@@ -10890,7 +10986,7 @@
         <v>10</v>
       </c>
       <c r="G113" s="1" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H113" t="s">
         <v>55</v>
@@ -10919,7 +11015,7 @@
         <v>10</v>
       </c>
       <c r="G114" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="H114" t="s">
         <v>237</v>
@@ -10948,7 +11044,7 @@
         <v>242</v>
       </c>
       <c r="G115" s="1" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="H115" t="s">
         <v>242</v>
@@ -10977,7 +11073,7 @@
         <v>10</v>
       </c>
       <c r="G116" s="1" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="H116" t="s">
         <v>245</v>
@@ -10997,24 +11093,21 @@
         <v>248</v>
       </c>
       <c r="D117" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="E117">
-        <v>120</v>
+        <v>170</v>
       </c>
       <c r="F117" t="s">
         <v>10</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="H117" t="s">
         <v>65</v>
       </c>
       <c r="I117" s="5"/>
-      <c r="J117" t="s">
-        <v>472</v>
-      </c>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
@@ -11033,7 +11126,7 @@
         <v>10</v>
       </c>
       <c r="G118" s="1" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="H118" t="s">
         <v>65</v>
@@ -11060,7 +11153,7 @@
         <v>10</v>
       </c>
       <c r="G119" s="1" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="H119" t="s">
         <v>65</v>
@@ -11087,7 +11180,7 @@
         <v>10</v>
       </c>
       <c r="G120" s="1" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="H120" t="s">
         <v>65</v>
@@ -11114,7 +11207,7 @@
         <v>10</v>
       </c>
       <c r="G121" s="1" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="H121" t="s">
         <v>65</v>
@@ -11138,7 +11231,7 @@
         <v>10</v>
       </c>
       <c r="G122" s="1" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="H122" t="s">
         <v>65</v>
@@ -11165,7 +11258,7 @@
         <v>10</v>
       </c>
       <c r="G123" s="1" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="H123" t="s">
         <v>65</v>
@@ -11192,7 +11285,7 @@
         <v>10</v>
       </c>
       <c r="G124" s="1" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="H124" t="s">
         <v>566</v>
@@ -11221,7 +11314,7 @@
         <v>10</v>
       </c>
       <c r="G125" s="1" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="H125" t="s">
         <v>65</v>
@@ -11248,7 +11341,7 @@
         <v>263</v>
       </c>
       <c r="G126" s="1" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="H126" t="s">
         <v>264</v>
@@ -11277,7 +11370,7 @@
         <v>263</v>
       </c>
       <c r="G127" s="1" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="H127" t="s">
         <v>264</v>
@@ -11306,7 +11399,7 @@
         <v>263</v>
       </c>
       <c r="G128" s="1" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="H128" t="s">
         <v>264</v>
@@ -11332,7 +11425,7 @@
         <v>10</v>
       </c>
       <c r="G129" s="1" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="H129" t="s">
         <v>237</v>
@@ -11361,7 +11454,7 @@
         <v>280</v>
       </c>
       <c r="G130" s="1" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="H130" s="2" t="s">
         <v>281</v>
@@ -11390,7 +11483,7 @@
         <v>280</v>
       </c>
       <c r="G131" s="1" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="H131" t="s">
         <v>286</v>
@@ -11416,7 +11509,7 @@
         <v>280</v>
       </c>
       <c r="G132" s="1" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="H132" t="s">
         <v>290</v>
@@ -11427,553 +11520,539 @@
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>292</v>
+        <v>336</v>
       </c>
       <c r="B133" t="s">
         <v>261</v>
       </c>
       <c r="C133" t="s">
-        <v>417</v>
+        <v>337</v>
       </c>
       <c r="D133" t="s">
-        <v>770</v>
-      </c>
-      <c r="E133">
-        <v>200</v>
+        <v>463</v>
       </c>
       <c r="F133" t="s">
         <v>10</v>
       </c>
       <c r="G133" s="1" t="s">
-        <v>756</v>
+        <v>669</v>
       </c>
       <c r="H133" t="s">
-        <v>65</v>
-      </c>
-      <c r="I133" s="5"/>
-      <c r="J133" t="s">
-        <v>419</v>
+        <v>338</v>
+      </c>
+      <c r="I133" s="5" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>293</v>
+        <v>340</v>
       </c>
       <c r="B134" t="s">
         <v>261</v>
       </c>
       <c r="C134" t="s">
-        <v>416</v>
+        <v>341</v>
       </c>
       <c r="D134" t="s">
-        <v>770</v>
-      </c>
-      <c r="E134">
-        <v>120</v>
+        <v>463</v>
       </c>
       <c r="F134" t="s">
         <v>10</v>
       </c>
       <c r="G134" s="1" t="s">
-        <v>756</v>
+        <v>670</v>
       </c>
       <c r="H134" t="s">
         <v>65</v>
       </c>
       <c r="I134" s="5"/>
-      <c r="J134" t="s">
-        <v>418</v>
-      </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>296</v>
+        <v>342</v>
       </c>
       <c r="B135" t="s">
         <v>261</v>
       </c>
       <c r="C135" t="s">
-        <v>297</v>
+        <v>343</v>
       </c>
       <c r="D135" t="s">
-        <v>770</v>
+        <v>463</v>
       </c>
       <c r="F135" t="s">
         <v>10</v>
       </c>
       <c r="G135" s="1" t="s">
-        <v>757</v>
+        <v>671</v>
       </c>
       <c r="H135" t="s">
-        <v>65</v>
-      </c>
-      <c r="I135" s="5"/>
-      <c r="J135" t="s">
-        <v>471</v>
+        <v>344</v>
+      </c>
+      <c r="I135" s="5" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>298</v>
+        <v>346</v>
       </c>
       <c r="B136" t="s">
         <v>261</v>
       </c>
       <c r="C136" t="s">
-        <v>299</v>
+        <v>347</v>
       </c>
       <c r="D136" t="s">
-        <v>770</v>
+        <v>463</v>
       </c>
       <c r="F136" t="s">
         <v>10</v>
       </c>
       <c r="G136" s="1" t="s">
-        <v>758</v>
+        <v>672</v>
       </c>
       <c r="H136" t="s">
-        <v>65</v>
+        <v>348</v>
       </c>
       <c r="I136" s="5"/>
-      <c r="J136" s="4" t="s">
-        <v>470</v>
+      <c r="J136" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>300</v>
+        <v>350</v>
       </c>
       <c r="B137" t="s">
         <v>261</v>
       </c>
       <c r="C137" t="s">
-        <v>294</v>
+        <v>351</v>
       </c>
       <c r="D137" t="s">
-        <v>770</v>
+        <v>463</v>
       </c>
       <c r="F137" t="s">
         <v>10</v>
       </c>
       <c r="G137" s="1" t="s">
-        <v>759</v>
+        <v>673</v>
       </c>
       <c r="H137" t="s">
         <v>65</v>
       </c>
       <c r="I137" s="5"/>
-      <c r="J137" t="s">
-        <v>295</v>
-      </c>
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>301</v>
+        <v>352</v>
       </c>
       <c r="B138" t="s">
         <v>261</v>
       </c>
       <c r="C138" t="s">
-        <v>302</v>
+        <v>353</v>
       </c>
       <c r="D138" t="s">
         <v>463</v>
       </c>
       <c r="F138" t="s">
-        <v>280</v>
+        <v>10</v>
       </c>
       <c r="G138" s="1" t="s">
-        <v>760</v>
+        <v>674</v>
       </c>
       <c r="H138" t="s">
-        <v>303</v>
-      </c>
-      <c r="I138" s="8" t="s">
-        <v>304</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="I138" s="5"/>
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>305</v>
+        <v>354</v>
       </c>
       <c r="B139" t="s">
         <v>261</v>
       </c>
       <c r="C139" t="s">
-        <v>306</v>
+        <v>355</v>
       </c>
       <c r="D139" t="s">
         <v>463</v>
       </c>
       <c r="F139" t="s">
-        <v>280</v>
+        <v>10</v>
       </c>
       <c r="G139" s="1" t="s">
-        <v>761</v>
+        <v>662</v>
       </c>
       <c r="H139" t="s">
-        <v>303</v>
-      </c>
-      <c r="I139" s="8" t="s">
-        <v>307</v>
+        <v>65</v>
+      </c>
+      <c r="I139" s="5"/>
+      <c r="J139" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>308</v>
+        <v>357</v>
       </c>
       <c r="B140" t="s">
         <v>261</v>
       </c>
       <c r="C140" t="s">
-        <v>309</v>
+        <v>554</v>
       </c>
       <c r="D140" t="s">
         <v>463</v>
       </c>
       <c r="F140" t="s">
-        <v>280</v>
+        <v>10</v>
       </c>
       <c r="G140" s="1" t="s">
-        <v>762</v>
+        <v>661</v>
       </c>
       <c r="H140" t="s">
-        <v>303</v>
+        <v>358</v>
       </c>
       <c r="I140" s="5" t="s">
-        <v>310</v>
+        <v>359</v>
+      </c>
+      <c r="J140" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>311</v>
+        <v>361</v>
       </c>
       <c r="B141" t="s">
         <v>261</v>
       </c>
       <c r="C141" t="s">
-        <v>312</v>
+        <v>362</v>
       </c>
       <c r="D141" t="s">
         <v>463</v>
       </c>
       <c r="F141" t="s">
-        <v>280</v>
+        <v>139</v>
       </c>
       <c r="G141" s="1" t="s">
-        <v>763</v>
+        <v>660</v>
       </c>
       <c r="H141" t="s">
-        <v>303</v>
+        <v>36</v>
       </c>
       <c r="I141" s="5" t="s">
-        <v>313</v>
+        <v>363</v>
+      </c>
+      <c r="J141" t="s">
+        <v>789</v>
       </c>
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>314</v>
+        <v>365</v>
       </c>
       <c r="B142" t="s">
         <v>261</v>
       </c>
       <c r="C142" t="s">
-        <v>315</v>
+        <v>507</v>
       </c>
       <c r="D142" t="s">
         <v>463</v>
       </c>
       <c r="F142" t="s">
-        <v>280</v>
+        <v>10</v>
       </c>
       <c r="G142" s="1" t="s">
-        <v>764</v>
+        <v>659</v>
       </c>
       <c r="H142" t="s">
-        <v>303</v>
-      </c>
-      <c r="I142" s="5" t="s">
-        <v>316</v>
+        <v>65</v>
+      </c>
+      <c r="I142" s="5"/>
+      <c r="J142" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>317</v>
+        <v>545</v>
       </c>
       <c r="B143" t="s">
         <v>261</v>
       </c>
       <c r="C143" t="s">
-        <v>318</v>
+        <v>546</v>
       </c>
       <c r="D143" t="s">
         <v>463</v>
       </c>
-      <c r="F143" t="s">
-        <v>280</v>
+      <c r="E143">
+        <v>1</v>
+      </c>
+      <c r="F143" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="G143" s="1" t="s">
-        <v>765</v>
+        <v>788</v>
       </c>
       <c r="H143" t="s">
-        <v>303</v>
-      </c>
-      <c r="I143" s="5" t="s">
-        <v>319</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="I143" s="5"/>
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>320</v>
+        <v>612</v>
       </c>
       <c r="B144" t="s">
         <v>261</v>
       </c>
       <c r="C144" t="s">
-        <v>321</v>
+        <v>613</v>
       </c>
       <c r="D144" t="s">
         <v>463</v>
       </c>
+      <c r="E144">
+        <v>1</v>
+      </c>
       <c r="F144" t="s">
-        <v>280</v>
+        <v>10</v>
       </c>
       <c r="G144" s="1" t="s">
-        <v>766</v>
+        <v>658</v>
       </c>
       <c r="H144" t="s">
-        <v>303</v>
-      </c>
-      <c r="I144" s="5" t="s">
-        <v>322</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="I144" s="5"/>
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>323</v>
+        <v>614</v>
       </c>
       <c r="B145" t="s">
         <v>261</v>
       </c>
       <c r="C145" t="s">
-        <v>324</v>
+        <v>615</v>
       </c>
       <c r="D145" t="s">
-        <v>463</v>
+        <v>535</v>
+      </c>
+      <c r="E145">
+        <v>1</v>
       </c>
       <c r="F145" t="s">
-        <v>280</v>
+        <v>10</v>
       </c>
       <c r="G145" s="1" t="s">
-        <v>767</v>
+        <v>657</v>
       </c>
       <c r="H145" t="s">
-        <v>303</v>
-      </c>
-      <c r="I145" s="5" t="s">
-        <v>325</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="I145" s="5"/>
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>326</v>
+        <v>367</v>
       </c>
       <c r="B146" t="s">
         <v>261</v>
       </c>
       <c r="C146" t="s">
-        <v>327</v>
+        <v>368</v>
       </c>
       <c r="D146" t="s">
         <v>463</v>
       </c>
       <c r="F146" t="s">
-        <v>280</v>
+        <v>10</v>
       </c>
       <c r="G146" s="1" t="s">
-        <v>768</v>
+        <v>656</v>
       </c>
       <c r="H146" t="s">
-        <v>303</v>
-      </c>
-      <c r="I146" s="5" t="s">
-        <v>328</v>
+        <v>65</v>
+      </c>
+      <c r="I146" s="5"/>
+      <c r="J146" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>329</v>
+        <v>370</v>
       </c>
       <c r="B147" t="s">
         <v>261</v>
       </c>
       <c r="C147" t="s">
-        <v>330</v>
+        <v>599</v>
       </c>
       <c r="D147" t="s">
         <v>463</v>
       </c>
       <c r="F147" t="s">
-        <v>139</v>
+        <v>10</v>
       </c>
       <c r="G147" s="1" t="s">
-        <v>664</v>
+        <v>654</v>
       </c>
       <c r="H147" t="s">
-        <v>303</v>
-      </c>
-      <c r="I147" s="5" t="s">
-        <v>331</v>
-      </c>
-      <c r="J147" t="s">
-        <v>332</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="I147" s="5"/>
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>333</v>
+        <v>371</v>
       </c>
       <c r="B148" t="s">
         <v>261</v>
       </c>
       <c r="C148" t="s">
-        <v>426</v>
+        <v>435</v>
       </c>
       <c r="D148" t="s">
         <v>463</v>
       </c>
       <c r="F148" t="s">
-        <v>280</v>
+        <v>10</v>
       </c>
       <c r="G148" s="1" t="s">
-        <v>665</v>
+        <v>655</v>
       </c>
       <c r="H148" t="s">
-        <v>303</v>
-      </c>
-      <c r="I148" s="5" t="s">
-        <v>432</v>
+        <v>65</v>
+      </c>
+      <c r="I148" s="5"/>
+      <c r="J148" t="s">
+        <v>436</v>
       </c>
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>334</v>
+        <v>371</v>
       </c>
       <c r="B149" t="s">
         <v>261</v>
       </c>
       <c r="C149" t="s">
-        <v>427</v>
+        <v>598</v>
       </c>
       <c r="D149" t="s">
         <v>463</v>
       </c>
       <c r="F149" t="s">
-        <v>280</v>
-      </c>
-      <c r="G149" s="3" t="s">
-        <v>666</v>
+        <v>10</v>
+      </c>
+      <c r="G149" s="1" t="s">
+        <v>654</v>
       </c>
       <c r="H149" t="s">
-        <v>303</v>
+        <v>115</v>
       </c>
       <c r="I149" s="5" t="s">
-        <v>430</v>
+        <v>437</v>
       </c>
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>335</v>
+        <v>372</v>
       </c>
       <c r="B150" t="s">
         <v>261</v>
       </c>
       <c r="C150" t="s">
-        <v>428</v>
+        <v>452</v>
       </c>
       <c r="D150" t="s">
         <v>463</v>
       </c>
       <c r="F150" t="s">
-        <v>280</v>
+        <v>10</v>
       </c>
       <c r="G150" s="1" t="s">
-        <v>667</v>
+        <v>653</v>
       </c>
       <c r="H150" t="s">
-        <v>303</v>
+        <v>225</v>
       </c>
       <c r="I150" s="5" t="s">
-        <v>431</v>
+        <v>373</v>
       </c>
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>420</v>
+        <v>374</v>
       </c>
       <c r="B151" t="s">
         <v>261</v>
       </c>
       <c r="C151" t="s">
-        <v>467</v>
+        <v>375</v>
       </c>
       <c r="D151" t="s">
         <v>463</v>
       </c>
       <c r="F151" t="s">
-        <v>280</v>
-      </c>
-      <c r="G151" s="3" t="s">
-        <v>668</v>
+        <v>10</v>
+      </c>
+      <c r="G151" s="1" t="s">
+        <v>652</v>
       </c>
       <c r="H151" t="s">
-        <v>303</v>
+        <v>225</v>
       </c>
       <c r="I151" s="5" t="s">
-        <v>424</v>
-      </c>
-      <c r="J151" t="s">
-        <v>469</v>
+        <v>376</v>
       </c>
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>421</v>
+        <v>377</v>
       </c>
       <c r="B152" t="s">
         <v>261</v>
       </c>
       <c r="C152" t="s">
-        <v>677</v>
+        <v>451</v>
       </c>
       <c r="D152" t="s">
         <v>463</v>
       </c>
       <c r="F152" t="s">
-        <v>280</v>
+        <v>10</v>
       </c>
       <c r="G152" s="1" t="s">
-        <v>668</v>
+        <v>651</v>
       </c>
       <c r="H152" t="s">
-        <v>303</v>
+        <v>225</v>
       </c>
       <c r="I152" s="5" t="s">
-        <v>425</v>
-      </c>
-      <c r="J152" t="s">
-        <v>469</v>
+        <v>378</v>
       </c>
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>422</v>
+        <v>379</v>
       </c>
       <c r="B153" t="s">
         <v>261</v>
       </c>
       <c r="C153" t="s">
-        <v>676</v>
+        <v>380</v>
       </c>
       <c r="D153" t="s">
         <v>463</v>
@@ -11982,24 +12061,24 @@
         <v>280</v>
       </c>
       <c r="G153" s="1" t="s">
-        <v>669</v>
+        <v>650</v>
       </c>
       <c r="H153" t="s">
-        <v>303</v>
-      </c>
-      <c r="I153" s="10" t="s">
-        <v>429</v>
+        <v>381</v>
+      </c>
+      <c r="I153" s="5" t="s">
+        <v>382</v>
       </c>
     </row>
     <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>336</v>
+        <v>383</v>
       </c>
       <c r="B154" t="s">
         <v>261</v>
       </c>
       <c r="C154" t="s">
-        <v>337</v>
+        <v>384</v>
       </c>
       <c r="D154" t="s">
         <v>463</v>
@@ -12008,24 +12087,24 @@
         <v>10</v>
       </c>
       <c r="G154" s="1" t="s">
-        <v>670</v>
+        <v>649</v>
       </c>
       <c r="H154" t="s">
-        <v>338</v>
+        <v>385</v>
       </c>
       <c r="I154" s="5" t="s">
-        <v>339</v>
+        <v>386</v>
       </c>
     </row>
     <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>340</v>
+        <v>387</v>
       </c>
       <c r="B155" t="s">
         <v>261</v>
       </c>
       <c r="C155" t="s">
-        <v>341</v>
+        <v>434</v>
       </c>
       <c r="D155" t="s">
         <v>463</v>
@@ -12034,22 +12113,24 @@
         <v>10</v>
       </c>
       <c r="G155" s="1" t="s">
-        <v>671</v>
+        <v>646</v>
       </c>
       <c r="H155" t="s">
-        <v>65</v>
-      </c>
-      <c r="I155" s="5"/>
+        <v>388</v>
+      </c>
+      <c r="I155" s="5" t="s">
+        <v>433</v>
+      </c>
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>342</v>
+        <v>562</v>
       </c>
       <c r="B156" t="s">
         <v>261</v>
       </c>
       <c r="C156" t="s">
-        <v>343</v>
+        <v>563</v>
       </c>
       <c r="D156" t="s">
         <v>463</v>
@@ -12058,84 +12139,93 @@
         <v>10</v>
       </c>
       <c r="G156" s="1" t="s">
-        <v>672</v>
+        <v>645</v>
       </c>
       <c r="H156" t="s">
-        <v>344</v>
-      </c>
-      <c r="I156" s="5" t="s">
-        <v>345</v>
+        <v>65</v>
+      </c>
+      <c r="I156" s="5"/>
+      <c r="J156" t="s">
+        <v>564</v>
       </c>
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>346</v>
+        <v>513</v>
       </c>
       <c r="B157" t="s">
-        <v>261</v>
+        <v>438</v>
       </c>
       <c r="C157" t="s">
-        <v>347</v>
+        <v>461</v>
       </c>
       <c r="D157" t="s">
         <v>463</v>
       </c>
+      <c r="E157">
+        <v>1</v>
+      </c>
       <c r="F157" t="s">
         <v>10</v>
       </c>
       <c r="G157" s="1" t="s">
-        <v>673</v>
+        <v>644</v>
       </c>
       <c r="H157" t="s">
-        <v>348</v>
-      </c>
-      <c r="I157" s="5"/>
-      <c r="J157" t="s">
-        <v>349</v>
+        <v>454</v>
+      </c>
+      <c r="I157" s="5">
+        <v>92003</v>
       </c>
     </row>
     <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>350</v>
+        <v>514</v>
       </c>
       <c r="B158" t="s">
-        <v>261</v>
+        <v>438</v>
       </c>
       <c r="C158" t="s">
-        <v>351</v>
+        <v>439</v>
       </c>
       <c r="D158" t="s">
         <v>463</v>
       </c>
+      <c r="E158">
+        <v>1</v>
+      </c>
       <c r="F158" t="s">
-        <v>10</v>
-      </c>
-      <c r="G158" s="1" t="s">
-        <v>674</v>
+        <v>210</v>
       </c>
       <c r="H158" t="s">
         <v>65</v>
       </c>
       <c r="I158" s="5"/>
+      <c r="J158" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>352</v>
+        <v>515</v>
       </c>
       <c r="B159" t="s">
-        <v>261</v>
+        <v>438</v>
       </c>
       <c r="C159" t="s">
-        <v>353</v>
+        <v>440</v>
       </c>
       <c r="D159" t="s">
-        <v>463</v>
+        <v>770</v>
+      </c>
+      <c r="E159">
+        <v>1</v>
       </c>
       <c r="F159" t="s">
         <v>10</v>
       </c>
-      <c r="G159" s="1" t="s">
-        <v>675</v>
+      <c r="G159" t="s">
+        <v>775</v>
       </c>
       <c r="H159" t="s">
         <v>65</v>
@@ -12144,125 +12234,112 @@
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>354</v>
+        <v>516</v>
       </c>
       <c r="B160" t="s">
-        <v>261</v>
+        <v>438</v>
       </c>
       <c r="C160" t="s">
-        <v>355</v>
+        <v>776</v>
       </c>
       <c r="D160" t="s">
         <v>463</v>
       </c>
+      <c r="E160">
+        <v>1</v>
+      </c>
       <c r="F160" t="s">
         <v>10</v>
       </c>
       <c r="G160" s="1" t="s">
-        <v>663</v>
+        <v>777</v>
       </c>
       <c r="H160" t="s">
         <v>65</v>
       </c>
       <c r="I160" s="5"/>
-      <c r="J160" t="s">
-        <v>356</v>
-      </c>
     </row>
     <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>357</v>
+        <v>517</v>
       </c>
       <c r="B161" t="s">
-        <v>261</v>
+        <v>438</v>
       </c>
       <c r="C161" t="s">
-        <v>554</v>
+        <v>442</v>
       </c>
       <c r="D161" t="s">
         <v>463</v>
       </c>
-      <c r="F161" t="s">
-        <v>10</v>
-      </c>
-      <c r="G161" s="1" t="s">
-        <v>662</v>
+      <c r="E161">
+        <v>1</v>
       </c>
       <c r="H161" t="s">
-        <v>358</v>
-      </c>
-      <c r="I161" s="5" t="s">
-        <v>359</v>
-      </c>
-      <c r="J161" t="s">
-        <v>360</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="I161" s="5"/>
     </row>
     <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>361</v>
+        <v>518</v>
       </c>
       <c r="B162" t="s">
-        <v>261</v>
+        <v>438</v>
       </c>
       <c r="C162" t="s">
-        <v>362</v>
+        <v>443</v>
       </c>
       <c r="D162" t="s">
         <v>463</v>
       </c>
-      <c r="F162" t="s">
-        <v>139</v>
-      </c>
-      <c r="G162" s="1" t="s">
-        <v>661</v>
+      <c r="E162">
+        <v>1</v>
       </c>
       <c r="H162" t="s">
-        <v>36</v>
-      </c>
-      <c r="I162" s="5" t="s">
-        <v>363</v>
-      </c>
-      <c r="J162" t="s">
-        <v>790</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="I162" s="5"/>
     </row>
     <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>365</v>
+        <v>519</v>
       </c>
       <c r="B163" t="s">
-        <v>261</v>
+        <v>438</v>
       </c>
       <c r="C163" t="s">
-        <v>507</v>
+        <v>447</v>
       </c>
       <c r="D163" t="s">
         <v>463</v>
       </c>
+      <c r="E163">
+        <v>1</v>
+      </c>
       <c r="F163" t="s">
         <v>10</v>
       </c>
-      <c r="G163" s="1" t="s">
-        <v>660</v>
+      <c r="G163" t="s">
+        <v>786</v>
       </c>
       <c r="H163" t="s">
         <v>65</v>
       </c>
       <c r="I163" s="5"/>
       <c r="J163" t="s">
-        <v>366</v>
+        <v>787</v>
       </c>
     </row>
     <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>545</v>
+        <v>520</v>
       </c>
       <c r="B164" t="s">
-        <v>261</v>
+        <v>438</v>
       </c>
       <c r="C164" t="s">
-        <v>546</v>
+        <v>521</v>
       </c>
       <c r="D164" t="s">
         <v>463</v>
@@ -12270,26 +12347,17 @@
       <c r="E164">
         <v>1</v>
       </c>
-      <c r="F164" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G164" s="1" t="s">
-        <v>789</v>
-      </c>
-      <c r="H164" t="s">
-        <v>65</v>
-      </c>
       <c r="I164" s="5"/>
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>612</v>
+        <v>522</v>
       </c>
       <c r="B165" t="s">
-        <v>261</v>
+        <v>438</v>
       </c>
       <c r="C165" t="s">
-        <v>613</v>
+        <v>785</v>
       </c>
       <c r="D165" t="s">
         <v>463</v>
@@ -12300,447 +12368,386 @@
       <c r="F165" t="s">
         <v>10</v>
       </c>
-      <c r="G165" s="1" t="s">
-        <v>659</v>
+      <c r="G165" t="s">
+        <v>782</v>
       </c>
       <c r="H165" t="s">
-        <v>65</v>
-      </c>
-      <c r="I165" s="5"/>
+        <v>783</v>
+      </c>
+      <c r="I165" s="5" t="s">
+        <v>784</v>
+      </c>
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>614</v>
+        <v>523</v>
       </c>
       <c r="B166" t="s">
-        <v>261</v>
+        <v>438</v>
       </c>
       <c r="C166" t="s">
-        <v>615</v>
+        <v>445</v>
       </c>
       <c r="D166" t="s">
-        <v>535</v>
+        <v>463</v>
       </c>
       <c r="E166">
         <v>1</v>
       </c>
-      <c r="F166" t="s">
-        <v>10</v>
-      </c>
-      <c r="G166" s="1" t="s">
-        <v>658</v>
-      </c>
-      <c r="H166" t="s">
-        <v>65</v>
-      </c>
       <c r="I166" s="5"/>
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>367</v>
+        <v>524</v>
       </c>
       <c r="B167" t="s">
-        <v>261</v>
+        <v>438</v>
       </c>
       <c r="C167" t="s">
-        <v>368</v>
+        <v>446</v>
       </c>
       <c r="D167" t="s">
         <v>463</v>
       </c>
+      <c r="E167">
+        <v>1</v>
+      </c>
       <c r="F167" t="s">
         <v>10</v>
       </c>
-      <c r="G167" s="1" t="s">
-        <v>657</v>
+      <c r="G167" t="s">
+        <v>778</v>
       </c>
       <c r="H167" t="s">
-        <v>65</v>
-      </c>
-      <c r="I167" s="5"/>
-      <c r="J167" t="s">
-        <v>369</v>
+        <v>779</v>
+      </c>
+      <c r="I167" s="5" t="s">
+        <v>780</v>
       </c>
     </row>
     <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>370</v>
+        <v>525</v>
       </c>
       <c r="B168" t="s">
-        <v>261</v>
+        <v>438</v>
       </c>
       <c r="C168" t="s">
-        <v>599</v>
+        <v>771</v>
       </c>
       <c r="D168" t="s">
         <v>463</v>
       </c>
-      <c r="F168" t="s">
-        <v>10</v>
-      </c>
-      <c r="G168" s="1" t="s">
-        <v>655</v>
-      </c>
-      <c r="H168" t="s">
-        <v>65</v>
+      <c r="E168">
+        <v>1</v>
       </c>
       <c r="I168" s="5"/>
+      <c r="J168" t="s">
+        <v>772</v>
+      </c>
     </row>
     <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>371</v>
+        <v>528</v>
       </c>
       <c r="B169" t="s">
-        <v>261</v>
+        <v>438</v>
       </c>
       <c r="C169" t="s">
-        <v>435</v>
+        <v>529</v>
       </c>
       <c r="D169" t="s">
-        <v>463</v>
-      </c>
-      <c r="F169" t="s">
-        <v>10</v>
-      </c>
-      <c r="G169" s="1" t="s">
-        <v>656</v>
-      </c>
-      <c r="H169" t="s">
-        <v>65</v>
+        <v>770</v>
+      </c>
+      <c r="E169">
+        <v>1</v>
       </c>
       <c r="I169" s="5"/>
-      <c r="J169" t="s">
-        <v>436</v>
-      </c>
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>371</v>
+        <v>530</v>
       </c>
       <c r="B170" t="s">
-        <v>261</v>
+        <v>438</v>
       </c>
       <c r="C170" t="s">
-        <v>598</v>
+        <v>532</v>
       </c>
       <c r="D170" t="s">
-        <v>463</v>
-      </c>
-      <c r="F170" t="s">
-        <v>10</v>
-      </c>
-      <c r="G170" s="1" t="s">
-        <v>655</v>
-      </c>
-      <c r="H170" t="s">
-        <v>115</v>
-      </c>
-      <c r="I170" s="5" t="s">
-        <v>437</v>
-      </c>
+        <v>770</v>
+      </c>
+      <c r="E170">
+        <v>1</v>
+      </c>
+      <c r="I170" s="5"/>
     </row>
     <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>372</v>
+        <v>531</v>
       </c>
       <c r="B171" t="s">
-        <v>261</v>
+        <v>438</v>
       </c>
       <c r="C171" t="s">
-        <v>452</v>
+        <v>533</v>
       </c>
       <c r="D171" t="s">
-        <v>463</v>
-      </c>
-      <c r="F171" t="s">
-        <v>10</v>
-      </c>
-      <c r="G171" s="1" t="s">
-        <v>654</v>
-      </c>
-      <c r="H171" t="s">
-        <v>225</v>
-      </c>
-      <c r="I171" s="5" t="s">
-        <v>373</v>
-      </c>
+        <v>770</v>
+      </c>
+      <c r="E171">
+        <v>1</v>
+      </c>
+      <c r="I171" s="5"/>
     </row>
     <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>374</v>
+        <v>541</v>
       </c>
       <c r="B172" t="s">
-        <v>261</v>
+        <v>438</v>
       </c>
       <c r="C172" t="s">
-        <v>375</v>
+        <v>773</v>
       </c>
       <c r="D172" t="s">
         <v>463</v>
       </c>
+      <c r="E172">
+        <v>1</v>
+      </c>
       <c r="F172" t="s">
         <v>10</v>
       </c>
-      <c r="G172" s="1" t="s">
-        <v>653</v>
+      <c r="G172" t="s">
+        <v>774</v>
       </c>
       <c r="H172" t="s">
-        <v>225</v>
+        <v>542</v>
       </c>
       <c r="I172" s="5" t="s">
-        <v>376</v>
+        <v>543</v>
       </c>
     </row>
     <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>377</v>
+        <v>551</v>
       </c>
       <c r="B173" t="s">
-        <v>261</v>
+        <v>438</v>
       </c>
       <c r="C173" t="s">
-        <v>451</v>
+        <v>229</v>
       </c>
       <c r="D173" t="s">
         <v>463</v>
       </c>
+      <c r="E173">
+        <v>1</v>
+      </c>
       <c r="F173" t="s">
         <v>10</v>
       </c>
       <c r="G173" s="1" t="s">
-        <v>652</v>
+        <v>647</v>
       </c>
       <c r="H173" t="s">
-        <v>225</v>
-      </c>
-      <c r="I173" s="5" t="s">
-        <v>378</v>
-      </c>
+        <v>230</v>
+      </c>
+      <c r="I173" s="5"/>
     </row>
     <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>379</v>
+        <v>527</v>
       </c>
       <c r="B174" t="s">
-        <v>261</v>
+        <v>438</v>
       </c>
       <c r="C174" t="s">
-        <v>380</v>
+        <v>450</v>
       </c>
       <c r="D174" t="s">
-        <v>463</v>
-      </c>
-      <c r="F174" t="s">
-        <v>280</v>
-      </c>
-      <c r="G174" s="1" t="s">
-        <v>651</v>
-      </c>
-      <c r="H174" t="s">
-        <v>381</v>
-      </c>
-      <c r="I174" s="5" t="s">
-        <v>382</v>
-      </c>
+        <v>535</v>
+      </c>
+      <c r="E174">
+        <v>1</v>
+      </c>
+      <c r="I174" s="5"/>
     </row>
     <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>383</v>
+        <v>534</v>
       </c>
       <c r="B175" t="s">
-        <v>261</v>
+        <v>438</v>
       </c>
       <c r="C175" t="s">
-        <v>384</v>
+        <v>448</v>
       </c>
       <c r="D175" t="s">
         <v>463</v>
       </c>
+      <c r="E175">
+        <v>1</v>
+      </c>
       <c r="F175" t="s">
         <v>10</v>
       </c>
-      <c r="G175" s="1" t="s">
-        <v>650</v>
+      <c r="G175" t="s">
+        <v>781</v>
       </c>
       <c r="H175" t="s">
-        <v>385</v>
-      </c>
-      <c r="I175" s="5" t="s">
-        <v>386</v>
+        <v>65</v>
+      </c>
+      <c r="I175" s="5"/>
+      <c r="J175" t="s">
+        <v>449</v>
       </c>
     </row>
     <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>387</v>
+        <v>606</v>
       </c>
       <c r="B176" t="s">
-        <v>261</v>
+        <v>438</v>
       </c>
       <c r="C176" t="s">
-        <v>434</v>
+        <v>607</v>
       </c>
       <c r="D176" t="s">
         <v>463</v>
       </c>
+      <c r="E176">
+        <v>1</v>
+      </c>
       <c r="F176" t="s">
-        <v>10</v>
-      </c>
-      <c r="G176" s="1" t="s">
-        <v>647</v>
+        <v>210</v>
       </c>
       <c r="H176" t="s">
-        <v>388</v>
-      </c>
-      <c r="I176" s="5" t="s">
-        <v>433</v>
+        <v>65</v>
+      </c>
+      <c r="I176" s="5"/>
+      <c r="J176" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>562</v>
+        <v>609</v>
       </c>
       <c r="B177" t="s">
-        <v>261</v>
+        <v>438</v>
       </c>
       <c r="C177" t="s">
-        <v>563</v>
+        <v>610</v>
       </c>
       <c r="D177" t="s">
-        <v>463</v>
-      </c>
-      <c r="F177" t="s">
-        <v>10</v>
-      </c>
-      <c r="G177" s="1" t="s">
-        <v>646</v>
-      </c>
-      <c r="H177" t="s">
-        <v>65</v>
+        <v>770</v>
+      </c>
+      <c r="E177">
+        <v>1</v>
       </c>
       <c r="I177" s="5"/>
       <c r="J177" t="s">
-        <v>564</v>
+        <v>611</v>
       </c>
     </row>
     <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>513</v>
+        <v>616</v>
       </c>
       <c r="B178" t="s">
         <v>438</v>
       </c>
       <c r="C178" t="s">
-        <v>461</v>
+        <v>618</v>
       </c>
       <c r="D178" t="s">
-        <v>463</v>
+        <v>770</v>
       </c>
       <c r="E178">
         <v>1</v>
       </c>
-      <c r="F178" t="s">
-        <v>10</v>
-      </c>
-      <c r="G178" s="1" t="s">
-        <v>645</v>
-      </c>
-      <c r="H178" t="s">
-        <v>454</v>
-      </c>
-      <c r="I178" s="5">
-        <v>92003</v>
+      <c r="I178" s="5"/>
+      <c r="J178" t="s">
+        <v>619</v>
       </c>
     </row>
     <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>514</v>
+        <v>798</v>
       </c>
       <c r="B179" t="s">
         <v>438</v>
       </c>
       <c r="C179" t="s">
-        <v>439</v>
+        <v>617</v>
       </c>
       <c r="D179" t="s">
-        <v>463</v>
+        <v>770</v>
       </c>
       <c r="E179">
         <v>1</v>
       </c>
-      <c r="F179" t="s">
-        <v>210</v>
-      </c>
-      <c r="H179" t="s">
-        <v>65</v>
-      </c>
       <c r="I179" s="5"/>
       <c r="J179" t="s">
-        <v>453</v>
+        <v>619</v>
       </c>
     </row>
     <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>515</v>
+        <v>805</v>
       </c>
       <c r="B180" t="s">
-        <v>438</v>
+        <v>799</v>
       </c>
       <c r="C180" t="s">
-        <v>440</v>
+        <v>800</v>
       </c>
       <c r="D180" t="s">
-        <v>771</v>
+        <v>463</v>
       </c>
       <c r="E180">
         <v>1</v>
       </c>
       <c r="F180" t="s">
-        <v>10</v>
-      </c>
-      <c r="G180" t="s">
-        <v>776</v>
-      </c>
-      <c r="H180" t="s">
-        <v>65</v>
+        <v>210</v>
       </c>
       <c r="I180" s="5"/>
+      <c r="J180" t="s">
+        <v>801</v>
+      </c>
     </row>
     <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>516</v>
+        <v>806</v>
       </c>
       <c r="B181" t="s">
-        <v>438</v>
+        <v>799</v>
       </c>
       <c r="C181" t="s">
-        <v>777</v>
+        <v>802</v>
       </c>
       <c r="D181" t="s">
         <v>463</v>
       </c>
       <c r="E181">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F181" t="s">
-        <v>10</v>
-      </c>
-      <c r="G181" s="1" t="s">
-        <v>778</v>
-      </c>
-      <c r="H181" t="s">
-        <v>65</v>
+        <v>210</v>
       </c>
       <c r="I181" s="5"/>
     </row>
     <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>517</v>
+        <v>807</v>
       </c>
       <c r="B182" t="s">
-        <v>438</v>
+        <v>799</v>
       </c>
       <c r="C182" t="s">
-        <v>442</v>
+        <v>803</v>
       </c>
       <c r="D182" t="s">
         <v>463</v>
@@ -12748,467 +12755,651 @@
       <c r="E182">
         <v>1</v>
       </c>
-      <c r="H182" t="s">
-        <v>65</v>
+      <c r="F182" t="s">
+        <v>210</v>
       </c>
       <c r="I182" s="5"/>
     </row>
     <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>518</v>
+        <v>808</v>
       </c>
       <c r="B183" t="s">
-        <v>438</v>
+        <v>799</v>
       </c>
       <c r="C183" t="s">
-        <v>443</v>
+        <v>804</v>
       </c>
       <c r="D183" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="E183">
-        <v>1</v>
-      </c>
-      <c r="H183" t="s">
-        <v>65</v>
+        <v>3</v>
+      </c>
+      <c r="F183" t="s">
+        <v>210</v>
       </c>
       <c r="I183" s="5"/>
     </row>
     <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>519</v>
+        <v>809</v>
       </c>
       <c r="B184" t="s">
-        <v>438</v>
+        <v>799</v>
       </c>
       <c r="C184" t="s">
-        <v>447</v>
+        <v>417</v>
       </c>
       <c r="D184" t="s">
-        <v>463</v>
+        <v>769</v>
       </c>
       <c r="E184">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="F184" t="s">
         <v>10</v>
       </c>
-      <c r="G184" t="s">
-        <v>787</v>
+      <c r="G184" s="1" t="s">
+        <v>755</v>
       </c>
       <c r="H184" t="s">
         <v>65</v>
       </c>
       <c r="I184" s="5"/>
       <c r="J184" t="s">
-        <v>788</v>
+        <v>419</v>
       </c>
     </row>
     <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>520</v>
+        <v>810</v>
       </c>
       <c r="B185" t="s">
-        <v>438</v>
+        <v>799</v>
       </c>
       <c r="C185" t="s">
-        <v>521</v>
+        <v>416</v>
       </c>
       <c r="D185" t="s">
-        <v>463</v>
+        <v>769</v>
       </c>
       <c r="E185">
-        <v>1</v>
+        <v>120</v>
+      </c>
+      <c r="F185" t="s">
+        <v>10</v>
+      </c>
+      <c r="G185" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="H185" t="s">
+        <v>65</v>
       </c>
       <c r="I185" s="5"/>
+      <c r="J185" t="s">
+        <v>418</v>
+      </c>
     </row>
     <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>522</v>
+        <v>812</v>
       </c>
       <c r="B186" t="s">
-        <v>438</v>
+        <v>799</v>
       </c>
       <c r="C186" t="s">
-        <v>786</v>
+        <v>297</v>
       </c>
       <c r="D186" t="s">
-        <v>463</v>
+        <v>769</v>
       </c>
       <c r="E186">
-        <v>1</v>
+        <v>580</v>
       </c>
       <c r="F186" t="s">
         <v>10</v>
       </c>
-      <c r="G186" t="s">
-        <v>783</v>
+      <c r="G186" s="1" t="s">
+        <v>756</v>
       </c>
       <c r="H186" t="s">
-        <v>784</v>
-      </c>
-      <c r="I186" s="5" t="s">
-        <v>785</v>
+        <v>65</v>
+      </c>
+      <c r="I186" s="5"/>
+      <c r="J186" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>523</v>
+        <v>811</v>
       </c>
       <c r="B187" t="s">
-        <v>438</v>
+        <v>799</v>
       </c>
       <c r="C187" t="s">
-        <v>445</v>
+        <v>299</v>
       </c>
       <c r="D187" t="s">
-        <v>463</v>
+        <v>769</v>
       </c>
       <c r="E187">
-        <v>1</v>
+        <v>7995</v>
+      </c>
+      <c r="F187" t="s">
+        <v>10</v>
+      </c>
+      <c r="G187" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="H187" t="s">
+        <v>65</v>
       </c>
       <c r="I187" s="5"/>
+      <c r="J187" s="4" t="s">
+        <v>470</v>
+      </c>
     </row>
     <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>524</v>
+        <v>813</v>
       </c>
       <c r="B188" t="s">
-        <v>438</v>
+        <v>799</v>
       </c>
       <c r="C188" t="s">
-        <v>446</v>
+        <v>294</v>
       </c>
       <c r="D188" t="s">
-        <v>463</v>
+        <v>769</v>
       </c>
       <c r="E188">
-        <v>1</v>
+        <v>565</v>
       </c>
       <c r="F188" t="s">
         <v>10</v>
       </c>
-      <c r="G188" t="s">
-        <v>779</v>
+      <c r="G188" s="1" t="s">
+        <v>758</v>
       </c>
       <c r="H188" t="s">
-        <v>780</v>
-      </c>
-      <c r="I188" s="5" t="s">
-        <v>781</v>
+        <v>65</v>
+      </c>
+      <c r="I188" s="5"/>
+      <c r="J188" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>525</v>
+        <v>815</v>
       </c>
       <c r="B189" t="s">
-        <v>438</v>
+        <v>799</v>
       </c>
       <c r="C189" t="s">
-        <v>772</v>
+        <v>302</v>
       </c>
       <c r="D189" t="s">
         <v>463</v>
       </c>
-      <c r="E189">
-        <v>1</v>
-      </c>
-      <c r="I189" s="5"/>
-      <c r="J189" t="s">
-        <v>773</v>
+      <c r="F189" t="s">
+        <v>280</v>
+      </c>
+      <c r="G189" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="H189" t="s">
+        <v>303</v>
+      </c>
+      <c r="I189" s="8" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>528</v>
+        <v>815</v>
       </c>
       <c r="B190" t="s">
-        <v>438</v>
+        <v>799</v>
       </c>
       <c r="C190" t="s">
-        <v>529</v>
+        <v>306</v>
       </c>
       <c r="D190" t="s">
-        <v>771</v>
-      </c>
-      <c r="E190">
-        <v>1</v>
-      </c>
-      <c r="I190" s="5"/>
+        <v>463</v>
+      </c>
+      <c r="F190" t="s">
+        <v>280</v>
+      </c>
+      <c r="G190" s="1" t="s">
+        <v>760</v>
+      </c>
+      <c r="H190" t="s">
+        <v>303</v>
+      </c>
+      <c r="I190" s="8" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>530</v>
+        <v>821</v>
       </c>
       <c r="B191" t="s">
-        <v>438</v>
+        <v>799</v>
       </c>
       <c r="C191" t="s">
-        <v>532</v>
+        <v>309</v>
       </c>
       <c r="D191" t="s">
-        <v>771</v>
-      </c>
-      <c r="E191">
-        <v>1</v>
-      </c>
-      <c r="I191" s="5"/>
+        <v>463</v>
+      </c>
+      <c r="F191" t="s">
+        <v>280</v>
+      </c>
+      <c r="G191" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="H191" t="s">
+        <v>303</v>
+      </c>
+      <c r="I191" s="5" t="s">
+        <v>310</v>
+      </c>
     </row>
     <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>531</v>
+        <v>822</v>
       </c>
       <c r="B192" t="s">
-        <v>438</v>
+        <v>799</v>
       </c>
       <c r="C192" t="s">
-        <v>533</v>
+        <v>312</v>
       </c>
       <c r="D192" t="s">
-        <v>771</v>
-      </c>
-      <c r="E192">
-        <v>1</v>
-      </c>
-      <c r="I192" s="5"/>
+        <v>463</v>
+      </c>
+      <c r="F192" t="s">
+        <v>280</v>
+      </c>
+      <c r="G192" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="H192" t="s">
+        <v>303</v>
+      </c>
+      <c r="I192" s="5" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="193" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>541</v>
+        <v>823</v>
       </c>
       <c r="B193" t="s">
-        <v>438</v>
+        <v>799</v>
       </c>
       <c r="C193" t="s">
-        <v>774</v>
+        <v>315</v>
       </c>
       <c r="D193" t="s">
         <v>463</v>
       </c>
-      <c r="E193">
-        <v>1</v>
-      </c>
       <c r="F193" t="s">
-        <v>10</v>
-      </c>
-      <c r="G193" t="s">
-        <v>775</v>
+        <v>280</v>
+      </c>
+      <c r="G193" s="1" t="s">
+        <v>763</v>
       </c>
       <c r="H193" t="s">
-        <v>542</v>
+        <v>303</v>
       </c>
       <c r="I193" s="5" t="s">
-        <v>543</v>
+        <v>316</v>
       </c>
     </row>
     <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>551</v>
+        <v>824</v>
       </c>
       <c r="B194" t="s">
-        <v>438</v>
+        <v>799</v>
       </c>
       <c r="C194" t="s">
-        <v>229</v>
+        <v>318</v>
       </c>
       <c r="D194" t="s">
         <v>463</v>
       </c>
-      <c r="E194">
-        <v>1</v>
-      </c>
       <c r="F194" t="s">
-        <v>10</v>
+        <v>280</v>
       </c>
       <c r="G194" s="1" t="s">
-        <v>648</v>
+        <v>764</v>
       </c>
       <c r="H194" t="s">
-        <v>230</v>
-      </c>
-      <c r="I194" s="5"/>
+        <v>303</v>
+      </c>
+      <c r="I194" s="5" t="s">
+        <v>319</v>
+      </c>
     </row>
     <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>553</v>
+        <v>825</v>
       </c>
       <c r="B195" t="s">
-        <v>223</v>
+        <v>799</v>
       </c>
       <c r="C195" t="s">
-        <v>251</v>
+        <v>321</v>
       </c>
       <c r="D195" t="s">
-        <v>465</v>
-      </c>
-      <c r="E195">
-        <v>1</v>
+        <v>463</v>
       </c>
       <c r="F195" t="s">
-        <v>10</v>
+        <v>280</v>
       </c>
       <c r="G195" s="1" t="s">
-        <v>649</v>
+        <v>765</v>
       </c>
       <c r="H195" t="s">
-        <v>252</v>
-      </c>
-      <c r="I195" s="5"/>
-      <c r="J195" t="s">
-        <v>473</v>
+        <v>303</v>
+      </c>
+      <c r="I195" s="5" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="196" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>527</v>
+        <v>826</v>
       </c>
       <c r="B196" t="s">
-        <v>438</v>
+        <v>799</v>
       </c>
       <c r="C196" t="s">
-        <v>450</v>
+        <v>324</v>
       </c>
       <c r="D196" t="s">
-        <v>535</v>
-      </c>
-      <c r="E196">
-        <v>1</v>
-      </c>
-      <c r="I196" s="5"/>
+        <v>463</v>
+      </c>
+      <c r="F196" t="s">
+        <v>280</v>
+      </c>
+      <c r="G196" s="1" t="s">
+        <v>766</v>
+      </c>
+      <c r="H196" t="s">
+        <v>303</v>
+      </c>
+      <c r="I196" s="5" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="197" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>534</v>
+        <v>827</v>
       </c>
       <c r="B197" t="s">
-        <v>438</v>
+        <v>799</v>
       </c>
       <c r="C197" t="s">
-        <v>448</v>
+        <v>327</v>
       </c>
       <c r="D197" t="s">
         <v>463</v>
       </c>
-      <c r="E197">
-        <v>1</v>
-      </c>
       <c r="F197" t="s">
-        <v>10</v>
-      </c>
-      <c r="G197" t="s">
-        <v>782</v>
+        <v>280</v>
+      </c>
+      <c r="G197" s="1" t="s">
+        <v>767</v>
       </c>
       <c r="H197" t="s">
-        <v>65</v>
-      </c>
-      <c r="I197" s="5"/>
-      <c r="J197" t="s">
-        <v>449</v>
+        <v>303</v>
+      </c>
+      <c r="I197" s="5" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>606</v>
+        <v>828</v>
       </c>
       <c r="B198" t="s">
-        <v>438</v>
+        <v>799</v>
       </c>
       <c r="C198" t="s">
-        <v>607</v>
+        <v>330</v>
       </c>
       <c r="D198" t="s">
         <v>463</v>
       </c>
-      <c r="E198">
-        <v>1</v>
-      </c>
       <c r="F198" t="s">
-        <v>210</v>
+        <v>139</v>
+      </c>
+      <c r="G198" s="1" t="s">
+        <v>663</v>
       </c>
       <c r="H198" t="s">
-        <v>65</v>
-      </c>
-      <c r="I198" s="5"/>
+        <v>303</v>
+      </c>
+      <c r="I198" s="5" t="s">
+        <v>331</v>
+      </c>
       <c r="J198" t="s">
-        <v>608</v>
+        <v>332</v>
       </c>
     </row>
     <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>609</v>
+        <v>816</v>
       </c>
       <c r="B199" t="s">
-        <v>438</v>
+        <v>799</v>
       </c>
       <c r="C199" t="s">
-        <v>610</v>
+        <v>426</v>
       </c>
       <c r="D199" t="s">
-        <v>771</v>
-      </c>
-      <c r="E199">
-        <v>1</v>
-      </c>
-      <c r="I199" s="5"/>
-      <c r="J199" t="s">
-        <v>611</v>
+        <v>463</v>
+      </c>
+      <c r="F199" t="s">
+        <v>280</v>
+      </c>
+      <c r="G199" s="1" t="s">
+        <v>664</v>
+      </c>
+      <c r="H199" t="s">
+        <v>303</v>
+      </c>
+      <c r="I199" s="5" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>616</v>
+        <v>817</v>
       </c>
       <c r="B200" t="s">
-        <v>438</v>
+        <v>799</v>
       </c>
       <c r="C200" t="s">
-        <v>619</v>
+        <v>427</v>
       </c>
       <c r="D200" t="s">
-        <v>771</v>
-      </c>
-      <c r="E200">
-        <v>1</v>
-      </c>
-      <c r="I200" s="5"/>
-      <c r="J200" t="s">
-        <v>620</v>
+        <v>463</v>
+      </c>
+      <c r="F200" t="s">
+        <v>280</v>
+      </c>
+      <c r="G200" s="3" t="s">
+        <v>665</v>
+      </c>
+      <c r="H200" t="s">
+        <v>303</v>
+      </c>
+      <c r="I200" s="5" t="s">
+        <v>430</v>
       </c>
     </row>
     <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>617</v>
+        <v>819</v>
       </c>
       <c r="B201" t="s">
+        <v>799</v>
+      </c>
+      <c r="C201" t="s">
+        <v>428</v>
+      </c>
+      <c r="D201" t="s">
+        <v>463</v>
+      </c>
+      <c r="F201" t="s">
+        <v>280</v>
+      </c>
+      <c r="G201" s="1" t="s">
+        <v>666</v>
+      </c>
+      <c r="H201" t="s">
+        <v>303</v>
+      </c>
+      <c r="I201" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>820</v>
+      </c>
+      <c r="B202" t="s">
+        <v>799</v>
+      </c>
+      <c r="C202" t="s">
+        <v>467</v>
+      </c>
+      <c r="D202" t="s">
+        <v>463</v>
+      </c>
+      <c r="F202" t="s">
+        <v>280</v>
+      </c>
+      <c r="G202" s="3" t="s">
+        <v>667</v>
+      </c>
+      <c r="H202" t="s">
+        <v>303</v>
+      </c>
+      <c r="I202" s="5" t="s">
+        <v>424</v>
+      </c>
+      <c r="J202" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>814</v>
+      </c>
+      <c r="B203" t="s">
+        <v>799</v>
+      </c>
+      <c r="C203" t="s">
+        <v>676</v>
+      </c>
+      <c r="D203" t="s">
+        <v>463</v>
+      </c>
+      <c r="F203" t="s">
+        <v>280</v>
+      </c>
+      <c r="G203" s="1" t="s">
+        <v>667</v>
+      </c>
+      <c r="H203" t="s">
+        <v>303</v>
+      </c>
+      <c r="I203" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="J203" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>818</v>
+      </c>
+      <c r="B204" t="s">
+        <v>799</v>
+      </c>
+      <c r="C204" t="s">
+        <v>675</v>
+      </c>
+      <c r="D204" t="s">
+        <v>463</v>
+      </c>
+      <c r="F204" t="s">
+        <v>280</v>
+      </c>
+      <c r="G204" s="1" t="s">
+        <v>668</v>
+      </c>
+      <c r="H204" t="s">
+        <v>303</v>
+      </c>
+      <c r="I204" s="10" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>829</v>
+      </c>
+      <c r="B205" t="s">
         <v>438</v>
       </c>
-      <c r="C201" t="s">
-        <v>618</v>
-      </c>
-      <c r="D201" t="s">
-        <v>771</v>
-      </c>
-      <c r="E201">
+      <c r="C205" t="s">
+        <v>251</v>
+      </c>
+      <c r="D205" t="s">
+        <v>465</v>
+      </c>
+      <c r="E205">
         <v>1</v>
       </c>
-      <c r="I201" s="5"/>
-      <c r="J201" t="s">
-        <v>620</v>
+      <c r="F205" t="s">
+        <v>10</v>
+      </c>
+      <c r="G205" s="1" t="s">
+        <v>648</v>
+      </c>
+      <c r="H205" t="s">
+        <v>252</v>
+      </c>
+      <c r="I205" s="5"/>
+      <c r="J205" t="s">
+        <v>473</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J17" r:id="rId1" display="Bulk Link" xr:uid="{F82FB24D-F456-4AD0-A18C-EFB9462C2336}"/>
-    <hyperlink ref="G2" r:id="rId2" xr:uid="{EC7FA136-5E31-4921-B95C-7A464909BD66}"/>
-    <hyperlink ref="G3" r:id="rId3" xr:uid="{71E787F6-211B-4241-8E76-CF22B248E3DB}"/>
-    <hyperlink ref="G4" r:id="rId4" xr:uid="{3B791CF3-5818-4AE7-9B9F-37B6ECA27E60}"/>
-    <hyperlink ref="G181" r:id="rId5" xr:uid="{D022707A-EC6F-4C5C-81E7-41B5B3AD1C37}"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{EC7FA136-5E31-4921-B95C-7A464909BD66}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{71E787F6-211B-4241-8E76-CF22B248E3DB}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{3B791CF3-5818-4AE7-9B9F-37B6ECA27E60}"/>
+    <hyperlink ref="G160" r:id="rId4" xr:uid="{D022707A-EC6F-4C5C-81E7-41B5B3AD1C37}"/>
+    <hyperlink ref="G31" r:id="rId5" xr:uid="{6EB12907-0812-466A-9C43-4E735EACE634}"/>
+    <hyperlink ref="G191" r:id="rId6" xr:uid="{A8AB8D34-CB3C-46EE-A784-757B50AE5104}"/>
+    <hyperlink ref="G195" r:id="rId7" xr:uid="{83EFA558-6064-4A22-B4F0-E0BF43E7DD16}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
   <tableParts count="1">
-    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>